<commit_message>
can delete this branch
</commit_message>
<xml_diff>
--- a/LandDInputCalculations-RetrospectiveDamages.xlsx
+++ b/LandDInputCalculations-RetrospectiveDamages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranchawla/Documents/GitHub/loss-and-damage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0382E05-99EF-BD41-9809-9C0C5B1400E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B3E551-C329-FB48-A02E-5513E95018E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" firstSheet="6" activeTab="11" xr2:uid="{5720ED0B-CBDF-AD47-AC09-0B39121B5DC0}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" activeTab="1" xr2:uid="{5720ED0B-CBDF-AD47-AC09-0B39121B5DC0}"/>
   </bookViews>
   <sheets>
     <sheet name="RICEPP-regionalLandDpayment" sheetId="15" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="RIChistoric_emissions_BP_183005" sheetId="12" r:id="rId11"/>
     <sheet name="RICEBP-CumulativeLandDcalcs" sheetId="13" r:id="rId12"/>
     <sheet name="RICEhistoric_damages_BP_00 (2)" sheetId="14" r:id="rId13"/>
+    <sheet name="Sheet1" sheetId="20" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -847,11 +848,10 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1231,7 +1231,7 @@
   <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C5" sqref="C5:N64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10438,8 +10438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B77074C9-7F59-1A49-92E2-CE92182646C6}">
   <dimension ref="A1:BR62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AT4" sqref="AT4:BE62"/>
+    <sheetView topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AT4" sqref="AT4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11096,51 +11096,51 @@
       <c r="AS4" t="s">
         <v>102</v>
       </c>
-      <c r="AT4" s="3">
+      <c r="AT4">
         <f>(C4/SUM($C4:$N4)-R4/SUM($R4:$AC4))*SUM('RICBP-it0_damagesbyregionoutput'!$A3:$L3)</f>
         <v>4.2979290000950472E-2</v>
       </c>
-      <c r="AU4" s="3">
+      <c r="AU4">
         <f>(D4/SUM($C4:$N4)-S4/SUM($R4:$AC4))*SUM('RICBP-it0_damagesbyregionoutput'!$A3:$L3)</f>
         <v>2.2457016714554679E-2</v>
       </c>
-      <c r="AV4" s="3">
+      <c r="AV4">
         <f>(E4/SUM($C4:$N4)-T4/SUM($R4:$AC4))*SUM('RICBP-it0_damagesbyregionoutput'!$A3:$L3)</f>
         <v>-1.5820095621005007E-2</v>
       </c>
-      <c r="AW4" s="3">
+      <c r="AW4">
         <f>(F4/SUM($C4:$N4)-U4/SUM($R4:$AC4))*SUM('RICBP-it0_damagesbyregionoutput'!$A3:$L3)</f>
         <v>3.8052169528352063E-3</v>
       </c>
-      <c r="AX4" s="3">
+      <c r="AX4">
         <f>(G4/SUM($C4:$N4)-V4/SUM($R4:$AC4))*SUM('RICBP-it0_damagesbyregionoutput'!$A3:$L3)</f>
         <v>1.5323055227499612E-2</v>
       </c>
-      <c r="AY4" s="3">
+      <c r="AY4">
         <f>(H4/SUM($C4:$N4)-W4/SUM($R4:$AC4))*SUM('RICBP-it0_damagesbyregionoutput'!$A3:$L3)</f>
         <v>5.3570458451981801E-3</v>
       </c>
-      <c r="AZ4" s="3">
+      <c r="AZ4">
         <f>(I4/SUM($C4:$N4)-X4/SUM($R4:$AC4))*SUM('RICBP-it0_damagesbyregionoutput'!$A3:$L3)</f>
         <v>3.5808675260103344E-3</v>
       </c>
-      <c r="BA4" s="3">
+      <c r="BA4">
         <f>(J4/SUM($C4:$N4)-Y4/SUM($R4:$AC4))*SUM('RICBP-it0_damagesbyregionoutput'!$A3:$L3)</f>
         <v>-2.2488602574037373E-2</v>
       </c>
-      <c r="BB4" s="3">
+      <c r="BB4">
         <f>(K4/SUM($C4:$N4)-Z4/SUM($R4:$AC4))*SUM('RICBP-it0_damagesbyregionoutput'!$A3:$L3)</f>
         <v>-1.2860938205895914E-2</v>
       </c>
-      <c r="BC4" s="3">
+      <c r="BC4">
         <f>(L4/SUM($C4:$N4)-AA4/SUM($R4:$AC4))*SUM('RICBP-it0_damagesbyregionoutput'!$A3:$L3)</f>
         <v>-1.8502032469882874E-2</v>
       </c>
-      <c r="BD4" s="3">
+      <c r="BD4">
         <f>(M4/SUM($C4:$N4)-AB4/SUM($R4:$AC4))*SUM('RICBP-it0_damagesbyregionoutput'!$A3:$L3)</f>
         <v>-7.9419802212742346E-3</v>
       </c>
-      <c r="BE4" s="3">
+      <c r="BE4">
         <f>(N4/SUM($C4:$N4)-AC4/SUM($R4:$AC4))*SUM('RICBP-it0_damagesbyregionoutput'!$A3:$L3)</f>
         <v>-1.5888843174953069E-2</v>
       </c>
@@ -11356,51 +11356,51 @@
         <f t="shared" si="0"/>
         <v>-0.11950679506036511</v>
       </c>
-      <c r="AT5" s="3">
+      <c r="AT5">
         <f>(C5/SUM($C5:$N5)-R5/SUM($R5:$AC5))*SUM('RICBP-it0_damagesbyregionoutput'!$A4:$L4)</f>
         <v>8.5234607741404622E-2</v>
       </c>
-      <c r="AU5" s="3">
+      <c r="AU5">
         <f>(D5/SUM($C5:$N5)-S5/SUM($R5:$AC5))*SUM('RICBP-it0_damagesbyregionoutput'!$A4:$L4)</f>
         <v>4.317990990127446E-2</v>
       </c>
-      <c r="AV5" s="3">
+      <c r="AV5">
         <f>(E5/SUM($C5:$N5)-T5/SUM($R5:$AC5))*SUM('RICBP-it0_damagesbyregionoutput'!$A4:$L4)</f>
         <v>-2.2416794753178544E-2</v>
       </c>
-      <c r="AW5" s="3">
+      <c r="AW5">
         <f>(F5/SUM($C5:$N5)-U5/SUM($R5:$AC5))*SUM('RICBP-it0_damagesbyregionoutput'!$A4:$L4)</f>
         <v>9.3906923034150248E-3</v>
       </c>
-      <c r="AX5" s="3">
+      <c r="AX5">
         <f>(G5/SUM($C5:$N5)-V5/SUM($R5:$AC5))*SUM('RICBP-it0_damagesbyregionoutput'!$A4:$L4)</f>
         <v>3.0241111661417748E-2</v>
       </c>
-      <c r="AY5" s="3">
+      <c r="AY5">
         <f>(H5/SUM($C5:$N5)-W5/SUM($R5:$AC5))*SUM('RICBP-it0_damagesbyregionoutput'!$A4:$L4)</f>
         <v>-6.7779804402777121E-3</v>
       </c>
-      <c r="AZ5" s="3">
+      <c r="AZ5">
         <f>(I5/SUM($C5:$N5)-X5/SUM($R5:$AC5))*SUM('RICBP-it0_damagesbyregionoutput'!$A4:$L4)</f>
         <v>1.7533913814719248E-3</v>
       </c>
-      <c r="BA5" s="3">
+      <c r="BA5">
         <f>(J5/SUM($C5:$N5)-Y5/SUM($R5:$AC5))*SUM('RICBP-it0_damagesbyregionoutput'!$A4:$L4)</f>
         <v>-4.3073462923487453E-2</v>
       </c>
-      <c r="BB5" s="3">
+      <c r="BB5">
         <f>(K5/SUM($C5:$N5)-Z5/SUM($R5:$AC5))*SUM('RICBP-it0_damagesbyregionoutput'!$A4:$L4)</f>
         <v>-2.548372811006103E-2</v>
       </c>
-      <c r="BC5" s="3">
+      <c r="BC5">
         <f>(L5/SUM($C5:$N5)-AA5/SUM($R5:$AC5))*SUM('RICBP-it0_damagesbyregionoutput'!$A4:$L4)</f>
         <v>-3.0891506361906733E-2</v>
       </c>
-      <c r="BD5" s="3">
+      <c r="BD5">
         <f>(M5/SUM($C5:$N5)-AB5/SUM($R5:$AC5))*SUM('RICBP-it0_damagesbyregionoutput'!$A4:$L4)</f>
         <v>-1.3506095549511814E-2</v>
       </c>
-      <c r="BE5" s="3">
+      <c r="BE5">
         <f>(N5/SUM($C5:$N5)-AC5/SUM($R5:$AC5))*SUM('RICBP-it0_damagesbyregionoutput'!$A4:$L4)</f>
         <v>-2.765014485056044E-2</v>
       </c>
@@ -11616,51 +11616,51 @@
         <f t="shared" si="0"/>
         <v>-0.15238613362421397</v>
       </c>
-      <c r="AT6" s="3">
+      <c r="AT6">
         <f>(C6/SUM($C6:$N6)-R6/SUM($R6:$AC6))*SUM('RICBP-it0_damagesbyregionoutput'!$A5:$L5)</f>
         <v>0.15847530973713264</v>
       </c>
-      <c r="AU6" s="3">
+      <c r="AU6">
         <f>(D6/SUM($C6:$N6)-S6/SUM($R6:$AC6))*SUM('RICBP-it0_damagesbyregionoutput'!$A5:$L5)</f>
         <v>8.139436660212622E-2</v>
       </c>
-      <c r="AV6" s="3">
+      <c r="AV6">
         <f>(E6/SUM($C6:$N6)-T6/SUM($R6:$AC6))*SUM('RICBP-it0_damagesbyregionoutput'!$A5:$L5)</f>
         <v>-2.457107437945109E-2</v>
       </c>
-      <c r="AW6" s="3">
+      <c r="AW6">
         <f>(F6/SUM($C6:$N6)-U6/SUM($R6:$AC6))*SUM('RICBP-it0_damagesbyregionoutput'!$A5:$L5)</f>
         <v>2.0751779868526863E-2</v>
       </c>
-      <c r="AX6" s="3">
+      <c r="AX6">
         <f>(G6/SUM($C6:$N6)-V6/SUM($R6:$AC6))*SUM('RICBP-it0_damagesbyregionoutput'!$A5:$L5)</f>
         <v>5.554204934617045E-2</v>
       </c>
-      <c r="AY6" s="3">
+      <c r="AY6">
         <f>(H6/SUM($C6:$N6)-W6/SUM($R6:$AC6))*SUM('RICBP-it0_damagesbyregionoutput'!$A5:$L5)</f>
         <v>-4.3521977884199099E-2</v>
       </c>
-      <c r="AZ6" s="3">
+      <c r="AZ6">
         <f>(I6/SUM($C6:$N6)-X6/SUM($R6:$AC6))*SUM('RICBP-it0_damagesbyregionoutput'!$A5:$L5)</f>
         <v>-7.0095336453263818E-3</v>
       </c>
-      <c r="BA6" s="3">
+      <c r="BA6">
         <f>(J6/SUM($C6:$N6)-Y6/SUM($R6:$AC6))*SUM('RICBP-it0_damagesbyregionoutput'!$A5:$L5)</f>
         <v>-7.6616108491247933E-2</v>
       </c>
-      <c r="BB6" s="3">
+      <c r="BB6">
         <f>(K6/SUM($C6:$N6)-Z6/SUM($R6:$AC6))*SUM('RICBP-it0_damagesbyregionoutput'!$A5:$L5)</f>
         <v>-5.2348073192009924E-2</v>
       </c>
-      <c r="BC6" s="3">
+      <c r="BC6">
         <f>(L6/SUM($C6:$N6)-AA6/SUM($R6:$AC6))*SUM('RICBP-it0_damagesbyregionoutput'!$A5:$L5)</f>
         <v>-4.6818976467276008E-2</v>
       </c>
-      <c r="BD6" s="3">
+      <c r="BD6">
         <f>(M6/SUM($C6:$N6)-AB6/SUM($R6:$AC6))*SUM('RICBP-it0_damagesbyregionoutput'!$A5:$L5)</f>
         <v>-1.9959945100594456E-2</v>
       </c>
-      <c r="BE6" s="3">
+      <c r="BE6">
         <f>(N6/SUM($C6:$N6)-AC6/SUM($R6:$AC6))*SUM('RICBP-it0_damagesbyregionoutput'!$A5:$L5)</f>
         <v>-4.5317816393851434E-2</v>
       </c>
@@ -11876,51 +11876,51 @@
         <f t="shared" si="0"/>
         <v>-0.213665181542017</v>
       </c>
-      <c r="AT7" s="3">
+      <c r="AT7">
         <f>(C7/SUM($C7:$N7)-R7/SUM($R7:$AC7))*SUM('RICBP-it0_damagesbyregionoutput'!$A6:$L6)</f>
         <v>0.27269047368106092</v>
       </c>
-      <c r="AU7" s="3">
+      <c r="AU7">
         <f>(D7/SUM($C7:$N7)-S7/SUM($R7:$AC7))*SUM('RICBP-it0_damagesbyregionoutput'!$A6:$L6)</f>
         <v>0.14636423154653819</v>
       </c>
-      <c r="AV7" s="3">
+      <c r="AV7">
         <f>(E7/SUM($C7:$N7)-T7/SUM($R7:$AC7))*SUM('RICBP-it0_damagesbyregionoutput'!$A6:$L6)</f>
         <v>-1.8160921466087259E-2</v>
       </c>
-      <c r="AW7" s="3">
+      <c r="AW7">
         <f>(F7/SUM($C7:$N7)-U7/SUM($R7:$AC7))*SUM('RICBP-it0_damagesbyregionoutput'!$A6:$L6)</f>
         <v>4.0046926336709372E-2</v>
       </c>
-      <c r="AX7" s="3">
+      <c r="AX7">
         <f>(G7/SUM($C7:$N7)-V7/SUM($R7:$AC7))*SUM('RICBP-it0_damagesbyregionoutput'!$A6:$L6)</f>
         <v>9.3885605723002433E-2</v>
       </c>
-      <c r="AY7" s="3">
+      <c r="AY7">
         <f>(H7/SUM($C7:$N7)-W7/SUM($R7:$AC7))*SUM('RICBP-it0_damagesbyregionoutput'!$A6:$L6)</f>
         <v>-0.11048170380777277</v>
       </c>
-      <c r="AZ7" s="3">
+      <c r="AZ7">
         <f>(I7/SUM($C7:$N7)-X7/SUM($R7:$AC7))*SUM('RICBP-it0_damagesbyregionoutput'!$A6:$L6)</f>
         <v>-2.6335282696151964E-2</v>
       </c>
-      <c r="BA7" s="3">
+      <c r="BA7">
         <f>(J7/SUM($C7:$N7)-Y7/SUM($R7:$AC7))*SUM('RICBP-it0_damagesbyregionoutput'!$A6:$L6)</f>
         <v>-0.12592394829131409</v>
       </c>
-      <c r="BB7" s="3">
+      <c r="BB7">
         <f>(K7/SUM($C7:$N7)-Z7/SUM($R7:$AC7))*SUM('RICBP-it0_damagesbyregionoutput'!$A6:$L6)</f>
         <v>-0.10870496690253367</v>
       </c>
-      <c r="BC7" s="3">
+      <c r="BC7">
         <f>(L7/SUM($C7:$N7)-AA7/SUM($R7:$AC7))*SUM('RICBP-it0_damagesbyregionoutput'!$A6:$L6)</f>
         <v>-6.6058889798638845E-2</v>
       </c>
-      <c r="BD7" s="3">
+      <c r="BD7">
         <f>(M7/SUM($C7:$N7)-AB7/SUM($R7:$AC7))*SUM('RICBP-it0_damagesbyregionoutput'!$A6:$L6)</f>
         <v>-2.5715829478013767E-2</v>
       </c>
-      <c r="BE7" s="3">
+      <c r="BE7">
         <f>(N7/SUM($C7:$N7)-AC7/SUM($R7:$AC7))*SUM('RICBP-it0_damagesbyregionoutput'!$A6:$L6)</f>
         <v>-7.1605694846798698E-2</v>
       </c>
@@ -12136,51 +12136,51 @@
         <f t="shared" si="0"/>
         <v>-0.31707771352830449</v>
       </c>
-      <c r="AT8" s="3">
+      <c r="AT8">
         <f>(C8/SUM($C8:$N8)-R8/SUM($R8:$AC8))*SUM('RICBP-it0_damagesbyregionoutput'!$A7:$L7)</f>
         <v>0.43767601606239492</v>
       </c>
-      <c r="AU8" s="3">
+      <c r="AU8">
         <f>(D8/SUM($C8:$N8)-S8/SUM($R8:$AC8))*SUM('RICBP-it0_damagesbyregionoutput'!$A7:$L7)</f>
         <v>0.24808204030288028</v>
       </c>
-      <c r="AV8" s="3">
+      <c r="AV8">
         <f>(E8/SUM($C8:$N8)-T8/SUM($R8:$AC8))*SUM('RICBP-it0_damagesbyregionoutput'!$A7:$L7)</f>
         <v>-1.4009272372336281E-3</v>
       </c>
-      <c r="AW8" s="3">
+      <c r="AW8">
         <f>(F8/SUM($C8:$N8)-U8/SUM($R8:$AC8))*SUM('RICBP-it0_damagesbyregionoutput'!$A7:$L7)</f>
         <v>6.8931603841435804E-2</v>
       </c>
-      <c r="AX8" s="3">
+      <c r="AX8">
         <f>(G8/SUM($C8:$N8)-V8/SUM($R8:$AC8))*SUM('RICBP-it0_damagesbyregionoutput'!$A7:$L7)</f>
         <v>0.14771760706500497</v>
       </c>
-      <c r="AY8" s="3">
+      <c r="AY8">
         <f>(H8/SUM($C8:$N8)-W8/SUM($R8:$AC8))*SUM('RICBP-it0_damagesbyregionoutput'!$A7:$L7)</f>
         <v>-0.20444759671858243</v>
       </c>
-      <c r="AZ8" s="3">
+      <c r="AZ8">
         <f>(I8/SUM($C8:$N8)-X8/SUM($R8:$AC8))*SUM('RICBP-it0_damagesbyregionoutput'!$A7:$L7)</f>
         <v>-5.7547714911497024E-2</v>
       </c>
-      <c r="BA8" s="3">
+      <c r="BA8">
         <f>(J8/SUM($C8:$N8)-Y8/SUM($R8:$AC8))*SUM('RICBP-it0_damagesbyregionoutput'!$A7:$L7)</f>
         <v>-0.19292736479281036</v>
       </c>
-      <c r="BB8" s="3">
+      <c r="BB8">
         <f>(K8/SUM($C8:$N8)-Z8/SUM($R8:$AC8))*SUM('RICBP-it0_damagesbyregionoutput'!$A7:$L7)</f>
         <v>-0.21758379873280179</v>
       </c>
-      <c r="BC8" s="3">
+      <c r="BC8">
         <f>(L8/SUM($C8:$N8)-AA8/SUM($R8:$AC8))*SUM('RICBP-it0_damagesbyregionoutput'!$A7:$L7)</f>
         <v>-8.9015322038386219E-2</v>
       </c>
-      <c r="BD8" s="3">
+      <c r="BD8">
         <f>(M8/SUM($C8:$N8)-AB8/SUM($R8:$AC8))*SUM('RICBP-it0_damagesbyregionoutput'!$A7:$L7)</f>
         <v>-2.9367037855331495E-2</v>
       </c>
-      <c r="BE8" s="3">
+      <c r="BE8">
         <f>(N8/SUM($C8:$N8)-AC8/SUM($R8:$AC8))*SUM('RICBP-it0_damagesbyregionoutput'!$A7:$L7)</f>
         <v>-0.11011750498507321</v>
       </c>
@@ -12396,51 +12396,51 @@
         <f t="shared" si="0"/>
         <v>-0.47684568816030276</v>
       </c>
-      <c r="AT9" s="3">
+      <c r="AT9">
         <f>(C9/SUM($C9:$N9)-R9/SUM($R9:$AC9))*SUM('RICBP-it0_damagesbyregionoutput'!$A8:$L8)</f>
         <v>0.66165476492950959</v>
       </c>
-      <c r="AU9" s="3">
+      <c r="AU9">
         <f>(D9/SUM($C9:$N9)-S9/SUM($R9:$AC9))*SUM('RICBP-it0_damagesbyregionoutput'!$A8:$L8)</f>
         <v>0.39529251355690759</v>
       </c>
-      <c r="AV9" s="3">
+      <c r="AV9">
         <f>(E9/SUM($C9:$N9)-T9/SUM($R9:$AC9))*SUM('RICBP-it0_damagesbyregionoutput'!$A8:$L8)</f>
         <v>2.6575775463825443E-2</v>
       </c>
-      <c r="AW9" s="3">
+      <c r="AW9">
         <f>(F9/SUM($C9:$N9)-U9/SUM($R9:$AC9))*SUM('RICBP-it0_damagesbyregionoutput'!$A8:$L8)</f>
         <v>0.10860196112932825</v>
       </c>
-      <c r="AX9" s="3">
+      <c r="AX9">
         <f>(G9/SUM($C9:$N9)-V9/SUM($R9:$AC9))*SUM('RICBP-it0_damagesbyregionoutput'!$A8:$L8)</f>
         <v>0.21895728624943564</v>
       </c>
-      <c r="AY9" s="3">
+      <c r="AY9">
         <f>(H9/SUM($C9:$N9)-W9/SUM($R9:$AC9))*SUM('RICBP-it0_damagesbyregionoutput'!$A8:$L8)</f>
         <v>-0.31849067339994941</v>
       </c>
-      <c r="AZ9" s="3">
+      <c r="AZ9">
         <f>(I9/SUM($C9:$N9)-X9/SUM($R9:$AC9))*SUM('RICBP-it0_damagesbyregionoutput'!$A8:$L8)</f>
         <v>-9.9261318771818166E-2</v>
       </c>
-      <c r="BA9" s="3">
+      <c r="BA9">
         <f>(J9/SUM($C9:$N9)-Y9/SUM($R9:$AC9))*SUM('RICBP-it0_damagesbyregionoutput'!$A8:$L8)</f>
         <v>-0.2775010382268166</v>
       </c>
-      <c r="BB9" s="3">
+      <c r="BB9">
         <f>(K9/SUM($C9:$N9)-Z9/SUM($R9:$AC9))*SUM('RICBP-it0_damagesbyregionoutput'!$A8:$L8)</f>
         <v>-0.4075671931515123</v>
       </c>
-      <c r="BC9" s="3">
+      <c r="BC9">
         <f>(L9/SUM($C9:$N9)-AA9/SUM($R9:$AC9))*SUM('RICBP-it0_damagesbyregionoutput'!$A8:$L8)</f>
         <v>-0.11514593599783569</v>
       </c>
-      <c r="BD9" s="3">
+      <c r="BD9">
         <f>(M9/SUM($C9:$N9)-AB9/SUM($R9:$AC9))*SUM('RICBP-it0_damagesbyregionoutput'!$A8:$L8)</f>
         <v>-2.9695039301199901E-2</v>
       </c>
-      <c r="BE9" s="3">
+      <c r="BE9">
         <f>(N9/SUM($C9:$N9)-AC9/SUM($R9:$AC9))*SUM('RICBP-it0_damagesbyregionoutput'!$A8:$L8)</f>
         <v>-0.16342110247987457</v>
       </c>
@@ -12656,51 +12656,51 @@
         <f t="shared" si="0"/>
         <v>-0.70563632668322962</v>
       </c>
-      <c r="AT10" s="3">
+      <c r="AT10">
         <f>(C10/SUM($C10:$N10)-R10/SUM($R10:$AC10))*SUM('RICBP-it0_damagesbyregionoutput'!$A9:$L9)</f>
         <v>0.9519705954175226</v>
       </c>
-      <c r="AU10" s="3">
+      <c r="AU10">
         <f>(D10/SUM($C10:$N10)-S10/SUM($R10:$AC10))*SUM('RICBP-it0_damagesbyregionoutput'!$A9:$L9)</f>
         <v>0.59498062698149756</v>
       </c>
-      <c r="AV10" s="3">
+      <c r="AV10">
         <f>(E10/SUM($C10:$N10)-T10/SUM($R10:$AC10))*SUM('RICBP-it0_damagesbyregionoutput'!$A9:$L9)</f>
         <v>6.6394206322480956E-2</v>
       </c>
-      <c r="AW10" s="3">
+      <c r="AW10">
         <f>(F10/SUM($C10:$N10)-U10/SUM($R10:$AC10))*SUM('RICBP-it0_damagesbyregionoutput'!$A9:$L9)</f>
         <v>0.15986607231323785</v>
       </c>
-      <c r="AX10" s="3">
+      <c r="AX10">
         <f>(G10/SUM($C10:$N10)-V10/SUM($R10:$AC10))*SUM('RICBP-it0_damagesbyregionoutput'!$A9:$L9)</f>
         <v>0.30908492549216815</v>
       </c>
-      <c r="AY10" s="3">
+      <c r="AY10">
         <f>(H10/SUM($C10:$N10)-W10/SUM($R10:$AC10))*SUM('RICBP-it0_damagesbyregionoutput'!$A9:$L9)</f>
         <v>-0.44656760909000209</v>
       </c>
-      <c r="AZ10" s="3">
+      <c r="AZ10">
         <f>(I10/SUM($C10:$N10)-X10/SUM($R10:$AC10))*SUM('RICBP-it0_damagesbyregionoutput'!$A9:$L9)</f>
         <v>-0.14766869850633954</v>
       </c>
-      <c r="BA10" s="3">
+      <c r="BA10">
         <f>(J10/SUM($C10:$N10)-Y10/SUM($R10:$AC10))*SUM('RICBP-it0_damagesbyregionoutput'!$A9:$L9)</f>
         <v>-0.37775262117592595</v>
       </c>
-      <c r="BB10" s="3">
+      <c r="BB10">
         <f>(K10/SUM($C10:$N10)-Z10/SUM($R10:$AC10))*SUM('RICBP-it0_damagesbyregionoutput'!$A9:$L9)</f>
         <v>-0.7100233903870522</v>
       </c>
-      <c r="BC10" s="3">
+      <c r="BC10">
         <f>(L10/SUM($C10:$N10)-AA10/SUM($R10:$AC10))*SUM('RICBP-it0_damagesbyregionoutput'!$A9:$L9)</f>
         <v>-0.14246442028609599</v>
       </c>
-      <c r="BD10" s="3">
+      <c r="BD10">
         <f>(M10/SUM($C10:$N10)-AB10/SUM($R10:$AC10))*SUM('RICBP-it0_damagesbyregionoutput'!$A9:$L9)</f>
         <v>-2.5540236362137581E-2</v>
       </c>
-      <c r="BE10" s="3">
+      <c r="BE10">
         <f>(N10/SUM($C10:$N10)-AC10/SUM($R10:$AC10))*SUM('RICBP-it0_damagesbyregionoutput'!$A9:$L9)</f>
         <v>-0.23227945071935366</v>
       </c>
@@ -12916,51 +12916,51 @@
         <f t="shared" si="0"/>
         <v>-1.0127329092152308</v>
       </c>
-      <c r="AT11" s="3">
+      <c r="AT11">
         <f>(C11/SUM($C11:$N11)-R11/SUM($R11:$AC11))*SUM('RICBP-it0_damagesbyregionoutput'!$A10:$L10)</f>
         <v>1.3139990174880145</v>
       </c>
-      <c r="AU11" s="3">
+      <c r="AU11">
         <f>(D11/SUM($C11:$N11)-S11/SUM($R11:$AC11))*SUM('RICBP-it0_damagesbyregionoutput'!$A10:$L10)</f>
         <v>0.85199310407300477</v>
       </c>
-      <c r="AV11" s="3">
+      <c r="AV11">
         <f>(E11/SUM($C11:$N11)-T11/SUM($R11:$AC11))*SUM('RICBP-it0_damagesbyregionoutput'!$A10:$L10)</f>
         <v>0.11845514286714902</v>
       </c>
-      <c r="AW11" s="3">
+      <c r="AW11">
         <f>(F11/SUM($C11:$N11)-U11/SUM($R11:$AC11))*SUM('RICBP-it0_damagesbyregionoutput'!$A10:$L10)</f>
         <v>0.22294831449574565</v>
       </c>
-      <c r="AX11" s="3">
+      <c r="AX11">
         <f>(G11/SUM($C11:$N11)-V11/SUM($R11:$AC11))*SUM('RICBP-it0_damagesbyregionoutput'!$A10:$L10)</f>
         <v>0.41879453154039126</v>
       </c>
-      <c r="AY11" s="3">
+      <c r="AY11">
         <f>(H11/SUM($C11:$N11)-W11/SUM($R11:$AC11))*SUM('RICBP-it0_damagesbyregionoutput'!$A10:$L10)</f>
         <v>-0.5848621478027497</v>
       </c>
-      <c r="AZ11" s="3">
+      <c r="AZ11">
         <f>(I11/SUM($C11:$N11)-X11/SUM($R11:$AC11))*SUM('RICBP-it0_damagesbyregionoutput'!$A10:$L10)</f>
         <v>-0.19735208674912785</v>
       </c>
-      <c r="BA11" s="3">
+      <c r="BA11">
         <f>(J11/SUM($C11:$N11)-Y11/SUM($R11:$AC11))*SUM('RICBP-it0_damagesbyregionoutput'!$A10:$L10)</f>
         <v>-0.49024031307457694</v>
       </c>
-      <c r="BB11" s="3">
+      <c r="BB11">
         <f>(K11/SUM($C11:$N11)-Z11/SUM($R11:$AC11))*SUM('RICBP-it0_damagesbyregionoutput'!$A10:$L10)</f>
         <v>-1.154671704196135</v>
       </c>
-      <c r="BC11" s="3">
+      <c r="BC11">
         <f>(L11/SUM($C11:$N11)-AA11/SUM($R11:$AC11))*SUM('RICBP-it0_damagesbyregionoutput'!$A10:$L10)</f>
         <v>-0.16778213861289937</v>
       </c>
-      <c r="BD11" s="3">
+      <c r="BD11">
         <f>(M11/SUM($C11:$N11)-AB11/SUM($R11:$AC11))*SUM('RICBP-it0_damagesbyregionoutput'!$A10:$L10)</f>
         <v>-1.5872040608963082E-2</v>
       </c>
-      <c r="BE11" s="3">
+      <c r="BE11">
         <f>(N11/SUM($C11:$N11)-AC11/SUM($R11:$AC11))*SUM('RICBP-it0_damagesbyregionoutput'!$A10:$L10)</f>
         <v>-0.31540967941985404</v>
       </c>
@@ -13176,51 +13176,51 @@
         <f t="shared" si="0"/>
         <v>-1.403527332390776</v>
       </c>
-      <c r="AT12" s="3">
+      <c r="AT12">
         <f>(C12/SUM($C12:$N12)-R12/SUM($R12:$AC12))*SUM('RICBP-it0_damagesbyregionoutput'!$A11:$L11)</f>
         <v>1.7492618931575943</v>
       </c>
-      <c r="AU12" s="3">
+      <c r="AU12">
         <f>(D12/SUM($C12:$N12)-S12/SUM($R12:$AC12))*SUM('RICBP-it0_damagesbyregionoutput'!$A11:$L11)</f>
         <v>1.1686285214079213</v>
       </c>
-      <c r="AV12" s="3">
+      <c r="AV12">
         <f>(E12/SUM($C12:$N12)-T12/SUM($R12:$AC12))*SUM('RICBP-it0_damagesbyregionoutput'!$A11:$L11)</f>
         <v>0.1828867279981482</v>
       </c>
-      <c r="AW12" s="3">
+      <c r="AW12">
         <f>(F12/SUM($C12:$N12)-U12/SUM($R12:$AC12))*SUM('RICBP-it0_damagesbyregionoutput'!$A11:$L11)</f>
         <v>0.29736011310671462</v>
       </c>
-      <c r="AX12" s="3">
+      <c r="AX12">
         <f>(G12/SUM($C12:$N12)-V12/SUM($R12:$AC12))*SUM('RICBP-it0_damagesbyregionoutput'!$A11:$L11)</f>
         <v>0.54765953914195031</v>
       </c>
-      <c r="AY12" s="3">
+      <c r="AY12">
         <f>(H12/SUM($C12:$N12)-W12/SUM($R12:$AC12))*SUM('RICBP-it0_damagesbyregionoutput'!$A11:$L11)</f>
         <v>-0.73208174575079199</v>
       </c>
-      <c r="AZ12" s="3">
+      <c r="AZ12">
         <f>(I12/SUM($C12:$N12)-X12/SUM($R12:$AC12))*SUM('RICBP-it0_damagesbyregionoutput'!$A11:$L11)</f>
         <v>-0.24218750524996785</v>
       </c>
-      <c r="BA12" s="3">
+      <c r="BA12">
         <f>(J12/SUM($C12:$N12)-Y12/SUM($R12:$AC12))*SUM('RICBP-it0_damagesbyregionoutput'!$A11:$L11)</f>
         <v>-0.61007654664202859</v>
       </c>
-      <c r="BB12" s="3">
+      <c r="BB12">
         <f>(K12/SUM($C12:$N12)-Z12/SUM($R12:$AC12))*SUM('RICBP-it0_damagesbyregionoutput'!$A11:$L11)</f>
         <v>-1.7640897502607</v>
       </c>
-      <c r="BC12" s="3">
+      <c r="BC12">
         <f>(L12/SUM($C12:$N12)-AA12/SUM($R12:$AC12))*SUM('RICBP-it0_damagesbyregionoutput'!$A11:$L11)</f>
         <v>-0.18744107369015914</v>
       </c>
-      <c r="BD12" s="3">
+      <c r="BD12">
         <f>(M12/SUM($C12:$N12)-AB12/SUM($R12:$AC12))*SUM('RICBP-it0_damagesbyregionoutput'!$A11:$L11)</f>
         <v>-5.7574107395280509E-5</v>
       </c>
-      <c r="BE12" s="3">
+      <c r="BE12">
         <f>(N12/SUM($C12:$N12)-AC12/SUM($R12:$AC12))*SUM('RICBP-it0_damagesbyregionoutput'!$A11:$L11)</f>
         <v>-0.40986259911128708</v>
       </c>
@@ -13436,51 +13436,51 @@
         <f t="shared" si="0"/>
         <v>-1.8994054492751693</v>
       </c>
-      <c r="AT13" s="3">
+      <c r="AT13">
         <f>(C13/SUM($C13:$N13)-R13/SUM($R13:$AC13))*SUM('RICBP-it0_damagesbyregionoutput'!$A12:$L12)</f>
         <v>2.2506627572666176</v>
       </c>
-      <c r="AU13" s="3">
+      <c r="AU13">
         <f>(D13/SUM($C13:$N13)-S13/SUM($R13:$AC13))*SUM('RICBP-it0_damagesbyregionoutput'!$A12:$L12)</f>
         <v>1.5385123497703344</v>
       </c>
-      <c r="AV13" s="3">
+      <c r="AV13">
         <f>(E13/SUM($C13:$N13)-T13/SUM($R13:$AC13))*SUM('RICBP-it0_damagesbyregionoutput'!$A12:$L12)</f>
         <v>0.25802834559162019</v>
       </c>
-      <c r="AW13" s="3">
+      <c r="AW13">
         <f>(F13/SUM($C13:$N13)-U13/SUM($R13:$AC13))*SUM('RICBP-it0_damagesbyregionoutput'!$A12:$L12)</f>
         <v>0.38065965657617012</v>
       </c>
-      <c r="AX13" s="3">
+      <c r="AX13">
         <f>(G13/SUM($C13:$N13)-V13/SUM($R13:$AC13))*SUM('RICBP-it0_damagesbyregionoutput'!$A12:$L12)</f>
         <v>0.69198075091116928</v>
       </c>
-      <c r="AY13" s="3">
+      <c r="AY13">
         <f>(H13/SUM($C13:$N13)-W13/SUM($R13:$AC13))*SUM('RICBP-it0_damagesbyregionoutput'!$A12:$L12)</f>
         <v>-0.90258040690272845</v>
       </c>
-      <c r="AZ13" s="3">
+      <c r="AZ13">
         <f>(I13/SUM($C13:$N13)-X13/SUM($R13:$AC13))*SUM('RICBP-it0_damagesbyregionoutput'!$A12:$L12)</f>
         <v>-0.28531456860724125</v>
       </c>
-      <c r="BA13" s="3">
+      <c r="BA13">
         <f>(J13/SUM($C13:$N13)-Y13/SUM($R13:$AC13))*SUM('RICBP-it0_damagesbyregionoutput'!$A12:$L12)</f>
         <v>-0.73161786513514626</v>
       </c>
-      <c r="BB13" s="3">
+      <c r="BB13">
         <f>(K13/SUM($C13:$N13)-Z13/SUM($R13:$AC13))*SUM('RICBP-it0_damagesbyregionoutput'!$A12:$L12)</f>
         <v>-2.5047757241022932</v>
       </c>
-      <c r="BC13" s="3">
+      <c r="BC13">
         <f>(L13/SUM($C13:$N13)-AA13/SUM($R13:$AC13))*SUM('RICBP-it0_damagesbyregionoutput'!$A12:$L12)</f>
         <v>-0.20161945065187925</v>
       </c>
-      <c r="BD13" s="3">
+      <c r="BD13">
         <f>(M13/SUM($C13:$N13)-AB13/SUM($R13:$AC13))*SUM('RICBP-it0_damagesbyregionoutput'!$A12:$L12)</f>
         <v>2.2150475729472825E-2</v>
       </c>
-      <c r="BE13" s="3">
+      <c r="BE13">
         <f>(N13/SUM($C13:$N13)-AC13/SUM($R13:$AC13))*SUM('RICBP-it0_damagesbyregionoutput'!$A12:$L12)</f>
         <v>-0.51608632044609559</v>
       </c>
@@ -13696,51 +13696,51 @@
         <f t="shared" si="0"/>
         <v>-2.5164858360564466</v>
       </c>
-      <c r="AT14" s="3">
+      <c r="AT14">
         <f>(C14/SUM($C14:$N14)-R14/SUM($R14:$AC14))*SUM('RICBP-it0_damagesbyregionoutput'!$A13:$L13)</f>
         <v>2.8028235530762173</v>
       </c>
-      <c r="AU14" s="3">
+      <c r="AU14">
         <f>(D14/SUM($C14:$N14)-S14/SUM($R14:$AC14))*SUM('RICBP-it0_damagesbyregionoutput'!$A13:$L13)</f>
         <v>1.9504733426762906</v>
       </c>
-      <c r="AV14" s="3">
+      <c r="AV14">
         <f>(E14/SUM($C14:$N14)-T14/SUM($R14:$AC14))*SUM('RICBP-it0_damagesbyregionoutput'!$A13:$L13)</f>
         <v>0.34163326351975376</v>
       </c>
-      <c r="AW14" s="3">
+      <c r="AW14">
         <f>(F14/SUM($C14:$N14)-U14/SUM($R14:$AC14))*SUM('RICBP-it0_damagesbyregionoutput'!$A13:$L13)</f>
         <v>0.47157785621906689</v>
       </c>
-      <c r="AX14" s="3">
+      <c r="AX14">
         <f>(G14/SUM($C14:$N14)-V14/SUM($R14:$AC14))*SUM('RICBP-it0_damagesbyregionoutput'!$A13:$L13)</f>
         <v>0.8480999123839752</v>
       </c>
-      <c r="AY14" s="3">
+      <c r="AY14">
         <f>(H14/SUM($C14:$N14)-W14/SUM($R14:$AC14))*SUM('RICBP-it0_damagesbyregionoutput'!$A13:$L13)</f>
         <v>-1.1039261902892437</v>
       </c>
-      <c r="AZ14" s="3">
+      <c r="AZ14">
         <f>(I14/SUM($C14:$N14)-X14/SUM($R14:$AC14))*SUM('RICBP-it0_damagesbyregionoutput'!$A13:$L13)</f>
         <v>-0.32624505676537813</v>
       </c>
-      <c r="BA14" s="3">
+      <c r="BA14">
         <f>(J14/SUM($C14:$N14)-Y14/SUM($R14:$AC14))*SUM('RICBP-it0_damagesbyregionoutput'!$A13:$L13)</f>
         <v>-0.85000583661306706</v>
       </c>
-      <c r="BB14" s="3">
+      <c r="BB14">
         <f>(K14/SUM($C14:$N14)-Z14/SUM($R14:$AC14))*SUM('RICBP-it0_damagesbyregionoutput'!$A13:$L13)</f>
         <v>-3.3433867309957659</v>
       </c>
-      <c r="BC14" s="3">
+      <c r="BC14">
         <f>(L14/SUM($C14:$N14)-AA14/SUM($R14:$AC14))*SUM('RICBP-it0_damagesbyregionoutput'!$A13:$L13)</f>
         <v>-0.20907009562562776</v>
       </c>
-      <c r="BD14" s="3">
+      <c r="BD14">
         <f>(M14/SUM($C14:$N14)-AB14/SUM($R14:$AC14))*SUM('RICBP-it0_damagesbyregionoutput'!$A13:$L13)</f>
         <v>5.0124739193433909E-2</v>
       </c>
-      <c r="BE14" s="3">
+      <c r="BE14">
         <f>(N14/SUM($C14:$N14)-AC14/SUM($R14:$AC14))*SUM('RICBP-it0_damagesbyregionoutput'!$A13:$L13)</f>
         <v>-0.63209875677965688</v>
       </c>
@@ -13956,51 +13956,51 @@
         <f t="shared" si="0"/>
         <v>-3.2725127594145422</v>
       </c>
-      <c r="AT15" s="3">
+      <c r="AT15">
         <f>(C15/SUM($C15:$N15)-R15/SUM($R15:$AC15))*SUM('RICBP-it0_damagesbyregionoutput'!$A14:$L14)</f>
         <v>3.3865981305124548</v>
       </c>
-      <c r="AU15" s="3">
+      <c r="AU15">
         <f>(D15/SUM($C15:$N15)-S15/SUM($R15:$AC15))*SUM('RICBP-it0_damagesbyregionoutput'!$A14:$L14)</f>
         <v>2.3921618998714633</v>
       </c>
-      <c r="AV15" s="3">
+      <c r="AV15">
         <f>(E15/SUM($C15:$N15)-T15/SUM($R15:$AC15))*SUM('RICBP-it0_damagesbyregionoutput'!$A14:$L14)</f>
         <v>0.43111924496069798</v>
       </c>
-      <c r="AW15" s="3">
+      <c r="AW15">
         <f>(F15/SUM($C15:$N15)-U15/SUM($R15:$AC15))*SUM('RICBP-it0_damagesbyregionoutput'!$A14:$L14)</f>
         <v>0.56752636973618242</v>
       </c>
-      <c r="AX15" s="3">
+      <c r="AX15">
         <f>(G15/SUM($C15:$N15)-V15/SUM($R15:$AC15))*SUM('RICBP-it0_damagesbyregionoutput'!$A14:$L14)</f>
         <v>1.0114063247023604</v>
       </c>
-      <c r="AY15" s="3">
+      <c r="AY15">
         <f>(H15/SUM($C15:$N15)-W15/SUM($R15:$AC15))*SUM('RICBP-it0_damagesbyregionoutput'!$A14:$L14)</f>
         <v>-1.3269870642188644</v>
       </c>
-      <c r="AZ15" s="3">
+      <c r="AZ15">
         <f>(I15/SUM($C15:$N15)-X15/SUM($R15:$AC15))*SUM('RICBP-it0_damagesbyregionoutput'!$A14:$L14)</f>
         <v>-0.36491635193095467</v>
       </c>
-      <c r="BA15" s="3">
+      <c r="BA15">
         <f>(J15/SUM($C15:$N15)-Y15/SUM($R15:$AC15))*SUM('RICBP-it0_damagesbyregionoutput'!$A14:$L14)</f>
         <v>-0.96331264789130477</v>
       </c>
-      <c r="BB15" s="3">
+      <c r="BB15">
         <f>(K15/SUM($C15:$N15)-Z15/SUM($R15:$AC15))*SUM('RICBP-it0_damagesbyregionoutput'!$A14:$L14)</f>
         <v>-4.2505048261524117</v>
       </c>
-      <c r="BC15" s="3">
+      <c r="BC15">
         <f>(L15/SUM($C15:$N15)-AA15/SUM($R15:$AC15))*SUM('RICBP-it0_damagesbyregionoutput'!$A14:$L14)</f>
         <v>-0.20950467269247267</v>
       </c>
-      <c r="BD15" s="3">
+      <c r="BD15">
         <f>(M15/SUM($C15:$N15)-AB15/SUM($R15:$AC15))*SUM('RICBP-it0_damagesbyregionoutput'!$A14:$L14)</f>
         <v>8.2737114795640485E-2</v>
       </c>
-      <c r="BE15" s="3">
+      <c r="BE15">
         <f>(N15/SUM($C15:$N15)-AC15/SUM($R15:$AC15))*SUM('RICBP-it0_damagesbyregionoutput'!$A14:$L14)</f>
         <v>-0.75632352169279449</v>
       </c>
@@ -14216,51 +14216,51 @@
         <f t="shared" si="0"/>
         <v>-4.1923535619809842</v>
       </c>
-      <c r="AT16" s="3">
+      <c r="AT16">
         <f>(C16/SUM($C16:$N16)-R16/SUM($R16:$AC16))*SUM('RICBP-it0_damagesbyregionoutput'!$A15:$L15)</f>
         <v>4.007094883604033</v>
       </c>
-      <c r="AU16" s="3">
+      <c r="AU16">
         <f>(D16/SUM($C16:$N16)-S16/SUM($R16:$AC16))*SUM('RICBP-it0_damagesbyregionoutput'!$A15:$L15)</f>
         <v>2.8600443477078072</v>
       </c>
-      <c r="AV16" s="3">
+      <c r="AV16">
         <f>(E16/SUM($C16:$N16)-T16/SUM($R16:$AC16))*SUM('RICBP-it0_damagesbyregionoutput'!$A15:$L15)</f>
         <v>0.52569903508039295</v>
       </c>
-      <c r="AW16" s="3">
+      <c r="AW16">
         <f>(F16/SUM($C16:$N16)-U16/SUM($R16:$AC16))*SUM('RICBP-it0_damagesbyregionoutput'!$A15:$L15)</f>
         <v>0.66834563764399191</v>
       </c>
-      <c r="AX16" s="3">
+      <c r="AX16">
         <f>(G16/SUM($C16:$N16)-V16/SUM($R16:$AC16))*SUM('RICBP-it0_damagesbyregionoutput'!$A15:$L15)</f>
         <v>1.1816599248175055</v>
       </c>
-      <c r="AY16" s="3">
+      <c r="AY16">
         <f>(H16/SUM($C16:$N16)-W16/SUM($R16:$AC16))*SUM('RICBP-it0_damagesbyregionoutput'!$A15:$L15)</f>
         <v>-1.5737127452357016</v>
       </c>
-      <c r="AZ16" s="3">
+      <c r="AZ16">
         <f>(I16/SUM($C16:$N16)-X16/SUM($R16:$AC16))*SUM('RICBP-it0_damagesbyregionoutput'!$A15:$L15)</f>
         <v>-0.40258390735528687</v>
       </c>
-      <c r="BA16" s="3">
+      <c r="BA16">
         <f>(J16/SUM($C16:$N16)-Y16/SUM($R16:$AC16))*SUM('RICBP-it0_damagesbyregionoutput'!$A15:$L15)</f>
         <v>-1.0703869784022462</v>
       </c>
-      <c r="BB16" s="3">
+      <c r="BB16">
         <f>(K16/SUM($C16:$N16)-Z16/SUM($R16:$AC16))*SUM('RICBP-it0_damagesbyregionoutput'!$A15:$L15)</f>
         <v>-5.2195183895237065</v>
       </c>
-      <c r="BC16" s="3">
+      <c r="BC16">
         <f>(L16/SUM($C16:$N16)-AA16/SUM($R16:$AC16))*SUM('RICBP-it0_damagesbyregionoutput'!$A15:$L15)</f>
         <v>-0.20397707851585078</v>
       </c>
-      <c r="BD16" s="3">
+      <c r="BD16">
         <f>(M16/SUM($C16:$N16)-AB16/SUM($R16:$AC16))*SUM('RICBP-it0_damagesbyregionoutput'!$A15:$L15)</f>
         <v>0.1185311976266077</v>
       </c>
-      <c r="BE16" s="3">
+      <c r="BE16">
         <f>(N16/SUM($C16:$N16)-AC16/SUM($R16:$AC16))*SUM('RICBP-it0_damagesbyregionoutput'!$A15:$L15)</f>
         <v>-0.89119592744754583</v>
       </c>
@@ -14476,51 +14476,51 @@
         <f t="shared" si="0"/>
         <v>-5.2928742811173688</v>
       </c>
-      <c r="AT17" s="3">
+      <c r="AT17">
         <f>(C17/SUM($C17:$N17)-R17/SUM($R17:$AC17))*SUM('RICBP-it0_damagesbyregionoutput'!$A16:$L16)</f>
         <v>4.6532425837308207</v>
       </c>
-      <c r="AU17" s="3">
+      <c r="AU17">
         <f>(D17/SUM($C17:$N17)-S17/SUM($R17:$AC17))*SUM('RICBP-it0_damagesbyregionoutput'!$A16:$L16)</f>
         <v>3.3417116818885413</v>
       </c>
-      <c r="AV17" s="3">
+      <c r="AV17">
         <f>(E17/SUM($C17:$N17)-T17/SUM($R17:$AC17))*SUM('RICBP-it0_damagesbyregionoutput'!$A16:$L16)</f>
         <v>0.62315141440736421</v>
       </c>
-      <c r="AW17" s="3">
+      <c r="AW17">
         <f>(F17/SUM($C17:$N17)-U17/SUM($R17:$AC17))*SUM('RICBP-it0_damagesbyregionoutput'!$A16:$L16)</f>
         <v>0.77230273030599172</v>
       </c>
-      <c r="AX17" s="3">
+      <c r="AX17">
         <f>(G17/SUM($C17:$N17)-V17/SUM($R17:$AC17))*SUM('RICBP-it0_damagesbyregionoutput'!$A16:$L16)</f>
         <v>1.3560048175289536</v>
       </c>
-      <c r="AY17" s="3">
+      <c r="AY17">
         <f>(H17/SUM($C17:$N17)-W17/SUM($R17:$AC17))*SUM('RICBP-it0_damagesbyregionoutput'!$A16:$L16)</f>
         <v>-1.8459965783195789</v>
       </c>
-      <c r="AZ17" s="3">
+      <c r="AZ17">
         <f>(I17/SUM($C17:$N17)-X17/SUM($R17:$AC17))*SUM('RICBP-it0_damagesbyregionoutput'!$A16:$L16)</f>
         <v>-0.43187078774938653</v>
       </c>
-      <c r="BA17" s="3">
+      <c r="BA17">
         <f>(J17/SUM($C17:$N17)-Y17/SUM($R17:$AC17))*SUM('RICBP-it0_damagesbyregionoutput'!$A16:$L16)</f>
         <v>-1.1644389475432566</v>
       </c>
-      <c r="BB17" s="3">
+      <c r="BB17">
         <f>(K17/SUM($C17:$N17)-Z17/SUM($R17:$AC17))*SUM('RICBP-it0_damagesbyregionoutput'!$A16:$L16)</f>
         <v>-6.2301620352620732</v>
       </c>
-      <c r="BC17" s="3">
+      <c r="BC17">
         <f>(L17/SUM($C17:$N17)-AA17/SUM($R17:$AC17))*SUM('RICBP-it0_damagesbyregionoutput'!$A16:$L16)</f>
         <v>-0.19542219883931922</v>
       </c>
-      <c r="BD17" s="3">
+      <c r="BD17">
         <f>(M17/SUM($C17:$N17)-AB17/SUM($R17:$AC17))*SUM('RICBP-it0_damagesbyregionoutput'!$A16:$L16)</f>
         <v>0.15772060663443482</v>
       </c>
-      <c r="BE17" s="3">
+      <c r="BE17">
         <f>(N17/SUM($C17:$N17)-AC17/SUM($R17:$AC17))*SUM('RICBP-it0_damagesbyregionoutput'!$A16:$L16)</f>
         <v>-1.0362432867824991</v>
       </c>
@@ -14736,51 +14736,51 @@
         <f t="shared" si="0"/>
         <v>-6.5374260213925552</v>
       </c>
-      <c r="AT18" s="3">
+      <c r="AT18">
         <f>(C18/SUM($C18:$N18)-R18/SUM($R18:$AC18))*SUM('RICBP-it0_damagesbyregionoutput'!$A17:$L17)</f>
         <v>5.3235005960171913</v>
       </c>
-      <c r="AU18" s="3">
+      <c r="AU18">
         <f>(D18/SUM($C18:$N18)-S18/SUM($R18:$AC18))*SUM('RICBP-it0_damagesbyregionoutput'!$A17:$L17)</f>
         <v>3.8346939931269719</v>
       </c>
-      <c r="AV18" s="3">
+      <c r="AV18">
         <f>(E18/SUM($C18:$N18)-T18/SUM($R18:$AC18))*SUM('RICBP-it0_damagesbyregionoutput'!$A17:$L17)</f>
         <v>0.72316000973838779</v>
       </c>
-      <c r="AW18" s="3">
+      <c r="AW18">
         <f>(F18/SUM($C18:$N18)-U18/SUM($R18:$AC18))*SUM('RICBP-it0_damagesbyregionoutput'!$A17:$L17)</f>
         <v>0.87934906600904894</v>
       </c>
-      <c r="AX18" s="3">
+      <c r="AX18">
         <f>(G18/SUM($C18:$N18)-V18/SUM($R18:$AC18))*SUM('RICBP-it0_damagesbyregionoutput'!$A17:$L17)</f>
         <v>1.5345765509694969</v>
       </c>
-      <c r="AY18" s="3">
+      <c r="AY18">
         <f>(H18/SUM($C18:$N18)-W18/SUM($R18:$AC18))*SUM('RICBP-it0_damagesbyregionoutput'!$A17:$L17)</f>
         <v>-2.1484584708082632</v>
       </c>
-      <c r="AZ18" s="3">
+      <c r="AZ18">
         <f>(I18/SUM($C18:$N18)-X18/SUM($R18:$AC18))*SUM('RICBP-it0_damagesbyregionoutput'!$A17:$L17)</f>
         <v>-0.4513100223526707</v>
       </c>
-      <c r="BA18" s="3">
+      <c r="BA18">
         <f>(J18/SUM($C18:$N18)-Y18/SUM($R18:$AC18))*SUM('RICBP-it0_damagesbyregionoutput'!$A17:$L17)</f>
         <v>-1.2479349910185749</v>
       </c>
-      <c r="BB18" s="3">
+      <c r="BB18">
         <f>(K18/SUM($C18:$N18)-Z18/SUM($R18:$AC18))*SUM('RICBP-it0_damagesbyregionoutput'!$A17:$L17)</f>
         <v>-7.2840055634164544</v>
       </c>
-      <c r="BC18" s="3">
+      <c r="BC18">
         <f>(L18/SUM($C18:$N18)-AA18/SUM($R18:$AC18))*SUM('RICBP-it0_damagesbyregionoutput'!$A17:$L17)</f>
         <v>-0.18002575837898621</v>
       </c>
-      <c r="BD18" s="3">
+      <c r="BD18">
         <f>(M18/SUM($C18:$N18)-AB18/SUM($R18:$AC18))*SUM('RICBP-it0_damagesbyregionoutput'!$A17:$L17)</f>
         <v>0.19967611493220352</v>
       </c>
-      <c r="BE18" s="3">
+      <c r="BE18">
         <f>(N18/SUM($C18:$N18)-AC18/SUM($R18:$AC18))*SUM('RICBP-it0_damagesbyregionoutput'!$A17:$L17)</f>
         <v>-1.1832215248183531</v>
       </c>
@@ -14996,51 +14996,51 @@
         <f t="shared" si="3"/>
         <v>-7.9298963025883449</v>
       </c>
-      <c r="AT19" s="3">
+      <c r="AT19">
         <f>(C19/SUM($C19:$N19)-R19/SUM($R19:$AC19))*SUM('RICBP-it0_damagesbyregionoutput'!$A18:$L18)</f>
         <v>6.0239249225210187</v>
       </c>
-      <c r="AU19" s="3">
+      <c r="AU19">
         <f>(D19/SUM($C19:$N19)-S19/SUM($R19:$AC19))*SUM('RICBP-it0_damagesbyregionoutput'!$A18:$L18)</f>
         <v>4.3472888158303826</v>
       </c>
-      <c r="AV19" s="3">
+      <c r="AV19">
         <f>(E19/SUM($C19:$N19)-T19/SUM($R19:$AC19))*SUM('RICBP-it0_damagesbyregionoutput'!$A18:$L18)</f>
         <v>0.82743671649102668</v>
       </c>
-      <c r="AW19" s="3">
+      <c r="AW19">
         <f>(F19/SUM($C19:$N19)-U19/SUM($R19:$AC19))*SUM('RICBP-it0_damagesbyregionoutput'!$A18:$L18)</f>
         <v>0.99063255061633937</v>
       </c>
-      <c r="AX19" s="3">
+      <c r="AX19">
         <f>(G19/SUM($C19:$N19)-V19/SUM($R19:$AC19))*SUM('RICBP-it0_damagesbyregionoutput'!$A18:$L18)</f>
         <v>1.7195102794590298</v>
       </c>
-      <c r="AY19" s="3">
+      <c r="AY19">
         <f>(H19/SUM($C19:$N19)-W19/SUM($R19:$AC19))*SUM('RICBP-it0_damagesbyregionoutput'!$A18:$L18)</f>
         <v>-2.4852562391340425</v>
       </c>
-      <c r="AZ19" s="3">
+      <c r="AZ19">
         <f>(I19/SUM($C19:$N19)-X19/SUM($R19:$AC19))*SUM('RICBP-it0_damagesbyregionoutput'!$A18:$L18)</f>
         <v>-0.46099894270400149</v>
       </c>
-      <c r="BA19" s="3">
+      <c r="BA19">
         <f>(J19/SUM($C19:$N19)-Y19/SUM($R19:$AC19))*SUM('RICBP-it0_damagesbyregionoutput'!$A18:$L18)</f>
         <v>-1.3235781621056073</v>
       </c>
-      <c r="BB19" s="3">
+      <c r="BB19">
         <f>(K19/SUM($C19:$N19)-Z19/SUM($R19:$AC19))*SUM('RICBP-it0_damagesbyregionoutput'!$A18:$L18)</f>
         <v>-8.3923413074733251</v>
       </c>
-      <c r="BC19" s="3">
+      <c r="BC19">
         <f>(L19/SUM($C19:$N19)-AA19/SUM($R19:$AC19))*SUM('RICBP-it0_damagesbyregionoutput'!$A18:$L18)</f>
         <v>-0.1567979996886239</v>
       </c>
-      <c r="BD19" s="3">
+      <c r="BD19">
         <f>(M19/SUM($C19:$N19)-AB19/SUM($R19:$AC19))*SUM('RICBP-it0_damagesbyregionoutput'!$A18:$L18)</f>
         <v>0.2441760974566804</v>
       </c>
-      <c r="BE19" s="3">
+      <c r="BE19">
         <f>(N19/SUM($C19:$N19)-AC19/SUM($R19:$AC19))*SUM('RICBP-it0_damagesbyregionoutput'!$A18:$L18)</f>
         <v>-1.3339967312688827</v>
       </c>
@@ -15256,51 +15256,51 @@
         <f t="shared" si="3"/>
         <v>-9.4758869163897579</v>
       </c>
-      <c r="AT20" s="3">
+      <c r="AT20">
         <f>(C20/SUM($C20:$N20)-R20/SUM($R20:$AC20))*SUM('RICBP-it0_damagesbyregionoutput'!$A19:$L19)</f>
         <v>6.7618332647444923</v>
       </c>
-      <c r="AU20" s="3">
+      <c r="AU20">
         <f>(D20/SUM($C20:$N20)-S20/SUM($R20:$AC20))*SUM('RICBP-it0_damagesbyregionoutput'!$A19:$L19)</f>
         <v>4.8849550956458261</v>
       </c>
-      <c r="AV20" s="3">
+      <c r="AV20">
         <f>(E20/SUM($C20:$N20)-T20/SUM($R20:$AC20))*SUM('RICBP-it0_damagesbyregionoutput'!$A19:$L19)</f>
         <v>0.93705961070244825</v>
       </c>
-      <c r="AW20" s="3">
+      <c r="AW20">
         <f>(F20/SUM($C20:$N20)-U20/SUM($R20:$AC20))*SUM('RICBP-it0_damagesbyregionoutput'!$A19:$L19)</f>
         <v>1.1074532969322437</v>
       </c>
-      <c r="AX20" s="3">
+      <c r="AX20">
         <f>(G20/SUM($C20:$N20)-V20/SUM($R20:$AC20))*SUM('RICBP-it0_damagesbyregionoutput'!$A19:$L19)</f>
         <v>1.9131313206244436</v>
       </c>
-      <c r="AY20" s="3">
+      <c r="AY20">
         <f>(H20/SUM($C20:$N20)-W20/SUM($R20:$AC20))*SUM('RICBP-it0_damagesbyregionoutput'!$A19:$L19)</f>
         <v>-2.8592660355012947</v>
       </c>
-      <c r="AZ20" s="3">
+      <c r="AZ20">
         <f>(I20/SUM($C20:$N20)-X20/SUM($R20:$AC20))*SUM('RICBP-it0_damagesbyregionoutput'!$A19:$L19)</f>
         <v>-0.46061830780675161</v>
       </c>
-      <c r="BA20" s="3">
+      <c r="BA20">
         <f>(J20/SUM($C20:$N20)-Y20/SUM($R20:$AC20))*SUM('RICBP-it0_damagesbyregionoutput'!$A19:$L19)</f>
         <v>-1.3933138130341878</v>
       </c>
-      <c r="BB20" s="3">
+      <c r="BB20">
         <f>(K20/SUM($C20:$N20)-Z20/SUM($R20:$AC20))*SUM('RICBP-it0_damagesbyregionoutput'!$A19:$L19)</f>
         <v>-9.5664123547883069</v>
       </c>
-      <c r="BC20" s="3">
+      <c r="BC20">
         <f>(L20/SUM($C20:$N20)-AA20/SUM($R20:$AC20))*SUM('RICBP-it0_damagesbyregionoutput'!$A19:$L19)</f>
         <v>-0.12591923462399879</v>
       </c>
-      <c r="BD20" s="3">
+      <c r="BD20">
         <f>(M20/SUM($C20:$N20)-AB20/SUM($R20:$AC20))*SUM('RICBP-it0_damagesbyregionoutput'!$A19:$L19)</f>
         <v>0.29145850991057071</v>
       </c>
-      <c r="BE20" s="3">
+      <c r="BE20">
         <f>(N20/SUM($C20:$N20)-AC20/SUM($R20:$AC20))*SUM('RICBP-it0_damagesbyregionoutput'!$A19:$L19)</f>
         <v>-1.4903613528054966</v>
       </c>
@@ -15516,51 +15516,51 @@
         <f t="shared" si="3"/>
         <v>-11.183980442024749</v>
       </c>
-      <c r="AT21" s="3">
+      <c r="AT21">
         <f>(C21/SUM($C21:$N21)-R21/SUM($R21:$AC21))*SUM('RICBP-it0_damagesbyregionoutput'!$A20:$L20)</f>
         <v>7.5430415180765413</v>
       </c>
-      <c r="AU21" s="3">
+      <c r="AU21">
         <f>(D21/SUM($C21:$N21)-S21/SUM($R21:$AC21))*SUM('RICBP-it0_damagesbyregionoutput'!$A20:$L20)</f>
         <v>5.4522132341669698</v>
       </c>
-      <c r="AV21" s="3">
+      <c r="AV21">
         <f>(E21/SUM($C21:$N21)-T21/SUM($R21:$AC21))*SUM('RICBP-it0_damagesbyregionoutput'!$A20:$L20)</f>
         <v>1.0529179421207244</v>
       </c>
-      <c r="AW21" s="3">
+      <c r="AW21">
         <f>(F21/SUM($C21:$N21)-U21/SUM($R21:$AC21))*SUM('RICBP-it0_damagesbyregionoutput'!$A20:$L20)</f>
         <v>1.2308318782646968</v>
       </c>
-      <c r="AX21" s="3">
+      <c r="AX21">
         <f>(G21/SUM($C21:$N21)-V21/SUM($R21:$AC21))*SUM('RICBP-it0_damagesbyregionoutput'!$A20:$L20)</f>
         <v>2.1172446106748479</v>
       </c>
-      <c r="AY21" s="3">
+      <c r="AY21">
         <f>(H21/SUM($C21:$N21)-W21/SUM($R21:$AC21))*SUM('RICBP-it0_damagesbyregionoutput'!$A20:$L20)</f>
         <v>-3.2725648530689995</v>
       </c>
-      <c r="AZ21" s="3">
+      <c r="AZ21">
         <f>(I21/SUM($C21:$N21)-X21/SUM($R21:$AC21))*SUM('RICBP-it0_damagesbyregionoutput'!$A20:$L20)</f>
         <v>-0.44989138654497252</v>
       </c>
-      <c r="BA21" s="3">
+      <c r="BA21">
         <f>(J21/SUM($C21:$N21)-Y21/SUM($R21:$AC21))*SUM('RICBP-it0_damagesbyregionoutput'!$A20:$L20)</f>
         <v>-1.4584793426351399</v>
       </c>
-      <c r="BB21" s="3">
+      <c r="BB21">
         <f>(K21/SUM($C21:$N21)-Z21/SUM($R21:$AC21))*SUM('RICBP-it0_damagesbyregionoutput'!$A20:$L20)</f>
         <v>-10.815650757245068</v>
       </c>
-      <c r="BC21" s="3">
+      <c r="BC21">
         <f>(L21/SUM($C21:$N21)-AA21/SUM($R21:$AC21))*SUM('RICBP-it0_damagesbyregionoutput'!$A20:$L20)</f>
         <v>-8.7490771365153888E-2</v>
       </c>
-      <c r="BD21" s="3">
+      <c r="BD21">
         <f>(M21/SUM($C21:$N21)-AB21/SUM($R21:$AC21))*SUM('RICBP-it0_damagesbyregionoutput'!$A20:$L20)</f>
         <v>0.34181250831202475</v>
       </c>
-      <c r="BE21" s="3">
+      <c r="BE21">
         <f>(N21/SUM($C21:$N21)-AC21/SUM($R21:$AC21))*SUM('RICBP-it0_damagesbyregionoutput'!$A20:$L20)</f>
         <v>-1.6539845807564812</v>
       </c>
@@ -15776,51 +15776,51 @@
         <f t="shared" si="3"/>
         <v>-13.065402504033498</v>
       </c>
-      <c r="AT22" s="3">
+      <c r="AT22">
         <f>(C22/SUM($C22:$N22)-R22/SUM($R22:$AC22))*SUM('RICBP-it0_damagesbyregionoutput'!$A21:$L21)</f>
         <v>8.3721037783586407</v>
       </c>
-      <c r="AU22" s="3">
+      <c r="AU22">
         <f>(D22/SUM($C22:$N22)-S22/SUM($R22:$AC22))*SUM('RICBP-it0_damagesbyregionoutput'!$A21:$L21)</f>
         <v>6.0527078144187207</v>
       </c>
-      <c r="AV22" s="3">
+      <c r="AV22">
         <f>(E22/SUM($C22:$N22)-T22/SUM($R22:$AC22))*SUM('RICBP-it0_damagesbyregionoutput'!$A21:$L21)</f>
         <v>1.1757227753065083</v>
       </c>
-      <c r="AW22" s="3">
+      <c r="AW22">
         <f>(F22/SUM($C22:$N22)-U22/SUM($R22:$AC22))*SUM('RICBP-it0_damagesbyregionoutput'!$A21:$L21)</f>
         <v>1.3615585862210908</v>
       </c>
-      <c r="AX22" s="3">
+      <c r="AX22">
         <f>(G22/SUM($C22:$N22)-V22/SUM($R22:$AC22))*SUM('RICBP-it0_damagesbyregionoutput'!$A21:$L21)</f>
         <v>2.3332349009815996</v>
       </c>
-      <c r="AY22" s="3">
+      <c r="AY22">
         <f>(H22/SUM($C22:$N22)-W22/SUM($R22:$AC22))*SUM('RICBP-it0_damagesbyregionoutput'!$A21:$L21)</f>
         <v>-3.7266551374449457</v>
       </c>
-      <c r="AZ22" s="3">
+      <c r="AZ22">
         <f>(I22/SUM($C22:$N22)-X22/SUM($R22:$AC22))*SUM('RICBP-it0_damagesbyregionoutput'!$A21:$L21)</f>
         <v>-0.42857194117838743</v>
       </c>
-      <c r="BA22" s="3">
+      <c r="BA22">
         <f>(J22/SUM($C22:$N22)-Y22/SUM($R22:$AC22))*SUM('RICBP-it0_damagesbyregionoutput'!$A21:$L21)</f>
         <v>-1.5199735513216575</v>
       </c>
-      <c r="BB22" s="3">
+      <c r="BB22">
         <f>(K22/SUM($C22:$N22)-Z22/SUM($R22:$AC22))*SUM('RICBP-it0_damagesbyregionoutput'!$A21:$L21)</f>
         <v>-12.147703808403966</v>
       </c>
-      <c r="BC22" s="3">
+      <c r="BC22">
         <f>(L22/SUM($C22:$N22)-AA22/SUM($R22:$AC22))*SUM('RICBP-it0_damagesbyregionoutput'!$A21:$L21)</f>
         <v>-4.1562964081440334E-2</v>
       </c>
-      <c r="BD22" s="3">
+      <c r="BD22">
         <f>(M22/SUM($C22:$N22)-AB22/SUM($R22:$AC22))*SUM('RICBP-it0_damagesbyregionoutput'!$A21:$L21)</f>
         <v>0.39552614678365489</v>
       </c>
-      <c r="BE22" s="3">
+      <c r="BE22">
         <f>(N22/SUM($C22:$N22)-AC22/SUM($R22:$AC22))*SUM('RICBP-it0_damagesbyregionoutput'!$A21:$L21)</f>
         <v>-1.8263865996398216</v>
       </c>
@@ -16036,51 +16036,51 @@
         <f t="shared" si="3"/>
         <v>-15.133581208163355</v>
       </c>
-      <c r="AT23" s="3">
+      <c r="AT23">
         <f>(C23/SUM($C23:$N23)-R23/SUM($R23:$AC23))*SUM('RICBP-it0_damagesbyregionoutput'!$A22:$L22)</f>
         <v>9.2524281684472207</v>
       </c>
-      <c r="AU23" s="3">
+      <c r="AU23">
         <f>(D23/SUM($C23:$N23)-S23/SUM($R23:$AC23))*SUM('RICBP-it0_damagesbyregionoutput'!$A22:$L22)</f>
         <v>6.6892352550363441</v>
       </c>
-      <c r="AV23" s="3">
+      <c r="AV23">
         <f>(E23/SUM($C23:$N23)-T23/SUM($R23:$AC23))*SUM('RICBP-it0_damagesbyregionoutput'!$A22:$L22)</f>
         <v>1.3060155638851978</v>
       </c>
-      <c r="AW23" s="3">
+      <c r="AW23">
         <f>(F23/SUM($C23:$N23)-U23/SUM($R23:$AC23))*SUM('RICBP-it0_damagesbyregionoutput'!$A22:$L22)</f>
         <v>1.5002206359317636</v>
       </c>
-      <c r="AX23" s="3">
+      <c r="AX23">
         <f>(G23/SUM($C23:$N23)-V23/SUM($R23:$AC23))*SUM('RICBP-it0_damagesbyregionoutput'!$A22:$L22)</f>
         <v>2.5621240044853208</v>
       </c>
-      <c r="AY23" s="3">
+      <c r="AY23">
         <f>(H23/SUM($C23:$N23)-W23/SUM($R23:$AC23))*SUM('RICBP-it0_damagesbyregionoutput'!$A22:$L22)</f>
         <v>-4.2225575162760078</v>
       </c>
-      <c r="AZ23" s="3">
+      <c r="AZ23">
         <f>(I23/SUM($C23:$N23)-X23/SUM($R23:$AC23))*SUM('RICBP-it0_damagesbyregionoutput'!$A22:$L22)</f>
         <v>-0.39643522850615931</v>
       </c>
-      <c r="BA23" s="3">
+      <c r="BA23">
         <f>(J23/SUM($C23:$N23)-Y23/SUM($R23:$AC23))*SUM('RICBP-it0_damagesbyregionoutput'!$A22:$L22)</f>
         <v>-1.5783696652020343</v>
       </c>
-      <c r="BB23" s="3">
+      <c r="BB23">
         <f>(K23/SUM($C23:$N23)-Z23/SUM($R23:$AC23))*SUM('RICBP-it0_damagesbyregionoutput'!$A22:$L22)</f>
         <v>-13.568453820689735</v>
       </c>
-      <c r="BC23" s="3">
+      <c r="BC23">
         <f>(L23/SUM($C23:$N23)-AA23/SUM($R23:$AC23))*SUM('RICBP-it0_damagesbyregionoutput'!$A22:$L22)</f>
         <v>1.1844967674898696E-2</v>
       </c>
-      <c r="BD23" s="3">
+      <c r="BD23">
         <f>(M23/SUM($C23:$N23)-AB23/SUM($R23:$AC23))*SUM('RICBP-it0_damagesbyregionoutput'!$A22:$L22)</f>
         <v>0.45285619473414351</v>
       </c>
-      <c r="BE23" s="3">
+      <c r="BE23">
         <f>(N23/SUM($C23:$N23)-AC23/SUM($R23:$AC23))*SUM('RICBP-it0_damagesbyregionoutput'!$A22:$L22)</f>
         <v>-2.0089085595209593</v>
       </c>
@@ -16296,51 +16296,51 @@
         <f t="shared" si="3"/>
         <v>-17.403725393657488</v>
       </c>
-      <c r="AT24" s="3">
+      <c r="AT24">
         <f>(C24/SUM($C24:$N24)-R24/SUM($R24:$AC24))*SUM('RICBP-it0_damagesbyregionoutput'!$A23:$L23)</f>
         <v>10.186471474660092</v>
       </c>
-      <c r="AU24" s="3">
+      <c r="AU24">
         <f>(D24/SUM($C24:$N24)-S24/SUM($R24:$AC24))*SUM('RICBP-it0_damagesbyregionoutput'!$A23:$L23)</f>
         <v>7.3638656797885425</v>
       </c>
-      <c r="AV24" s="3">
+      <c r="AV24">
         <f>(E24/SUM($C24:$N24)-T24/SUM($R24:$AC24))*SUM('RICBP-it0_damagesbyregionoutput'!$A23:$L23)</f>
         <v>1.4441935624870219</v>
       </c>
-      <c r="AW24" s="3">
+      <c r="AW24">
         <f>(F24/SUM($C24:$N24)-U24/SUM($R24:$AC24))*SUM('RICBP-it0_damagesbyregionoutput'!$A23:$L23)</f>
         <v>1.6472400980096606</v>
       </c>
-      <c r="AX24" s="3">
+      <c r="AX24">
         <f>(G24/SUM($C24:$N24)-V24/SUM($R24:$AC24))*SUM('RICBP-it0_damagesbyregionoutput'!$A23:$L23)</f>
         <v>2.8046430393547932</v>
       </c>
-      <c r="AY24" s="3">
+      <c r="AY24">
         <f>(H24/SUM($C24:$N24)-W24/SUM($R24:$AC24))*SUM('RICBP-it0_damagesbyregionoutput'!$A23:$L23)</f>
         <v>-4.7609029776172926</v>
       </c>
-      <c r="AZ24" s="3">
+      <c r="AZ24">
         <f>(I24/SUM($C24:$N24)-X24/SUM($R24:$AC24))*SUM('RICBP-it0_damagesbyregionoutput'!$A23:$L23)</f>
         <v>-0.35328253107264146</v>
       </c>
-      <c r="BA24" s="3">
+      <c r="BA24">
         <f>(J24/SUM($C24:$N24)-Y24/SUM($R24:$AC24))*SUM('RICBP-it0_damagesbyregionoutput'!$A23:$L23)</f>
         <v>-1.6340180702449769</v>
       </c>
-      <c r="BB24" s="3">
+      <c r="BB24">
         <f>(K24/SUM($C24:$N24)-Z24/SUM($R24:$AC24))*SUM('RICBP-it0_damagesbyregionoutput'!$A23:$L23)</f>
         <v>-15.082233667943836</v>
       </c>
-      <c r="BC24" s="3">
+      <c r="BC24">
         <f>(L24/SUM($C24:$N24)-AA24/SUM($R24:$AC24))*SUM('RICBP-it0_damagesbyregionoutput'!$A23:$L23)</f>
         <v>7.272681680343436E-2</v>
       </c>
-      <c r="BD24" s="3">
+      <c r="BD24">
         <f>(M24/SUM($C24:$N24)-AB24/SUM($R24:$AC24))*SUM('RICBP-it0_damagesbyregionoutput'!$A23:$L23)</f>
         <v>0.51401660314509701</v>
       </c>
-      <c r="BE24" s="3">
+      <c r="BE24">
         <f>(N24/SUM($C24:$N24)-AC24/SUM($R24:$AC24))*SUM('RICBP-it0_damagesbyregionoutput'!$A23:$L23)</f>
         <v>-2.2027200273699115</v>
       </c>
@@ -16556,51 +16556,51 @@
         <f t="shared" si="3"/>
         <v>-19.892463380969154</v>
       </c>
-      <c r="AT25" s="3">
+      <c r="AT25">
         <f>(C25/SUM($C25:$N25)-R25/SUM($R25:$AC25))*SUM('RICBP-it0_damagesbyregionoutput'!$A24:$L24)</f>
         <v>11.175961348042442</v>
       </c>
-      <c r="AU25" s="3">
+      <c r="AU25">
         <f>(D25/SUM($C25:$N25)-S25/SUM($R25:$AC25))*SUM('RICBP-it0_damagesbyregionoutput'!$A24:$L24)</f>
         <v>8.0780990320820099</v>
       </c>
-      <c r="AV25" s="3">
+      <c r="AV25">
         <f>(E25/SUM($C25:$N25)-T25/SUM($R25:$AC25))*SUM('RICBP-it0_damagesbyregionoutput'!$A24:$L24)</f>
         <v>1.5905415102952274</v>
       </c>
-      <c r="AW25" s="3">
+      <c r="AW25">
         <f>(F25/SUM($C25:$N25)-U25/SUM($R25:$AC25))*SUM('RICBP-it0_damagesbyregionoutput'!$A24:$L24)</f>
         <v>1.8029142393367337</v>
       </c>
-      <c r="AX25" s="3">
+      <c r="AX25">
         <f>(G25/SUM($C25:$N25)-V25/SUM($R25:$AC25))*SUM('RICBP-it0_damagesbyregionoutput'!$A24:$L24)</f>
         <v>3.0613059310705553</v>
       </c>
-      <c r="AY25" s="3">
+      <c r="AY25">
         <f>(H25/SUM($C25:$N25)-W25/SUM($R25:$AC25))*SUM('RICBP-it0_damagesbyregionoutput'!$A24:$L24)</f>
         <v>-5.3420282622917012</v>
       </c>
-      <c r="AZ25" s="3">
+      <c r="AZ25">
         <f>(I25/SUM($C25:$N25)-X25/SUM($R25:$AC25))*SUM('RICBP-it0_damagesbyregionoutput'!$A24:$L24)</f>
         <v>-0.29894729482358889</v>
       </c>
-      <c r="BA25" s="3">
+      <c r="BA25">
         <f>(J25/SUM($C25:$N25)-Y25/SUM($R25:$AC25))*SUM('RICBP-it0_damagesbyregionoutput'!$A24:$L24)</f>
         <v>-1.6871285751509455</v>
       </c>
-      <c r="BB25" s="3">
+      <c r="BB25">
         <f>(K25/SUM($C25:$N25)-Z25/SUM($R25:$AC25))*SUM('RICBP-it0_damagesbyregionoutput'!$A24:$L24)</f>
         <v>-16.692128199412249</v>
       </c>
-      <c r="BC25" s="3">
+      <c r="BC25">
         <f>(L25/SUM($C25:$N25)-AA25/SUM($R25:$AC25))*SUM('RICBP-it0_damagesbyregionoutput'!$A24:$L24)</f>
         <v>0.14107706722876662</v>
       </c>
-      <c r="BD25" s="3">
+      <c r="BD25">
         <f>(M25/SUM($C25:$N25)-AB25/SUM($R25:$AC25))*SUM('RICBP-it0_damagesbyregionoutput'!$A24:$L24)</f>
         <v>0.57917786737075805</v>
       </c>
-      <c r="BE25" s="3">
+      <c r="BE25">
         <f>(N25/SUM($C25:$N25)-AC25/SUM($R25:$AC25))*SUM('RICBP-it0_damagesbyregionoutput'!$A24:$L24)</f>
         <v>-2.4088446637480168</v>
       </c>
@@ -16816,51 +16816,51 @@
         <f t="shared" si="3"/>
         <v>-22.617553164670309</v>
       </c>
-      <c r="AT26" s="3">
+      <c r="AT26">
         <f>(C26/SUM($C26:$N26)-R26/SUM($R26:$AC26))*SUM('RICBP-it0_damagesbyregionoutput'!$A25:$L25)</f>
         <v>12.222105217042222</v>
       </c>
-      <c r="AU26" s="3">
+      <c r="AU26">
         <f>(D26/SUM($C26:$N26)-S26/SUM($R26:$AC26))*SUM('RICBP-it0_damagesbyregionoutput'!$A25:$L25)</f>
         <v>8.8330169760327557</v>
       </c>
-      <c r="AV26" s="3">
+      <c r="AV26">
         <f>(E26/SUM($C26:$N26)-T26/SUM($R26:$AC26))*SUM('RICBP-it0_damagesbyregionoutput'!$A25:$L25)</f>
         <v>1.7452624075835781</v>
       </c>
-      <c r="AW26" s="3">
+      <c r="AW26">
         <f>(F26/SUM($C26:$N26)-U26/SUM($R26:$AC26))*SUM('RICBP-it0_damagesbyregionoutput'!$A25:$L25)</f>
         <v>1.9674520757051888</v>
       </c>
-      <c r="AX26" s="3">
+      <c r="AX26">
         <f>(G26/SUM($C26:$N26)-V26/SUM($R26:$AC26))*SUM('RICBP-it0_damagesbyregionoutput'!$A25:$L25)</f>
         <v>3.3324743283482805</v>
       </c>
-      <c r="AY26" s="3">
+      <c r="AY26">
         <f>(H26/SUM($C26:$N26)-W26/SUM($R26:$AC26))*SUM('RICBP-it0_damagesbyregionoutput'!$A25:$L25)</f>
         <v>-5.9660676832663357</v>
       </c>
-      <c r="AZ26" s="3">
+      <c r="AZ26">
         <f>(I26/SUM($C26:$N26)-X26/SUM($R26:$AC26))*SUM('RICBP-it0_damagesbyregionoutput'!$A25:$L25)</f>
         <v>-0.23329719687710054</v>
       </c>
-      <c r="BA26" s="3">
+      <c r="BA26">
         <f>(J26/SUM($C26:$N26)-Y26/SUM($R26:$AC26))*SUM('RICBP-it0_damagesbyregionoutput'!$A25:$L25)</f>
         <v>-1.7378295186499717</v>
       </c>
-      <c r="BB26" s="3">
+      <c r="BB26">
         <f>(K26/SUM($C26:$N26)-Z26/SUM($R26:$AC26))*SUM('RICBP-it0_damagesbyregionoutput'!$A25:$L25)</f>
         <v>-18.400283263957981</v>
       </c>
-      <c r="BC26" s="3">
+      <c r="BC26">
         <f>(L26/SUM($C26:$N26)-AA26/SUM($R26:$AC26))*SUM('RICBP-it0_damagesbyregionoutput'!$A25:$L25)</f>
         <v>0.2168850930800689</v>
       </c>
-      <c r="BD26" s="3">
+      <c r="BD26">
         <f>(M26/SUM($C26:$N26)-AB26/SUM($R26:$AC26))*SUM('RICBP-it0_damagesbyregionoutput'!$A25:$L25)</f>
         <v>0.64847178700819419</v>
       </c>
-      <c r="BE26" s="3">
+      <c r="BE26">
         <f>(N26/SUM($C26:$N26)-AC26/SUM($R26:$AC26))*SUM('RICBP-it0_damagesbyregionoutput'!$A25:$L25)</f>
         <v>-2.6281902220489095</v>
       </c>
@@ -17076,51 +17076,51 @@
         <f t="shared" si="3"/>
         <v>-25.597661689346605</v>
       </c>
-      <c r="AT27" s="3">
+      <c r="AT27">
         <f>(C27/SUM($C27:$N27)-R27/SUM($R27:$AC27))*SUM('RICBP-it0_damagesbyregionoutput'!$A26:$L26)</f>
         <v>13.325770964811735</v>
       </c>
-      <c r="AU27" s="3">
+      <c r="AU27">
         <f>(D27/SUM($C27:$N27)-S27/SUM($R27:$AC27))*SUM('RICBP-it0_damagesbyregionoutput'!$A26:$L26)</f>
         <v>9.6294163460787683</v>
       </c>
-      <c r="AV27" s="3">
+      <c r="AV27">
         <f>(E27/SUM($C27:$N27)-T27/SUM($R27:$AC27))*SUM('RICBP-it0_damagesbyregionoutput'!$A26:$L26)</f>
         <v>1.908504614329865</v>
       </c>
-      <c r="AW27" s="3">
+      <c r="AW27">
         <f>(F27/SUM($C27:$N27)-U27/SUM($R27:$AC27))*SUM('RICBP-it0_damagesbyregionoutput'!$A26:$L26)</f>
         <v>2.1410052054265476</v>
       </c>
-      <c r="AX27" s="3">
+      <c r="AX27">
         <f>(G27/SUM($C27:$N27)-V27/SUM($R27:$AC27))*SUM('RICBP-it0_damagesbyregionoutput'!$A26:$L26)</f>
         <v>3.6184113553306023</v>
       </c>
-      <c r="AY27" s="3">
+      <c r="AY27">
         <f>(H27/SUM($C27:$N27)-W27/SUM($R27:$AC27))*SUM('RICBP-it0_damagesbyregionoutput'!$A26:$L26)</f>
         <v>-6.6330373619892402</v>
       </c>
-      <c r="AZ27" s="3">
+      <c r="AZ27">
         <f>(I27/SUM($C27:$N27)-X27/SUM($R27:$AC27))*SUM('RICBP-it0_damagesbyregionoutput'!$A26:$L26)</f>
         <v>-0.15623120928727288</v>
       </c>
-      <c r="BA27" s="3">
+      <c r="BA27">
         <f>(J27/SUM($C27:$N27)-Y27/SUM($R27:$AC27))*SUM('RICBP-it0_damagesbyregionoutput'!$A26:$L26)</f>
         <v>-1.7862071531262549</v>
       </c>
-      <c r="BB27" s="3">
+      <c r="BB27">
         <f>(K27/SUM($C27:$N27)-Z27/SUM($R27:$AC27))*SUM('RICBP-it0_damagesbyregionoutput'!$A26:$L26)</f>
         <v>-20.208188882915998</v>
       </c>
-      <c r="BC27" s="3">
+      <c r="BC27">
         <f>(L27/SUM($C27:$N27)-AA27/SUM($R27:$AC27))*SUM('RICBP-it0_damagesbyregionoutput'!$A26:$L26)</f>
         <v>0.30013462473612107</v>
       </c>
-      <c r="BD27" s="3">
+      <c r="BD27">
         <f>(M27/SUM($C27:$N27)-AB27/SUM($R27:$AC27))*SUM('RICBP-it0_damagesbyregionoutput'!$A26:$L26)</f>
         <v>0.72199854785331519</v>
       </c>
-      <c r="BE27" s="3">
+      <c r="BE27">
         <f>(N27/SUM($C27:$N27)-AC27/SUM($R27:$AC27))*SUM('RICBP-it0_damagesbyregionoutput'!$A26:$L26)</f>
         <v>-2.8615770512481888</v>
       </c>
@@ -17336,51 +17336,51 @@
         <f t="shared" si="3"/>
         <v>-28.852205499813898</v>
       </c>
-      <c r="AT28" s="3">
+      <c r="AT28">
         <f>(C28/SUM($C28:$N28)-R28/SUM($R28:$AC28))*SUM('RICBP-it0_damagesbyregionoutput'!$A27:$L27)</f>
         <v>14.487635916094478</v>
       </c>
-      <c r="AU28" s="3">
+      <c r="AU28">
         <f>(D28/SUM($C28:$N28)-S28/SUM($R28:$AC28))*SUM('RICBP-it0_damagesbyregionoutput'!$A27:$L27)</f>
         <v>10.467920360724246</v>
       </c>
-      <c r="AV28" s="3">
+      <c r="AV28">
         <f>(E28/SUM($C28:$N28)-T28/SUM($R28:$AC28))*SUM('RICBP-it0_damagesbyregionoutput'!$A27:$L27)</f>
         <v>2.0803844723617084</v>
       </c>
-      <c r="AW28" s="3">
+      <c r="AW28">
         <f>(F28/SUM($C28:$N28)-U28/SUM($R28:$AC28))*SUM('RICBP-it0_damagesbyregionoutput'!$A27:$L27)</f>
         <v>2.3236927680297623</v>
       </c>
-      <c r="AX28" s="3">
+      <c r="AX28">
         <f>(G28/SUM($C28:$N28)-V28/SUM($R28:$AC28))*SUM('RICBP-it0_damagesbyregionoutput'!$A27:$L27)</f>
         <v>3.9193244893997052</v>
       </c>
-      <c r="AY28" s="3">
+      <c r="AY28">
         <f>(H28/SUM($C28:$N28)-W28/SUM($R28:$AC28))*SUM('RICBP-it0_damagesbyregionoutput'!$A27:$L27)</f>
         <v>-7.3429093379031354</v>
       </c>
-      <c r="AZ28" s="3">
+      <c r="AZ28">
         <f>(I28/SUM($C28:$N28)-X28/SUM($R28:$AC28))*SUM('RICBP-it0_damagesbyregionoutput'!$A27:$L27)</f>
         <v>-6.7672663244915138E-2</v>
       </c>
-      <c r="BA28" s="3">
+      <c r="BA28">
         <f>(J28/SUM($C28:$N28)-Y28/SUM($R28:$AC28))*SUM('RICBP-it0_damagesbyregionoutput'!$A27:$L27)</f>
         <v>-1.8323300635700319</v>
       </c>
-      <c r="BB28" s="3">
+      <c r="BB28">
         <f>(K28/SUM($C28:$N28)-Z28/SUM($R28:$AC28))*SUM('RICBP-it0_damagesbyregionoutput'!$A27:$L27)</f>
         <v>-22.11692399728749</v>
       </c>
-      <c r="BC28" s="3">
+      <c r="BC28">
         <f>(L28/SUM($C28:$N28)-AA28/SUM($R28:$AC28))*SUM('RICBP-it0_damagesbyregionoutput'!$A27:$L27)</f>
         <v>0.39080673634669849</v>
       </c>
-      <c r="BD28" s="3">
+      <c r="BD28">
         <f>(M28/SUM($C28:$N28)-AB28/SUM($R28:$AC28))*SUM('RICBP-it0_damagesbyregionoutput'!$A27:$L27)</f>
         <v>0.79983444046747343</v>
       </c>
-      <c r="BE28" s="3">
+      <c r="BE28">
         <f>(N28/SUM($C28:$N28)-AC28/SUM($R28:$AC28))*SUM('RICBP-it0_damagesbyregionoutput'!$A27:$L27)</f>
         <v>-3.1097631214185153</v>
       </c>
@@ -17596,51 +17596,51 @@
         <f t="shared" si="3"/>
         <v>-32.403949920672943</v>
       </c>
-      <c r="AT29" s="3">
+      <c r="AT29">
         <f>(C29/SUM($C29:$N29)-R29/SUM($R29:$AC29))*SUM('RICBP-it0_damagesbyregionoutput'!$A28:$L28)</f>
         <v>15.713857055113662</v>
       </c>
-      <c r="AU29" s="3">
+      <c r="AU29">
         <f>(D29/SUM($C29:$N29)-S29/SUM($R29:$AC29))*SUM('RICBP-it0_damagesbyregionoutput'!$A28:$L28)</f>
         <v>11.353057527115299</v>
       </c>
-      <c r="AV29" s="3">
+      <c r="AV29">
         <f>(E29/SUM($C29:$N29)-T29/SUM($R29:$AC29))*SUM('RICBP-it0_damagesbyregionoutput'!$A28:$L28)</f>
         <v>2.2618022587746998</v>
       </c>
-      <c r="AW29" s="3">
+      <c r="AW29">
         <f>(F29/SUM($C29:$N29)-U29/SUM($R29:$AC29))*SUM('RICBP-it0_damagesbyregionoutput'!$A28:$L28)</f>
         <v>2.5165072525504169</v>
       </c>
-      <c r="AX29" s="3">
+      <c r="AX29">
         <f>(G29/SUM($C29:$N29)-V29/SUM($R29:$AC29))*SUM('RICBP-it0_damagesbyregionoutput'!$A28:$L28)</f>
         <v>4.2368925765311936</v>
       </c>
-      <c r="AY29" s="3">
+      <c r="AY29">
         <f>(H29/SUM($C29:$N29)-W29/SUM($R29:$AC29))*SUM('RICBP-it0_damagesbyregionoutput'!$A28:$L28)</f>
         <v>-8.0985351882112653</v>
       </c>
-      <c r="AZ29" s="3">
+      <c r="AZ29">
         <f>(I29/SUM($C29:$N29)-X29/SUM($R29:$AC29))*SUM('RICBP-it0_damagesbyregionoutput'!$A28:$L28)</f>
         <v>3.244402099466237E-2</v>
       </c>
-      <c r="BA29" s="3">
+      <c r="BA29">
         <f>(J29/SUM($C29:$N29)-Y29/SUM($R29:$AC29))*SUM('RICBP-it0_damagesbyregionoutput'!$A28:$L28)</f>
         <v>-1.8769511258103906</v>
       </c>
-      <c r="BB29" s="3">
+      <c r="BB29">
         <f>(K29/SUM($C29:$N29)-Z29/SUM($R29:$AC29))*SUM('RICBP-it0_damagesbyregionoutput'!$A28:$L28)</f>
         <v>-24.13567592846406</v>
       </c>
-      <c r="BC29" s="3">
+      <c r="BC29">
         <f>(L29/SUM($C29:$N29)-AA29/SUM($R29:$AC29))*SUM('RICBP-it0_damagesbyregionoutput'!$A28:$L28)</f>
         <v>0.48906466949756333</v>
       </c>
-      <c r="BD29" s="3">
+      <c r="BD29">
         <f>(M29/SUM($C29:$N29)-AB29/SUM($R29:$AC29))*SUM('RICBP-it0_damagesbyregionoutput'!$A28:$L28)</f>
         <v>0.88234617827187867</v>
       </c>
-      <c r="BE29" s="3">
+      <c r="BE29">
         <f>(N29/SUM($C29:$N29)-AC29/SUM($R29:$AC29))*SUM('RICBP-it0_damagesbyregionoutput'!$A28:$L28)</f>
         <v>-3.3748092963636731</v>
       </c>
@@ -17856,51 +17856,51 @@
         <f t="shared" si="3"/>
         <v>-36.273474157812302</v>
       </c>
-      <c r="AT30" s="3">
+      <c r="AT30">
         <f>(C30/SUM($C30:$N30)-R30/SUM($R30:$AC30))*SUM('RICBP-it0_damagesbyregionoutput'!$A29:$L29)</f>
         <v>16.999576488130188</v>
       </c>
-      <c r="AU30" s="3">
+      <c r="AU30">
         <f>(D30/SUM($C30:$N30)-S30/SUM($R30:$AC30))*SUM('RICBP-it0_damagesbyregionoutput'!$A29:$L29)</f>
         <v>12.281383377457583</v>
       </c>
-      <c r="AV30" s="3">
+      <c r="AV30">
         <f>(E30/SUM($C30:$N30)-T30/SUM($R30:$AC30))*SUM('RICBP-it0_damagesbyregionoutput'!$A29:$L29)</f>
         <v>2.452075457710817</v>
       </c>
-      <c r="AW30" s="3">
+      <c r="AW30">
         <f>(F30/SUM($C30:$N30)-U30/SUM($R30:$AC30))*SUM('RICBP-it0_damagesbyregionoutput'!$A29:$L29)</f>
         <v>2.7186773705672764</v>
       </c>
-      <c r="AX30" s="3">
+      <c r="AX30">
         <f>(G30/SUM($C30:$N30)-V30/SUM($R30:$AC30))*SUM('RICBP-it0_damagesbyregionoutput'!$A29:$L29)</f>
         <v>4.5698169101132073</v>
       </c>
-      <c r="AY30" s="3">
+      <c r="AY30">
         <f>(H30/SUM($C30:$N30)-W30/SUM($R30:$AC30))*SUM('RICBP-it0_damagesbyregionoutput'!$A29:$L29)</f>
         <v>-8.8972696498146462</v>
       </c>
-      <c r="AZ30" s="3">
+      <c r="AZ30">
         <f>(I30/SUM($C30:$N30)-X30/SUM($R30:$AC30))*SUM('RICBP-it0_damagesbyregionoutput'!$A29:$L29)</f>
         <v>0.14426227022617788</v>
       </c>
-      <c r="BA30" s="3">
+      <c r="BA30">
         <f>(J30/SUM($C30:$N30)-Y30/SUM($R30:$AC30))*SUM('RICBP-it0_damagesbyregionoutput'!$A29:$L29)</f>
         <v>-1.9194005612235814</v>
       </c>
-      <c r="BB30" s="3">
+      <c r="BB30">
         <f>(K30/SUM($C30:$N30)-Z30/SUM($R30:$AC30))*SUM('RICBP-it0_damagesbyregionoutput'!$A29:$L29)</f>
         <v>-26.25696819265325</v>
       </c>
-      <c r="BC30" s="3">
+      <c r="BC30">
         <f>(L30/SUM($C30:$N30)-AA30/SUM($R30:$AC30))*SUM('RICBP-it0_damagesbyregionoutput'!$A29:$L29)</f>
         <v>0.59477748560840848</v>
       </c>
-      <c r="BD30" s="3">
+      <c r="BD30">
         <f>(M30/SUM($C30:$N30)-AB30/SUM($R30:$AC30))*SUM('RICBP-it0_damagesbyregionoutput'!$A29:$L29)</f>
         <v>0.9692813447835904</v>
       </c>
-      <c r="BE30" s="3">
+      <c r="BE30">
         <f>(N30/SUM($C30:$N30)-AC30/SUM($R30:$AC30))*SUM('RICBP-it0_damagesbyregionoutput'!$A29:$L29)</f>
         <v>-3.6562123009057879</v>
       </c>
@@ -18116,51 +18116,51 @@
         <f t="shared" si="3"/>
         <v>-40.48115460778061</v>
       </c>
-      <c r="AT31" s="3">
+      <c r="AT31">
         <f>(C31/SUM($C31:$N31)-R31/SUM($R31:$AC31))*SUM('RICBP-it0_damagesbyregionoutput'!$A30:$L30)</f>
         <v>18.343672902008315</v>
       </c>
-      <c r="AU31" s="3">
+      <c r="AU31">
         <f>(D31/SUM($C31:$N31)-S31/SUM($R31:$AC31))*SUM('RICBP-it0_damagesbyregionoutput'!$A30:$L30)</f>
         <v>13.252147190929186</v>
       </c>
-      <c r="AV31" s="3">
+      <c r="AV31">
         <f>(E31/SUM($C31:$N31)-T31/SUM($R31:$AC31))*SUM('RICBP-it0_damagesbyregionoutput'!$A30:$L30)</f>
         <v>2.6510526856395611</v>
       </c>
-      <c r="AW31" s="3">
+      <c r="AW31">
         <f>(F31/SUM($C31:$N31)-U31/SUM($R31:$AC31))*SUM('RICBP-it0_damagesbyregionoutput'!$A30:$L30)</f>
         <v>2.9300332736888959</v>
       </c>
-      <c r="AX31" s="3">
+      <c r="AX31">
         <f>(G31/SUM($C31:$N31)-V31/SUM($R31:$AC31))*SUM('RICBP-it0_damagesbyregionoutput'!$A30:$L30)</f>
         <v>4.9178179415230137</v>
       </c>
-      <c r="AY31" s="3">
+      <c r="AY31">
         <f>(H31/SUM($C31:$N31)-W31/SUM($R31:$AC31))*SUM('RICBP-it0_damagesbyregionoutput'!$A30:$L30)</f>
         <v>-9.7382812233443783</v>
       </c>
-      <c r="AZ31" s="3">
+      <c r="AZ31">
         <f>(I31/SUM($C31:$N31)-X31/SUM($R31:$AC31))*SUM('RICBP-it0_damagesbyregionoutput'!$A30:$L30)</f>
         <v>0.26780622328401332</v>
       </c>
-      <c r="BA31" s="3">
+      <c r="BA31">
         <f>(J31/SUM($C31:$N31)-Y31/SUM($R31:$AC31))*SUM('RICBP-it0_damagesbyregionoutput'!$A30:$L30)</f>
         <v>-1.9595585394806752</v>
       </c>
-      <c r="BB31" s="3">
+      <c r="BB31">
         <f>(K31/SUM($C31:$N31)-Z31/SUM($R31:$AC31))*SUM('RICBP-it0_damagesbyregionoutput'!$A30:$L30)</f>
         <v>-28.47892700092661</v>
       </c>
-      <c r="BC31" s="3">
+      <c r="BC31">
         <f>(L31/SUM($C31:$N31)-AA31/SUM($R31:$AC31))*SUM('RICBP-it0_damagesbyregionoutput'!$A30:$L30)</f>
         <v>0.70786759569132118</v>
       </c>
-      <c r="BD31" s="3">
+      <c r="BD31">
         <f>(M31/SUM($C31:$N31)-AB31/SUM($R31:$AC31))*SUM('RICBP-it0_damagesbyregionoutput'!$A30:$L30)</f>
         <v>1.0605814063250381</v>
       </c>
-      <c r="BE31" s="3">
+      <c r="BE31">
         <f>(N31/SUM($C31:$N31)-AC31/SUM($R31:$AC31))*SUM('RICBP-it0_damagesbyregionoutput'!$A30:$L30)</f>
         <v>-3.9542124553377045</v>
       </c>
@@ -18376,51 +18376,51 @@
         <f t="shared" si="3"/>
         <v>-45.048034928266482</v>
       </c>
-      <c r="AT32" s="3">
+      <c r="AT32">
         <f>(C32/SUM($C32:$N32)-R32/SUM($R32:$AC32))*SUM('RICBP-it0_damagesbyregionoutput'!$A31:$L31)</f>
         <v>19.747255343712549</v>
       </c>
-      <c r="AU32" s="3">
+      <c r="AU32">
         <f>(D32/SUM($C32:$N32)-S32/SUM($R32:$AC32))*SUM('RICBP-it0_damagesbyregionoutput'!$A31:$L31)</f>
         <v>14.266187282908003</v>
       </c>
-      <c r="AV32" s="3">
+      <c r="AV32">
         <f>(E32/SUM($C32:$N32)-T32/SUM($R32:$AC32))*SUM('RICBP-it0_damagesbyregionoutput'!$A31:$L31)</f>
         <v>2.8589025719625916</v>
       </c>
-      <c r="AW32" s="3">
+      <c r="AW32">
         <f>(F32/SUM($C32:$N32)-U32/SUM($R32:$AC32))*SUM('RICBP-it0_damagesbyregionoutput'!$A31:$L31)</f>
         <v>3.150760909462146</v>
       </c>
-      <c r="AX32" s="3">
+      <c r="AX32">
         <f>(G32/SUM($C32:$N32)-V32/SUM($R32:$AC32))*SUM('RICBP-it0_damagesbyregionoutput'!$A31:$L31)</f>
         <v>5.281214031454013</v>
       </c>
-      <c r="AY32" s="3">
+      <c r="AY32">
         <f>(H32/SUM($C32:$N32)-W32/SUM($R32:$AC32))*SUM('RICBP-it0_damagesbyregionoutput'!$A31:$L31)</f>
         <v>-10.621951449509538</v>
       </c>
-      <c r="AZ32" s="3">
+      <c r="AZ32">
         <f>(I32/SUM($C32:$N32)-X32/SUM($R32:$AC32))*SUM('RICBP-it0_damagesbyregionoutput'!$A31:$L31)</f>
         <v>0.40311354957501649</v>
       </c>
-      <c r="BA32" s="3">
+      <c r="BA32">
         <f>(J32/SUM($C32:$N32)-Y32/SUM($R32:$AC32))*SUM('RICBP-it0_damagesbyregionoutput'!$A31:$L31)</f>
         <v>-1.9975630914083773</v>
       </c>
-      <c r="BB32" s="3">
+      <c r="BB32">
         <f>(K32/SUM($C32:$N32)-Z32/SUM($R32:$AC32))*SUM('RICBP-it0_damagesbyregionoutput'!$A31:$L31)</f>
         <v>-30.803053166104441</v>
       </c>
-      <c r="BC32" s="3">
+      <c r="BC32">
         <f>(L32/SUM($C32:$N32)-AA32/SUM($R32:$AC32))*SUM('RICBP-it0_damagesbyregionoutput'!$A31:$L31)</f>
         <v>0.82834064938511731</v>
       </c>
-      <c r="BD32" s="3">
+      <c r="BD32">
         <f>(M32/SUM($C32:$N32)-AB32/SUM($R32:$AC32))*SUM('RICBP-it0_damagesbyregionoutput'!$A31:$L31)</f>
         <v>1.156306256534255</v>
       </c>
-      <c r="BE32" s="3">
+      <c r="BE32">
         <f>(N32/SUM($C32:$N32)-AC32/SUM($R32:$AC32))*SUM('RICBP-it0_damagesbyregionoutput'!$A31:$L31)</f>
         <v>-4.2695128879713637</v>
       </c>
@@ -18636,51 +18636,51 @@
         <f t="shared" si="3"/>
         <v>-49.995959832911026</v>
       </c>
-      <c r="AT33" s="3">
+      <c r="AT33">
         <f>(C33/SUM($C33:$N33)-R33/SUM($R33:$AC33))*SUM('RICBP-it0_damagesbyregionoutput'!$A32:$L32)</f>
         <v>21.211891618718926</v>
       </c>
-      <c r="AU33" s="3">
+      <c r="AU33">
         <f>(D33/SUM($C33:$N33)-S33/SUM($R33:$AC33))*SUM('RICBP-it0_damagesbyregionoutput'!$A32:$L32)</f>
         <v>15.324651682625355</v>
       </c>
-      <c r="AV33" s="3">
+      <c r="AV33">
         <f>(E33/SUM($C33:$N33)-T33/SUM($R33:$AC33))*SUM('RICBP-it0_damagesbyregionoutput'!$A32:$L32)</f>
         <v>3.0758602010665301</v>
       </c>
-      <c r="AW33" s="3">
+      <c r="AW33">
         <f>(F33/SUM($C33:$N33)-U33/SUM($R33:$AC33))*SUM('RICBP-it0_damagesbyregionoutput'!$A32:$L32)</f>
         <v>3.3811177650923776</v>
       </c>
-      <c r="AX33" s="3">
+      <c r="AX33">
         <f>(G33/SUM($C33:$N33)-V33/SUM($R33:$AC33))*SUM('RICBP-it0_damagesbyregionoutput'!$A32:$L32)</f>
         <v>5.6604413684669721</v>
       </c>
-      <c r="AY33" s="3">
+      <c r="AY33">
         <f>(H33/SUM($C33:$N33)-W33/SUM($R33:$AC33))*SUM('RICBP-it0_damagesbyregionoutput'!$A32:$L32)</f>
         <v>-11.548995095970342</v>
       </c>
-      <c r="AZ33" s="3">
+      <c r="AZ33">
         <f>(I33/SUM($C33:$N33)-X33/SUM($R33:$AC33))*SUM('RICBP-it0_damagesbyregionoutput'!$A32:$L32)</f>
         <v>0.5502650991085194</v>
       </c>
-      <c r="BA33" s="3">
+      <c r="BA33">
         <f>(J33/SUM($C33:$N33)-Y33/SUM($R33:$AC33))*SUM('RICBP-it0_damagesbyregionoutput'!$A32:$L32)</f>
         <v>-2.0335721204423334</v>
       </c>
-      <c r="BB33" s="3">
+      <c r="BB33">
         <f>(K33/SUM($C33:$N33)-Z33/SUM($R33:$AC33))*SUM('RICBP-it0_damagesbyregionoutput'!$A32:$L32)</f>
         <v>-33.231538595402426</v>
       </c>
-      <c r="BC33" s="3">
+      <c r="BC33">
         <f>(L33/SUM($C33:$N33)-AA33/SUM($R33:$AC33))*SUM('RICBP-it0_damagesbyregionoutput'!$A32:$L32)</f>
         <v>0.95624638137148921</v>
       </c>
-      <c r="BD33" s="3">
+      <c r="BD33">
         <f>(M33/SUM($C33:$N33)-AB33/SUM($R33:$AC33))*SUM('RICBP-it0_damagesbyregionoutput'!$A32:$L32)</f>
         <v>1.2565380640546211</v>
       </c>
-      <c r="BE33" s="3">
+      <c r="BE33">
         <f>(N33/SUM($C33:$N33)-AC33/SUM($R33:$AC33))*SUM('RICBP-it0_damagesbyregionoutput'!$A32:$L32)</f>
         <v>-4.602906368689708</v>
       </c>
@@ -18896,51 +18896,51 @@
         <f t="shared" si="3"/>
         <v>-55.347555602966828</v>
       </c>
-      <c r="AT34" s="3">
+      <c r="AT34">
         <f>(C34/SUM($C34:$N34)-R34/SUM($R34:$AC34))*SUM('RICBP-it0_damagesbyregionoutput'!$A33:$L33)</f>
         <v>22.739228192693709</v>
       </c>
-      <c r="AU34" s="3">
+      <c r="AU34">
         <f>(D34/SUM($C34:$N34)-S34/SUM($R34:$AC34))*SUM('RICBP-it0_damagesbyregionoutput'!$A33:$L33)</f>
         <v>16.428727474039089</v>
       </c>
-      <c r="AV34" s="3">
+      <c r="AV34">
         <f>(E34/SUM($C34:$N34)-T34/SUM($R34:$AC34))*SUM('RICBP-it0_damagesbyregionoutput'!$A33:$L33)</f>
         <v>3.3021725207404522</v>
       </c>
-      <c r="AW34" s="3">
+      <c r="AW34">
         <f>(F34/SUM($C34:$N34)-U34/SUM($R34:$AC34))*SUM('RICBP-it0_damagesbyregionoutput'!$A33:$L33)</f>
         <v>3.6213724151908493</v>
       </c>
-      <c r="AX34" s="3">
+      <c r="AX34">
         <f>(G34/SUM($C34:$N34)-V34/SUM($R34:$AC34))*SUM('RICBP-it0_damagesbyregionoutput'!$A33:$L33)</f>
         <v>6.0559525055740702</v>
       </c>
-      <c r="AY34" s="3">
+      <c r="AY34">
         <f>(H34/SUM($C34:$N34)-W34/SUM($R34:$AC34))*SUM('RICBP-it0_damagesbyregionoutput'!$A33:$L33)</f>
         <v>-12.520255283166556</v>
       </c>
-      <c r="AZ34" s="3">
+      <c r="AZ34">
         <f>(I34/SUM($C34:$N34)-X34/SUM($R34:$AC34))*SUM('RICBP-it0_damagesbyregionoutput'!$A33:$L33)</f>
         <v>0.70938470314395097</v>
       </c>
-      <c r="BA34" s="3">
+      <c r="BA34">
         <f>(J34/SUM($C34:$N34)-Y34/SUM($R34:$AC34))*SUM('RICBP-it0_damagesbyregionoutput'!$A33:$L33)</f>
         <v>-2.0677190635196396</v>
       </c>
-      <c r="BB34" s="3">
+      <c r="BB34">
         <f>(K34/SUM($C34:$N34)-Z34/SUM($R34:$AC34))*SUM('RICBP-it0_damagesbyregionoutput'!$A33:$L33)</f>
         <v>-35.766695463249249</v>
       </c>
-      <c r="BC34" s="3">
+      <c r="BC34">
         <f>(L34/SUM($C34:$N34)-AA34/SUM($R34:$AC34))*SUM('RICBP-it0_damagesbyregionoutput'!$A33:$L33)</f>
         <v>1.0916645843905466</v>
       </c>
-      <c r="BD34" s="3">
+      <c r="BD34">
         <f>(M34/SUM($C34:$N34)-AB34/SUM($R34:$AC34))*SUM('RICBP-it0_damagesbyregionoutput'!$A33:$L33)</f>
         <v>1.3613609096525501</v>
       </c>
-      <c r="BE34" s="3">
+      <c r="BE34">
         <f>(N34/SUM($C34:$N34)-AC34/SUM($R34:$AC34))*SUM('RICBP-it0_damagesbyregionoutput'!$A33:$L33)</f>
         <v>-4.9551934954897714</v>
       </c>
@@ -19156,51 +19156,51 @@
         <f t="shared" si="3"/>
         <v>-61.126210376766203</v>
       </c>
-      <c r="AT35" s="3">
+      <c r="AT35">
         <f>(C35/SUM($C35:$N35)-R35/SUM($R35:$AC35))*SUM('RICBP-it0_damagesbyregionoutput'!$A34:$L34)</f>
         <v>24.330978800589264</v>
       </c>
-      <c r="AU35" s="3">
+      <c r="AU35">
         <f>(D35/SUM($C35:$N35)-S35/SUM($R35:$AC35))*SUM('RICBP-it0_damagesbyregionoutput'!$A34:$L34)</f>
         <v>17.579636410983568</v>
       </c>
-      <c r="AV35" s="3">
+      <c r="AV35">
         <f>(E35/SUM($C35:$N35)-T35/SUM($R35:$AC35))*SUM('RICBP-it0_damagesbyregionoutput'!$A34:$L34)</f>
         <v>3.5380967624971369</v>
       </c>
-      <c r="AW35" s="3">
+      <c r="AW35">
         <f>(F35/SUM($C35:$N35)-U35/SUM($R35:$AC35))*SUM('RICBP-it0_damagesbyregionoutput'!$A34:$L34)</f>
         <v>3.8718030321289549</v>
       </c>
-      <c r="AX35" s="3">
+      <c r="AX35">
         <f>(G35/SUM($C35:$N35)-V35/SUM($R35:$AC35))*SUM('RICBP-it0_damagesbyregionoutput'!$A34:$L34)</f>
         <v>6.4682141522303427</v>
       </c>
-      <c r="AY35" s="3">
+      <c r="AY35">
         <f>(H35/SUM($C35:$N35)-W35/SUM($R35:$AC35))*SUM('RICBP-it0_damagesbyregionoutput'!$A34:$L34)</f>
         <v>-13.536687428702113</v>
       </c>
-      <c r="AZ35" s="3">
+      <c r="AZ35">
         <f>(I35/SUM($C35:$N35)-X35/SUM($R35:$AC35))*SUM('RICBP-it0_damagesbyregionoutput'!$A34:$L34)</f>
         <v>0.88063746144828681</v>
       </c>
-      <c r="BA35" s="3">
+      <c r="BA35">
         <f>(J35/SUM($C35:$N35)-Y35/SUM($R35:$AC35))*SUM('RICBP-it0_damagesbyregionoutput'!$A34:$L34)</f>
         <v>-2.1001133230102549</v>
       </c>
-      <c r="BB35" s="3">
+      <c r="BB35">
         <f>(K35/SUM($C35:$N35)-Z35/SUM($R35:$AC35))*SUM('RICBP-it0_damagesbyregionoutput'!$A34:$L34)</f>
         <v>-38.410948931628504</v>
       </c>
-      <c r="BC35" s="3">
+      <c r="BC35">
         <f>(L35/SUM($C35:$N35)-AA35/SUM($R35:$AC35))*SUM('RICBP-it0_damagesbyregionoutput'!$A34:$L34)</f>
         <v>1.2347021183165172</v>
       </c>
-      <c r="BD35" s="3">
+      <c r="BD35">
         <f>(M35/SUM($C35:$N35)-AB35/SUM($R35:$AC35))*SUM('RICBP-it0_damagesbyregionoutput'!$A34:$L34)</f>
         <v>1.4708611277904506</v>
       </c>
-      <c r="BE35" s="3">
+      <c r="BE35">
         <f>(N35/SUM($C35:$N35)-AC35/SUM($R35:$AC35))*SUM('RICBP-it0_damagesbyregionoutput'!$A34:$L34)</f>
         <v>-5.3271801826436542</v>
       </c>
@@ -19416,51 +19416,51 @@
         <f t="shared" si="3"/>
         <v>-67.35608278538956</v>
       </c>
-      <c r="AT36" s="3">
+      <c r="AT36">
         <f>(C36/SUM($C36:$N36)-R36/SUM($R36:$AC36))*SUM('RICBP-it0_damagesbyregionoutput'!$A35:$L35)</f>
         <v>25.988979081340812</v>
       </c>
-      <c r="AU36" s="3">
+      <c r="AU36">
         <f>(D36/SUM($C36:$N36)-S36/SUM($R36:$AC36))*SUM('RICBP-it0_damagesbyregionoutput'!$A35:$L35)</f>
         <v>18.778677534774381</v>
       </c>
-      <c r="AV36" s="3">
+      <c r="AV36">
         <f>(E36/SUM($C36:$N36)-T36/SUM($R36:$AC36))*SUM('RICBP-it0_damagesbyregionoutput'!$A35:$L35)</f>
         <v>3.7839084323112799</v>
       </c>
-      <c r="AW36" s="3">
+      <c r="AW36">
         <f>(F36/SUM($C36:$N36)-U36/SUM($R36:$AC36))*SUM('RICBP-it0_damagesbyregionoutput'!$A35:$L35)</f>
         <v>4.1327063145091429</v>
       </c>
-      <c r="AX36" s="3">
+      <c r="AX36">
         <f>(G36/SUM($C36:$N36)-V36/SUM($R36:$AC36))*SUM('RICBP-it0_damagesbyregionoutput'!$A35:$L35)</f>
         <v>6.8977223296090653</v>
       </c>
-      <c r="AY36" s="3">
+      <c r="AY36">
         <f>(H36/SUM($C36:$N36)-W36/SUM($R36:$AC36))*SUM('RICBP-it0_damagesbyregionoutput'!$A35:$L35)</f>
         <v>-14.599380920100391</v>
       </c>
-      <c r="AZ36" s="3">
+      <c r="AZ36">
         <f>(I36/SUM($C36:$N36)-X36/SUM($R36:$AC36))*SUM('RICBP-it0_damagesbyregionoutput'!$A35:$L35)</f>
         <v>1.0642299625400282</v>
       </c>
-      <c r="BA36" s="3">
+      <c r="BA36">
         <f>(J36/SUM($C36:$N36)-Y36/SUM($R36:$AC36))*SUM('RICBP-it0_damagesbyregionoutput'!$A35:$L35)</f>
         <v>-2.1308465213010517</v>
       </c>
-      <c r="BB36" s="3">
+      <c r="BB36">
         <f>(K36/SUM($C36:$N36)-Z36/SUM($R36:$AC36))*SUM('RICBP-it0_damagesbyregionoutput'!$A35:$L35)</f>
         <v>-41.166930340494829</v>
       </c>
-      <c r="BC36" s="3">
+      <c r="BC36">
         <f>(L36/SUM($C36:$N36)-AA36/SUM($R36:$AC36))*SUM('RICBP-it0_damagesbyregionoutput'!$A35:$L35)</f>
         <v>1.3854935251687543</v>
       </c>
-      <c r="BD36" s="3">
+      <c r="BD36">
         <f>(M36/SUM($C36:$N36)-AB36/SUM($R36:$AC36))*SUM('RICBP-it0_damagesbyregionoutput'!$A35:$L35)</f>
         <v>1.5851314568442751</v>
       </c>
-      <c r="BE36" s="3">
+      <c r="BE36">
         <f>(N36/SUM($C36:$N36)-AC36/SUM($R36:$AC36))*SUM('RICBP-it0_damagesbyregionoutput'!$A35:$L35)</f>
         <v>-5.7196908552014936</v>
       </c>
@@ -19676,51 +19676,51 @@
         <f t="shared" si="3"/>
         <v>-74.062136071355795</v>
       </c>
-      <c r="AT37" s="3">
+      <c r="AT37">
         <f>(C37/SUM($C37:$N37)-R37/SUM($R37:$AC37))*SUM('RICBP-it0_damagesbyregionoutput'!$A36:$L36)</f>
         <v>27.715233896692514</v>
       </c>
-      <c r="AU37" s="3">
+      <c r="AU37">
         <f>(D37/SUM($C37:$N37)-S37/SUM($R37:$AC37))*SUM('RICBP-it0_damagesbyregionoutput'!$A36:$L36)</f>
         <v>20.02726385292161</v>
       </c>
-      <c r="AV37" s="3">
+      <c r="AV37">
         <f>(E37/SUM($C37:$N37)-T37/SUM($R37:$AC37))*SUM('RICBP-it0_damagesbyregionoutput'!$A36:$L36)</f>
         <v>4.0399082702959772</v>
       </c>
-      <c r="AW37" s="3">
+      <c r="AW37">
         <f>(F37/SUM($C37:$N37)-U37/SUM($R37:$AC37))*SUM('RICBP-it0_damagesbyregionoutput'!$A36:$L36)</f>
         <v>4.4044051562555619</v>
       </c>
-      <c r="AX37" s="3">
+      <c r="AX37">
         <f>(G37/SUM($C37:$N37)-V37/SUM($R37:$AC37))*SUM('RICBP-it0_damagesbyregionoutput'!$A36:$L36)</f>
         <v>7.34501531403059</v>
       </c>
-      <c r="AY37" s="3">
+      <c r="AY37">
         <f>(H37/SUM($C37:$N37)-W37/SUM($R37:$AC37))*SUM('RICBP-it0_damagesbyregionoutput'!$A36:$L36)</f>
         <v>-15.709579408930972</v>
       </c>
-      <c r="AZ37" s="3">
+      <c r="AZ37">
         <f>(I37/SUM($C37:$N37)-X37/SUM($R37:$AC37))*SUM('RICBP-it0_damagesbyregionoutput'!$A36:$L36)</f>
         <v>1.2604115672843323</v>
       </c>
-      <c r="BA37" s="3">
+      <c r="BA37">
         <f>(J37/SUM($C37:$N37)-Y37/SUM($R37:$AC37))*SUM('RICBP-it0_damagesbyregionoutput'!$A36:$L36)</f>
         <v>-2.1599968570012402</v>
       </c>
-      <c r="BB37" s="3">
+      <c r="BB37">
         <f>(K37/SUM($C37:$N37)-Z37/SUM($R37:$AC37))*SUM('RICBP-it0_damagesbyregionoutput'!$A36:$L36)</f>
         <v>-44.037557503326035</v>
       </c>
-      <c r="BC37" s="3">
+      <c r="BC37">
         <f>(L37/SUM($C37:$N37)-AA37/SUM($R37:$AC37))*SUM('RICBP-it0_damagesbyregionoutput'!$A36:$L36)</f>
         <v>1.5442023190756329</v>
       </c>
-      <c r="BD37" s="3">
+      <c r="BD37">
         <f>(M37/SUM($C37:$N37)-AB37/SUM($R37:$AC37))*SUM('RICBP-it0_damagesbyregionoutput'!$A36:$L36)</f>
         <v>1.7042747155442377</v>
       </c>
-      <c r="BE37" s="3">
+      <c r="BE37">
         <f>(N37/SUM($C37:$N37)-AC37/SUM($R37:$AC37))*SUM('RICBP-it0_damagesbyregionoutput'!$A36:$L36)</f>
         <v>-6.1335813228422502</v>
       </c>
@@ -19936,51 +19936,51 @@
         <f t="shared" si="3"/>
         <v>-81.270189871040586</v>
       </c>
-      <c r="AT38" s="3">
+      <c r="AT38">
         <f>(C38/SUM($C38:$N38)-R38/SUM($R38:$AC38))*SUM('RICBP-it0_damagesbyregionoutput'!$A37:$L37)</f>
         <v>29.511946957772491</v>
       </c>
-      <c r="AU38" s="3">
+      <c r="AU38">
         <f>(D38/SUM($C38:$N38)-S38/SUM($R38:$AC38))*SUM('RICBP-it0_damagesbyregionoutput'!$A37:$L37)</f>
         <v>21.326945715114892</v>
       </c>
-      <c r="AV38" s="3">
+      <c r="AV38">
         <f>(E38/SUM($C38:$N38)-T38/SUM($R38:$AC38))*SUM('RICBP-it0_damagesbyregionoutput'!$A37:$L37)</f>
         <v>4.3064266501121304</v>
       </c>
-      <c r="AW38" s="3">
+      <c r="AW38">
         <f>(F38/SUM($C38:$N38)-U38/SUM($R38:$AC38))*SUM('RICBP-it0_damagesbyregionoutput'!$A37:$L37)</f>
         <v>4.6872534462132158</v>
       </c>
-      <c r="AX38" s="3">
+      <c r="AX38">
         <f>(G38/SUM($C38:$N38)-V38/SUM($R38:$AC38))*SUM('RICBP-it0_damagesbyregionoutput'!$A37:$L37)</f>
         <v>7.810681724696142</v>
       </c>
-      <c r="AY38" s="3">
+      <c r="AY38">
         <f>(H38/SUM($C38:$N38)-W38/SUM($R38:$AC38))*SUM('RICBP-it0_damagesbyregionoutput'!$A37:$L37)</f>
         <v>-16.868693041906319</v>
       </c>
-      <c r="AZ38" s="3">
+      <c r="AZ38">
         <f>(I38/SUM($C38:$N38)-X38/SUM($R38:$AC38))*SUM('RICBP-it0_damagesbyregionoutput'!$A37:$L37)</f>
         <v>1.4694758599812581</v>
       </c>
-      <c r="BA38" s="3">
+      <c r="BA38">
         <f>(J38/SUM($C38:$N38)-Y38/SUM($R38:$AC38))*SUM('RICBP-it0_damagesbyregionoutput'!$A37:$L37)</f>
         <v>-2.1876312310162995</v>
       </c>
-      <c r="BB38" s="3">
+      <c r="BB38">
         <f>(K38/SUM($C38:$N38)-Z38/SUM($R38:$AC38))*SUM('RICBP-it0_damagesbyregionoutput'!$A37:$L37)</f>
         <v>-47.026085845819075</v>
       </c>
-      <c r="BC38" s="3">
+      <c r="BC38">
         <f>(L38/SUM($C38:$N38)-AA38/SUM($R38:$AC38))*SUM('RICBP-it0_damagesbyregionoutput'!$A37:$L37)</f>
         <v>1.7110220109549259</v>
       </c>
-      <c r="BD38" s="3">
+      <c r="BD38">
         <f>(M38/SUM($C38:$N38)-AB38/SUM($R38:$AC38))*SUM('RICBP-it0_damagesbyregionoutput'!$A37:$L37)</f>
         <v>1.8284063273516609</v>
       </c>
-      <c r="BE38" s="3">
+      <c r="BE38">
         <f>(N38/SUM($C38:$N38)-AC38/SUM($R38:$AC38))*SUM('RICBP-it0_damagesbyregionoutput'!$A37:$L37)</f>
         <v>-6.5697485734550654</v>
       </c>
@@ -20196,51 +20196,51 @@
         <f t="shared" si="5"/>
         <v>-89.006983217467734</v>
       </c>
-      <c r="AT39" s="3">
+      <c r="AT39">
         <f>(C39/SUM($C39:$N39)-R39/SUM($R39:$AC39))*SUM('RICBP-it0_damagesbyregionoutput'!$A38:$L38)</f>
         <v>31.381536574220988</v>
       </c>
-      <c r="AU39" s="3">
+      <c r="AU39">
         <f>(D39/SUM($C39:$N39)-S39/SUM($R39:$AC39))*SUM('RICBP-it0_damagesbyregionoutput'!$A38:$L38)</f>
         <v>22.679423752095158</v>
       </c>
-      <c r="AV39" s="3">
+      <c r="AV39">
         <f>(E39/SUM($C39:$N39)-T39/SUM($R39:$AC39))*SUM('RICBP-it0_damagesbyregionoutput'!$A38:$L38)</f>
         <v>4.5838259542479465</v>
       </c>
-      <c r="AW39" s="3">
+      <c r="AW39">
         <f>(F39/SUM($C39:$N39)-U39/SUM($R39:$AC39))*SUM('RICBP-it0_damagesbyregionoutput'!$A38:$L38)</f>
         <v>4.9816386346086654</v>
       </c>
-      <c r="AX39" s="3">
+      <c r="AX39">
         <f>(G39/SUM($C39:$N39)-V39/SUM($R39:$AC39))*SUM('RICBP-it0_damagesbyregionoutput'!$A38:$L38)</f>
         <v>8.29536485669224</v>
       </c>
-      <c r="AY39" s="3">
+      <c r="AY39">
         <f>(H39/SUM($C39:$N39)-W39/SUM($R39:$AC39))*SUM('RICBP-it0_damagesbyregionoutput'!$A38:$L38)</f>
         <v>-18.078303928439187</v>
       </c>
-      <c r="AZ39" s="3">
+      <c r="AZ39">
         <f>(I39/SUM($C39:$N39)-X39/SUM($R39:$AC39))*SUM('RICBP-it0_damagesbyregionoutput'!$A38:$L38)</f>
         <v>1.6917618438451587</v>
       </c>
-      <c r="BA39" s="3">
+      <c r="BA39">
         <f>(J39/SUM($C39:$N39)-Y39/SUM($R39:$AC39))*SUM('RICBP-it0_damagesbyregionoutput'!$A38:$L38)</f>
         <v>-2.2138060038474614</v>
       </c>
-      <c r="BB39" s="3">
+      <c r="BB39">
         <f>(K39/SUM($C39:$N39)-Z39/SUM($R39:$AC39))*SUM('RICBP-it0_damagesbyregionoutput'!$A38:$L38)</f>
         <v>-50.136136366645708</v>
       </c>
-      <c r="BC39" s="3">
+      <c r="BC39">
         <f>(L39/SUM($C39:$N39)-AA39/SUM($R39:$AC39))*SUM('RICBP-it0_damagesbyregionoutput'!$A38:$L38)</f>
         <v>1.8861766857110505</v>
       </c>
-      <c r="BD39" s="3">
+      <c r="BD39">
         <f>(M39/SUM($C39:$N39)-AB39/SUM($R39:$AC39))*SUM('RICBP-it0_damagesbyregionoutput'!$A38:$L38)</f>
         <v>1.9576558814932561</v>
       </c>
-      <c r="BE39" s="3">
+      <c r="BE39">
         <f>(N39/SUM($C39:$N39)-AC39/SUM($R39:$AC39))*SUM('RICBP-it0_damagesbyregionoutput'!$A38:$L38)</f>
         <v>-7.0291378839821235</v>
       </c>
@@ -20456,51 +20456,51 @@
         <f t="shared" si="5"/>
         <v>-97.300244452626444</v>
       </c>
-      <c r="AT40" s="3">
+      <c r="AT40">
         <f>(C40/SUM($C40:$N40)-R40/SUM($R40:$AC40))*SUM('RICBP-it0_damagesbyregionoutput'!$A39:$L39)</f>
         <v>33.326642644971486</v>
       </c>
-      <c r="AU40" s="3">
+      <c r="AU40">
         <f>(D40/SUM($C40:$N40)-S40/SUM($R40:$AC40))*SUM('RICBP-it0_damagesbyregionoutput'!$A39:$L39)</f>
         <v>24.08655515486301</v>
       </c>
-      <c r="AV40" s="3">
+      <c r="AV40">
         <f>(E40/SUM($C40:$N40)-T40/SUM($R40:$AC40))*SUM('RICBP-it0_damagesbyregionoutput'!$A39:$L39)</f>
         <v>4.8725016617103716</v>
       </c>
-      <c r="AW40" s="3">
+      <c r="AW40">
         <f>(F40/SUM($C40:$N40)-U40/SUM($R40:$AC40))*SUM('RICBP-it0_damagesbyregionoutput'!$A39:$L39)</f>
         <v>5.2879828960316457</v>
       </c>
-      <c r="AX40" s="3">
+      <c r="AX40">
         <f>(G40/SUM($C40:$N40)-V40/SUM($R40:$AC40))*SUM('RICBP-it0_damagesbyregionoutput'!$A39:$L39)</f>
         <v>8.7997646641664407</v>
       </c>
-      <c r="AY40" s="3">
+      <c r="AY40">
         <f>(H40/SUM($C40:$N40)-W40/SUM($R40:$AC40))*SUM('RICBP-it0_damagesbyregionoutput'!$A39:$L39)</f>
         <v>-19.340167252802559</v>
       </c>
-      <c r="AZ40" s="3">
+      <c r="AZ40">
         <f>(I40/SUM($C40:$N40)-X40/SUM($R40:$AC40))*SUM('RICBP-it0_damagesbyregionoutput'!$A39:$L39)</f>
         <v>1.9276547707972833</v>
       </c>
-      <c r="BA40" s="3">
+      <c r="BA40">
         <f>(J40/SUM($C40:$N40)-Y40/SUM($R40:$AC40))*SUM('RICBP-it0_damagesbyregionoutput'!$A39:$L39)</f>
         <v>-2.238567093577752</v>
       </c>
-      <c r="BB40" s="3">
+      <c r="BB40">
         <f>(K40/SUM($C40:$N40)-Z40/SUM($R40:$AC40))*SUM('RICBP-it0_damagesbyregionoutput'!$A39:$L39)</f>
         <v>-53.371708592310419</v>
       </c>
-      <c r="BC40" s="3">
+      <c r="BC40">
         <f>(L40/SUM($C40:$N40)-AA40/SUM($R40:$AC40))*SUM('RICBP-it0_damagesbyregionoutput'!$A39:$L39)</f>
         <v>2.0699211945787725</v>
       </c>
-      <c r="BD40" s="3">
+      <c r="BD40">
         <f>(M40/SUM($C40:$N40)-AB40/SUM($R40:$AC40))*SUM('RICBP-it0_damagesbyregionoutput'!$A39:$L39)</f>
         <v>2.0921680286220457</v>
       </c>
-      <c r="BE40" s="3">
+      <c r="BE40">
         <f>(N40/SUM($C40:$N40)-AC40/SUM($R40:$AC40))*SUM('RICBP-it0_damagesbyregionoutput'!$A39:$L39)</f>
         <v>-7.5127480770503512</v>
       </c>
@@ -20716,51 +20716,51 @@
         <f t="shared" si="5"/>
         <v>-106.17876538927273</v>
       </c>
-      <c r="AT41" s="3">
+      <c r="AT41">
         <f>(C41/SUM($C41:$N41)-R41/SUM($R41:$AC41))*SUM('RICBP-it0_damagesbyregionoutput'!$A40:$L40)</f>
         <v>35.350128681748892</v>
       </c>
-      <c r="AU41" s="3">
+      <c r="AU41">
         <f>(D41/SUM($C41:$N41)-S41/SUM($R41:$AC41))*SUM('RICBP-it0_damagesbyregionoutput'!$A40:$L40)</f>
         <v>25.550356091373391</v>
       </c>
-      <c r="AV41" s="3">
+      <c r="AV41">
         <f>(E41/SUM($C41:$N41)-T41/SUM($R41:$AC41))*SUM('RICBP-it0_damagesbyregionoutput'!$A40:$L40)</f>
         <v>5.1728826983930603</v>
       </c>
-      <c r="AW41" s="3">
+      <c r="AW41">
         <f>(F41/SUM($C41:$N41)-U41/SUM($R41:$AC41))*SUM('RICBP-it0_damagesbyregionoutput'!$A40:$L40)</f>
         <v>5.6067434986405162</v>
       </c>
-      <c r="AX41" s="3">
+      <c r="AX41">
         <f>(G41/SUM($C41:$N41)-V41/SUM($R41:$AC41))*SUM('RICBP-it0_damagesbyregionoutput'!$A40:$L40)</f>
         <v>9.3246384190813991</v>
       </c>
-      <c r="AY41" s="3">
+      <c r="AY41">
         <f>(H41/SUM($C41:$N41)-W41/SUM($R41:$AC41))*SUM('RICBP-it0_damagesbyregionoutput'!$A40:$L40)</f>
         <v>-20.65620995463312</v>
       </c>
-      <c r="AZ41" s="3">
+      <c r="AZ41">
         <f>(I41/SUM($C41:$N41)-X41/SUM($R41:$AC41))*SUM('RICBP-it0_damagesbyregionoutput'!$A40:$L40)</f>
         <v>2.1775866408196007</v>
       </c>
-      <c r="BA41" s="3">
+      <c r="BA41">
         <f>(J41/SUM($C41:$N41)-Y41/SUM($R41:$AC41))*SUM('RICBP-it0_damagesbyregionoutput'!$A40:$L40)</f>
         <v>-2.26194982869433</v>
       </c>
-      <c r="BB41" s="3">
+      <c r="BB41">
         <f>(K41/SUM($C41:$N41)-Z41/SUM($R41:$AC41))*SUM('RICBP-it0_damagesbyregionoutput'!$A40:$L40)</f>
         <v>-56.737184691202728</v>
       </c>
-      <c r="BC41" s="3">
+      <c r="BC41">
         <f>(L41/SUM($C41:$N41)-AA41/SUM($R41:$AC41))*SUM('RICBP-it0_damagesbyregionoutput'!$A40:$L40)</f>
         <v>2.2625410792399689</v>
       </c>
-      <c r="BD41" s="3">
+      <c r="BD41">
         <f>(M41/SUM($C41:$N41)-AB41/SUM($R41:$AC41))*SUM('RICBP-it0_damagesbyregionoutput'!$A40:$L40)</f>
         <v>2.2321029481650636</v>
       </c>
-      <c r="BE41" s="3">
+      <c r="BE41">
         <f>(N41/SUM($C41:$N41)-AC41/SUM($R41:$AC41))*SUM('RICBP-it0_damagesbyregionoutput'!$A40:$L40)</f>
         <v>-8.0216355829317365</v>
       </c>
@@ -20976,51 +20976,51 @@
         <f t="shared" si="5"/>
         <v>-115.67247815182338</v>
       </c>
-      <c r="AT42" s="3">
+      <c r="AT42">
         <f>(C42/SUM($C42:$N42)-R42/SUM($R42:$AC42))*SUM('RICBP-it0_damagesbyregionoutput'!$A41:$L41)</f>
         <v>37.455081285060338</v>
       </c>
-      <c r="AU42" s="3">
+      <c r="AU42">
         <f>(D42/SUM($C42:$N42)-S42/SUM($R42:$AC42))*SUM('RICBP-it0_damagesbyregionoutput'!$A41:$L41)</f>
         <v>27.073002054466624</v>
       </c>
-      <c r="AV42" s="3">
+      <c r="AV42">
         <f>(E42/SUM($C42:$N42)-T42/SUM($R42:$AC42))*SUM('RICBP-it0_damagesbyregionoutput'!$A41:$L41)</f>
         <v>5.4854314040401304</v>
       </c>
-      <c r="AW42" s="3">
+      <c r="AW42">
         <f>(F42/SUM($C42:$N42)-U42/SUM($R42:$AC42))*SUM('RICBP-it0_damagesbyregionoutput'!$A41:$L41)</f>
         <v>5.9384127668047473</v>
       </c>
-      <c r="AX42" s="3">
+      <c r="AX42">
         <f>(G42/SUM($C42:$N42)-V42/SUM($R42:$AC42))*SUM('RICBP-it0_damagesbyregionoutput'!$A41:$L41)</f>
         <v>9.8708006934628134</v>
       </c>
-      <c r="AY42" s="3">
+      <c r="AY42">
         <f>(H42/SUM($C42:$N42)-W42/SUM($R42:$AC42))*SUM('RICBP-it0_damagesbyregionoutput'!$A41:$L41)</f>
         <v>-22.028528264171594</v>
       </c>
-      <c r="AZ42" s="3">
+      <c r="AZ42">
         <f>(I42/SUM($C42:$N42)-X42/SUM($R42:$AC42))*SUM('RICBP-it0_damagesbyregionoutput'!$A41:$L41)</f>
         <v>2.442036456268045</v>
       </c>
-      <c r="BA42" s="3">
+      <c r="BA42">
         <f>(J42/SUM($C42:$N42)-Y42/SUM($R42:$AC42))*SUM('RICBP-it0_damagesbyregionoutput'!$A41:$L41)</f>
         <v>-2.283978761032325</v>
       </c>
-      <c r="BB42" s="3">
+      <c r="BB42">
         <f>(K42/SUM($C42:$N42)-Z42/SUM($R42:$AC42))*SUM('RICBP-it0_damagesbyregionoutput'!$A41:$L41)</f>
         <v>-60.237328773046031</v>
       </c>
-      <c r="BC42" s="3">
+      <c r="BC42">
         <f>(L42/SUM($C42:$N42)-AA42/SUM($R42:$AC42))*SUM('RICBP-it0_damagesbyregionoutput'!$A41:$L41)</f>
         <v>2.4643523363765785</v>
       </c>
-      <c r="BD42" s="3">
+      <c r="BD42">
         <f>(M42/SUM($C42:$N42)-AB42/SUM($R42:$AC42))*SUM('RICBP-it0_damagesbyregionoutput'!$A41:$L41)</f>
         <v>2.3776365502805263</v>
       </c>
-      <c r="BE42" s="3">
+      <c r="BE42">
         <f>(N42/SUM($C42:$N42)-AC42/SUM($R42:$AC42))*SUM('RICBP-it0_damagesbyregionoutput'!$A41:$L41)</f>
         <v>-8.5569177485098891</v>
       </c>
@@ -21236,51 +21236,51 @@
         <f t="shared" si="5"/>
         <v>-125.81253380679365</v>
       </c>
-      <c r="AT43" s="3">
+      <c r="AT43">
         <f>(C43/SUM($C43:$N43)-R43/SUM($R43:$AC43))*SUM('RICBP-it0_damagesbyregionoutput'!$A42:$L42)</f>
         <v>39.644808533634162</v>
       </c>
-      <c r="AU43" s="3">
+      <c r="AU43">
         <f>(D43/SUM($C43:$N43)-S43/SUM($R43:$AC43))*SUM('RICBP-it0_damagesbyregionoutput'!$A42:$L42)</f>
         <v>28.656827234104036</v>
       </c>
-      <c r="AV43" s="3">
+      <c r="AV43">
         <f>(E43/SUM($C43:$N43)-T43/SUM($R43:$AC43))*SUM('RICBP-it0_damagesbyregionoutput'!$A42:$L42)</f>
         <v>5.8106433312331198</v>
       </c>
-      <c r="AW43" s="3">
+      <c r="AW43">
         <f>(F43/SUM($C43:$N43)-U43/SUM($R43:$AC43))*SUM('RICBP-it0_damagesbyregionoutput'!$A42:$L42)</f>
         <v>6.2835178699644834</v>
       </c>
-      <c r="AX43" s="3">
+      <c r="AX43">
         <f>(G43/SUM($C43:$N43)-V43/SUM($R43:$AC43))*SUM('RICBP-it0_damagesbyregionoutput'!$A42:$L42)</f>
         <v>10.439123052785483</v>
       </c>
-      <c r="AY43" s="3">
+      <c r="AY43">
         <f>(H43/SUM($C43:$N43)-W43/SUM($R43:$AC43))*SUM('RICBP-it0_damagesbyregionoutput'!$A42:$L42)</f>
         <v>-23.459384895665906</v>
       </c>
-      <c r="AZ43" s="3">
+      <c r="AZ43">
         <f>(I43/SUM($C43:$N43)-X43/SUM($R43:$AC43))*SUM('RICBP-it0_damagesbyregionoutput'!$A42:$L42)</f>
         <v>2.7215303227961587</v>
       </c>
-      <c r="BA43" s="3">
+      <c r="BA43">
         <f>(J43/SUM($C43:$N43)-Y43/SUM($R43:$AC43))*SUM('RICBP-it0_damagesbyregionoutput'!$A42:$L42)</f>
         <v>-2.3046675250988287</v>
       </c>
-      <c r="BB43" s="3">
+      <c r="BB43">
         <f>(K43/SUM($C43:$N43)-Z43/SUM($R43:$AC43))*SUM('RICBP-it0_damagesbyregionoutput'!$A42:$L42)</f>
         <v>-63.877283875748986</v>
       </c>
-      <c r="BC43" s="3">
+      <c r="BC43">
         <f>(L43/SUM($C43:$N43)-AA43/SUM($R43:$AC43))*SUM('RICBP-it0_damagesbyregionoutput'!$A42:$L42)</f>
         <v>2.6757011084076314</v>
       </c>
-      <c r="BD43" s="3">
+      <c r="BD43">
         <f>(M43/SUM($C43:$N43)-AB43/SUM($R43:$AC43))*SUM('RICBP-it0_damagesbyregionoutput'!$A42:$L42)</f>
         <v>2.52896051989983</v>
       </c>
-      <c r="BE43" s="3">
+      <c r="BE43">
         <f>(N43/SUM($C43:$N43)-AC43/SUM($R43:$AC43))*SUM('RICBP-it0_damagesbyregionoutput'!$A42:$L42)</f>
         <v>-9.1197756763112388</v>
       </c>
@@ -21496,51 +21496,51 @@
         <f t="shared" si="5"/>
         <v>-136.63138231255448</v>
       </c>
-      <c r="AT44" s="3">
+      <c r="AT44">
         <f>(C44/SUM($C44:$N44)-R44/SUM($R44:$AC44))*SUM('RICBP-it0_damagesbyregionoutput'!$A43:$L43)</f>
         <v>41.922838150109555</v>
       </c>
-      <c r="AU44" s="3">
+      <c r="AU44">
         <f>(D44/SUM($C44:$N44)-S44/SUM($R44:$AC44))*SUM('RICBP-it0_damagesbyregionoutput'!$A43:$L43)</f>
         <v>30.304323569253871</v>
       </c>
-      <c r="AV44" s="3">
+      <c r="AV44">
         <f>(E44/SUM($C44:$N44)-T44/SUM($R44:$AC44))*SUM('RICBP-it0_damagesbyregionoutput'!$A43:$L43)</f>
         <v>6.1490470048098818</v>
       </c>
-      <c r="AW44" s="3">
+      <c r="AW44">
         <f>(F44/SUM($C44:$N44)-U44/SUM($R44:$AC44))*SUM('RICBP-it0_damagesbyregionoutput'!$A43:$L43)</f>
         <v>6.6426205746294142</v>
       </c>
-      <c r="AX44" s="3">
+      <c r="AX44">
         <f>(G44/SUM($C44:$N44)-V44/SUM($R44:$AC44))*SUM('RICBP-it0_damagesbyregionoutput'!$A43:$L43)</f>
         <v>11.030533687407621</v>
       </c>
-      <c r="AY44" s="3">
+      <c r="AY44">
         <f>(H44/SUM($C44:$N44)-W44/SUM($R44:$AC44))*SUM('RICBP-it0_damagesbyregionoutput'!$A43:$L43)</f>
         <v>-24.951206383965886</v>
       </c>
-      <c r="AZ44" s="3">
+      <c r="AZ44">
         <f>(I44/SUM($C44:$N44)-X44/SUM($R44:$AC44))*SUM('RICBP-it0_damagesbyregionoutput'!$A43:$L43)</f>
         <v>3.016641477751048</v>
       </c>
-      <c r="BA44" s="3">
+      <c r="BA44">
         <f>(J44/SUM($C44:$N44)-Y44/SUM($R44:$AC44))*SUM('RICBP-it0_damagesbyregionoutput'!$A43:$L43)</f>
         <v>-2.3240187692515244</v>
       </c>
-      <c r="BB44" s="3">
+      <c r="BB44">
         <f>(K44/SUM($C44:$N44)-Z44/SUM($R44:$AC44))*SUM('RICBP-it0_damagesbyregionoutput'!$A43:$L43)</f>
         <v>-67.662568171599162</v>
       </c>
-      <c r="BC44" s="3">
+      <c r="BC44">
         <f>(L44/SUM($C44:$N44)-AA44/SUM($R44:$AC44))*SUM('RICBP-it0_damagesbyregionoutput'!$A43:$L43)</f>
         <v>2.8969633635603316</v>
       </c>
-      <c r="BD44" s="3">
+      <c r="BD44">
         <f>(M44/SUM($C44:$N44)-AB44/SUM($R44:$AC44))*SUM('RICBP-it0_damagesbyregionoutput'!$A43:$L43)</f>
         <v>2.6862822735861172</v>
       </c>
-      <c r="BE44" s="3">
+      <c r="BE44">
         <f>(N44/SUM($C44:$N44)-AC44/SUM($R44:$AC44))*SUM('RICBP-it0_damagesbyregionoutput'!$A43:$L43)</f>
         <v>-9.7114567762913246</v>
       </c>
@@ -21756,51 +21756,51 @@
         <f t="shared" si="5"/>
         <v>-148.1628535777435</v>
       </c>
-      <c r="AT45" s="3">
+      <c r="AT45">
         <f>(C45/SUM($C45:$N45)-R45/SUM($R45:$AC45))*SUM('RICBP-it0_damagesbyregionoutput'!$A44:$L44)</f>
         <v>44.292915947248481</v>
       </c>
-      <c r="AU45" s="3">
+      <c r="AU45">
         <f>(D45/SUM($C45:$N45)-S45/SUM($R45:$AC45))*SUM('RICBP-it0_damagesbyregionoutput'!$A44:$L44)</f>
         <v>32.018139871326255</v>
       </c>
-      <c r="AV45" s="3">
+      <c r="AV45">
         <f>(E45/SUM($C45:$N45)-T45/SUM($R45:$AC45))*SUM('RICBP-it0_damagesbyregionoutput'!$A44:$L44)</f>
         <v>6.5012037175847945</v>
       </c>
-      <c r="AW45" s="3">
+      <c r="AW45">
         <f>(F45/SUM($C45:$N45)-U45/SUM($R45:$AC45))*SUM('RICBP-it0_damagesbyregionoutput'!$A44:$L44)</f>
         <v>7.016317039240703</v>
       </c>
-      <c r="AX45" s="3">
+      <c r="AX45">
         <f>(G45/SUM($C45:$N45)-V45/SUM($R45:$AC45))*SUM('RICBP-it0_damagesbyregionoutput'!$A44:$L44)</f>
         <v>11.646017113516935</v>
       </c>
-      <c r="AY45" s="3">
+      <c r="AY45">
         <f>(H45/SUM($C45:$N45)-W45/SUM($R45:$AC45))*SUM('RICBP-it0_damagesbyregionoutput'!$A44:$L44)</f>
         <v>-26.506580849395693</v>
       </c>
-      <c r="AZ45" s="3">
+      <c r="AZ45">
         <f>(I45/SUM($C45:$N45)-X45/SUM($R45:$AC45))*SUM('RICBP-it0_damagesbyregionoutput'!$A44:$L44)</f>
         <v>3.3279903113867415</v>
       </c>
-      <c r="BA45" s="3">
+      <c r="BA45">
         <f>(J45/SUM($C45:$N45)-Y45/SUM($R45:$AC45))*SUM('RICBP-it0_damagesbyregionoutput'!$A44:$L44)</f>
         <v>-2.3420241560191042</v>
       </c>
-      <c r="BB45" s="3">
+      <c r="BB45">
         <f>(K45/SUM($C45:$N45)-Z45/SUM($R45:$AC45))*SUM('RICBP-it0_damagesbyregionoutput'!$A44:$L44)</f>
         <v>-71.599071329117805</v>
       </c>
-      <c r="BC45" s="3">
+      <c r="BC45">
         <f>(L45/SUM($C45:$N45)-AA45/SUM($R45:$AC45))*SUM('RICBP-it0_damagesbyregionoutput'!$A44:$L44)</f>
         <v>3.1285446100312235</v>
       </c>
-      <c r="BD45" s="3">
+      <c r="BD45">
         <f>(M45/SUM($C45:$N45)-AB45/SUM($R45:$AC45))*SUM('RICBP-it0_damagesbyregionoutput'!$A44:$L44)</f>
         <v>2.8498248763413581</v>
       </c>
-      <c r="BE45" s="3">
+      <c r="BE45">
         <f>(N45/SUM($C45:$N45)-AC45/SUM($R45:$AC45))*SUM('RICBP-it0_damagesbyregionoutput'!$A44:$L44)</f>
         <v>-10.333277152143921</v>
       </c>
@@ -22016,51 +22016,51 @@
         <f t="shared" si="5"/>
         <v>-160.4422395805893</v>
       </c>
-      <c r="AT46" s="3">
+      <c r="AT46">
         <f>(C46/SUM($C46:$N46)-R46/SUM($R46:$AC46))*SUM('RICBP-it0_damagesbyregionoutput'!$A45:$L45)</f>
         <v>46.759004845825942</v>
       </c>
-      <c r="AU46" s="3">
+      <c r="AU46">
         <f>(D46/SUM($C46:$N46)-S46/SUM($R46:$AC46))*SUM('RICBP-it0_damagesbyregionoutput'!$A45:$L45)</f>
         <v>33.801081253263625</v>
       </c>
-      <c r="AV46" s="3">
+      <c r="AV46">
         <f>(E46/SUM($C46:$N46)-T46/SUM($R46:$AC46))*SUM('RICBP-it0_damagesbyregionoutput'!$A45:$L45)</f>
         <v>6.8677074067614132</v>
       </c>
-      <c r="AW46" s="3">
+      <c r="AW46">
         <f>(F46/SUM($C46:$N46)-U46/SUM($R46:$AC46))*SUM('RICBP-it0_damagesbyregionoutput'!$A45:$L45)</f>
         <v>7.4052376977724723</v>
       </c>
-      <c r="AX46" s="3">
+      <c r="AX46">
         <f>(G46/SUM($C46:$N46)-V46/SUM($R46:$AC46))*SUM('RICBP-it0_damagesbyregionoutput'!$A45:$L45)</f>
         <v>12.286614018855477</v>
       </c>
-      <c r="AY46" s="3">
+      <c r="AY46">
         <f>(H46/SUM($C46:$N46)-W46/SUM($R46:$AC46))*SUM('RICBP-it0_damagesbyregionoutput'!$A45:$L45)</f>
         <v>-28.12825635221683</v>
       </c>
-      <c r="AZ46" s="3">
+      <c r="AZ46">
         <f>(I46/SUM($C46:$N46)-X46/SUM($R46:$AC46))*SUM('RICBP-it0_damagesbyregionoutput'!$A45:$L45)</f>
         <v>3.6562444310670572</v>
       </c>
-      <c r="BA46" s="3">
+      <c r="BA46">
         <f>(J46/SUM($C46:$N46)-Y46/SUM($R46:$AC46))*SUM('RICBP-it0_damagesbyregionoutput'!$A45:$L45)</f>
         <v>-2.3586644175699636</v>
       </c>
-      <c r="BB46" s="3">
+      <c r="BB46">
         <f>(K46/SUM($C46:$N46)-Z46/SUM($R46:$AC46))*SUM('RICBP-it0_damagesbyregionoutput'!$A45:$L45)</f>
         <v>-75.693051602206751</v>
       </c>
-      <c r="BC46" s="3">
+      <c r="BC46">
         <f>(L46/SUM($C46:$N46)-AA46/SUM($R46:$AC46))*SUM('RICBP-it0_damagesbyregionoutput'!$A45:$L45)</f>
         <v>3.3708796750088683</v>
       </c>
-      <c r="BD46" s="3">
+      <c r="BD46">
         <f>(M46/SUM($C46:$N46)-AB46/SUM($R46:$AC46))*SUM('RICBP-it0_damagesbyregionoutput'!$A45:$L45)</f>
         <v>3.0198269502365442</v>
       </c>
-      <c r="BE46" s="3">
+      <c r="BE46">
         <f>(N46/SUM($C46:$N46)-AC46/SUM($R46:$AC46))*SUM('RICBP-it0_damagesbyregionoutput'!$A45:$L45)</f>
         <v>-10.986623906797893</v>
       </c>
@@ -22276,51 +22276,51 @@
         <f t="shared" si="5"/>
         <v>-173.50637760533866</v>
       </c>
-      <c r="AT47" s="3">
+      <c r="AT47">
         <f>(C47/SUM($C47:$N47)-R47/SUM($R47:$AC47))*SUM('RICBP-it0_damagesbyregionoutput'!$A46:$L46)</f>
         <v>49.32528462777605</v>
       </c>
-      <c r="AU47" s="3">
+      <c r="AU47">
         <f>(D47/SUM($C47:$N47)-S47/SUM($R47:$AC47))*SUM('RICBP-it0_damagesbyregionoutput'!$A46:$L46)</f>
         <v>35.656109002777583</v>
       </c>
-      <c r="AV47" s="3">
+      <c r="AV47">
         <f>(E47/SUM($C47:$N47)-T47/SUM($R47:$AC47))*SUM('RICBP-it0_damagesbyregionoutput'!$A46:$L46)</f>
         <v>7.2491846364195807</v>
       </c>
-      <c r="AW47" s="3">
+      <c r="AW47">
         <f>(F47/SUM($C47:$N47)-U47/SUM($R47:$AC47))*SUM('RICBP-it0_damagesbyregionoutput'!$A46:$L46)</f>
         <v>7.8100472577804787</v>
       </c>
-      <c r="AX47" s="3">
+      <c r="AX47">
         <f>(G47/SUM($C47:$N47)-V47/SUM($R47:$AC47))*SUM('RICBP-it0_damagesbyregionoutput'!$A46:$L46)</f>
         <v>12.953421295181895</v>
       </c>
-      <c r="AY47" s="3">
+      <c r="AY47">
         <f>(H47/SUM($C47:$N47)-W47/SUM($R47:$AC47))*SUM('RICBP-it0_damagesbyregionoutput'!$A46:$L46)</f>
         <v>-29.819139921406787</v>
       </c>
-      <c r="AZ47" s="3">
+      <c r="AZ47">
         <f>(I47/SUM($C47:$N47)-X47/SUM($R47:$AC47))*SUM('RICBP-it0_damagesbyregionoutput'!$A46:$L46)</f>
         <v>4.0021188055768491</v>
       </c>
-      <c r="BA47" s="3">
+      <c r="BA47">
         <f>(J47/SUM($C47:$N47)-Y47/SUM($R47:$AC47))*SUM('RICBP-it0_damagesbyregionoutput'!$A46:$L46)</f>
         <v>-2.3739094493179795</v>
       </c>
-      <c r="BB47" s="3">
+      <c r="BB47">
         <f>(K47/SUM($C47:$N47)-Z47/SUM($R47:$AC47))*SUM('RICBP-it0_damagesbyregionoutput'!$A46:$L46)</f>
         <v>-79.951133991944417</v>
       </c>
-      <c r="BC47" s="3">
+      <c r="BC47">
         <f>(L47/SUM($C47:$N47)-AA47/SUM($R47:$AC47))*SUM('RICBP-it0_damagesbyregionoutput'!$A46:$L46)</f>
         <v>3.624432569001018</v>
       </c>
-      <c r="BD47" s="3">
+      <c r="BD47">
         <f>(M47/SUM($C47:$N47)-AB47/SUM($R47:$AC47))*SUM('RICBP-it0_damagesbyregionoutput'!$A46:$L46)</f>
         <v>3.1965425966358048</v>
       </c>
-      <c r="BE47" s="3">
+      <c r="BE47">
         <f>(N47/SUM($C47:$N47)-AC47/SUM($R47:$AC47))*SUM('RICBP-it0_damagesbyregionoutput'!$A46:$L46)</f>
         <v>-11.672957428480094</v>
       </c>
@@ -22536,51 +22536,51 @@
         <f t="shared" si="5"/>
         <v>-187.39373471915113</v>
       </c>
-      <c r="AT48" s="3">
+      <c r="AT48">
         <f>(C48/SUM($C48:$N48)-R48/SUM($R48:$AC48))*SUM('RICBP-it0_damagesbyregionoutput'!$A47:$L47)</f>
         <v>51.996152510787311</v>
       </c>
-      <c r="AU48" s="3">
+      <c r="AU48">
         <f>(D48/SUM($C48:$N48)-S48/SUM($R48:$AC48))*SUM('RICBP-it0_damagesbyregionoutput'!$A47:$L47)</f>
         <v>37.586340979186041</v>
       </c>
-      <c r="AV48" s="3">
+      <c r="AV48">
         <f>(E48/SUM($C48:$N48)-T48/SUM($R48:$AC48))*SUM('RICBP-it0_damagesbyregionoutput'!$A47:$L47)</f>
         <v>7.6462946998184673</v>
       </c>
-      <c r="AW48" s="3">
+      <c r="AW48">
         <f>(F48/SUM($C48:$N48)-U48/SUM($R48:$AC48))*SUM('RICBP-it0_damagesbyregionoutput'!$A47:$L47)</f>
         <v>8.2314448264291169</v>
       </c>
-      <c r="AX48" s="3">
+      <c r="AX48">
         <f>(G48/SUM($C48:$N48)-V48/SUM($R48:$AC48))*SUM('RICBP-it0_damagesbyregionoutput'!$A47:$L47)</f>
         <v>13.647592279432004</v>
       </c>
-      <c r="AY48" s="3">
+      <c r="AY48">
         <f>(H48/SUM($C48:$N48)-W48/SUM($R48:$AC48))*SUM('RICBP-it0_damagesbyregionoutput'!$A47:$L47)</f>
         <v>-31.582297294979238</v>
       </c>
-      <c r="AZ48" s="3">
+      <c r="AZ48">
         <f>(I48/SUM($C48:$N48)-X48/SUM($R48:$AC48))*SUM('RICBP-it0_damagesbyregionoutput'!$A47:$L47)</f>
         <v>4.3663760161028513</v>
       </c>
-      <c r="BA48" s="3">
+      <c r="BA48">
         <f>(J48/SUM($C48:$N48)-Y48/SUM($R48:$AC48))*SUM('RICBP-it0_damagesbyregionoutput'!$A47:$L47)</f>
         <v>-2.3877184253871384</v>
       </c>
-      <c r="BB48" s="3">
+      <c r="BB48">
         <f>(K48/SUM($C48:$N48)-Z48/SUM($R48:$AC48))*SUM('RICBP-it0_damagesbyregionoutput'!$A47:$L47)</f>
         <v>-84.380309683252406</v>
       </c>
-      <c r="BC48" s="3">
+      <c r="BC48">
         <f>(L48/SUM($C48:$N48)-AA48/SUM($R48:$AC48))*SUM('RICBP-it0_damagesbyregionoutput'!$A47:$L47)</f>
         <v>3.8896964483958953</v>
       </c>
-      <c r="BD48" s="3">
+      <c r="BD48">
         <f>(M48/SUM($C48:$N48)-AB48/SUM($R48:$AC48))*SUM('RICBP-it0_damagesbyregionoutput'!$A47:$L47)</f>
         <v>3.3802413468950974</v>
       </c>
-      <c r="BE48" s="3">
+      <c r="BE48">
         <f>(N48/SUM($C48:$N48)-AC48/SUM($R48:$AC48))*SUM('RICBP-it0_damagesbyregionoutput'!$A47:$L47)</f>
         <v>-12.39381370342808</v>
       </c>
@@ -22796,51 +22796,51 @@
         <f t="shared" si="5"/>
         <v>-202.14449365653843</v>
       </c>
-      <c r="AT49" s="3">
+      <c r="AT49">
         <f>(C49/SUM($C49:$N49)-R49/SUM($R49:$AC49))*SUM('RICBP-it0_damagesbyregionoutput'!$A48:$L48)</f>
         <v>54.77622458302767</v>
       </c>
-      <c r="AU49" s="3">
+      <c r="AU49">
         <f>(D49/SUM($C49:$N49)-S49/SUM($R49:$AC49))*SUM('RICBP-it0_damagesbyregionoutput'!$A48:$L48)</f>
         <v>39.595052576155972</v>
       </c>
-      <c r="AV49" s="3">
+      <c r="AV49">
         <f>(E49/SUM($C49:$N49)-T49/SUM($R49:$AC49))*SUM('RICBP-it0_damagesbyregionoutput'!$A48:$L48)</f>
         <v>8.0597298480352588</v>
       </c>
-      <c r="AW49" s="3">
+      <c r="AW49">
         <f>(F49/SUM($C49:$N49)-U49/SUM($R49:$AC49))*SUM('RICBP-it0_damagesbyregionoutput'!$A48:$L48)</f>
         <v>8.6701641705862666</v>
       </c>
-      <c r="AX49" s="3">
+      <c r="AX49">
         <f>(G49/SUM($C49:$N49)-V49/SUM($R49:$AC49))*SUM('RICBP-it0_damagesbyregionoutput'!$A48:$L48)</f>
         <v>14.370337213385993</v>
       </c>
-      <c r="AY49" s="3">
+      <c r="AY49">
         <f>(H49/SUM($C49:$N49)-W49/SUM($R49:$AC49))*SUM('RICBP-it0_damagesbyregionoutput'!$A48:$L48)</f>
         <v>-33.420953379702837</v>
       </c>
-      <c r="AZ49" s="3">
+      <c r="AZ49">
         <f>(I49/SUM($C49:$N49)-X49/SUM($R49:$AC49))*SUM('RICBP-it0_damagesbyregionoutput'!$A48:$L48)</f>
         <v>4.7498266322146971</v>
       </c>
-      <c r="BA49" s="3">
+      <c r="BA49">
         <f>(J49/SUM($C49:$N49)-Y49/SUM($R49:$AC49))*SUM('RICBP-it0_damagesbyregionoutput'!$A48:$L48)</f>
         <v>-2.4000399218723216</v>
       </c>
-      <c r="BB49" s="3">
+      <c r="BB49">
         <f>(K49/SUM($C49:$N49)-Z49/SUM($R49:$AC49))*SUM('RICBP-it0_damagesbyregionoutput'!$A48:$L48)</f>
         <v>-88.987936866432648</v>
       </c>
-      <c r="BC49" s="3">
+      <c r="BC49">
         <f>(L49/SUM($C49:$N49)-AA49/SUM($R49:$AC49))*SUM('RICBP-it0_damagesbyregionoutput'!$A48:$L48)</f>
         <v>4.167193683786647</v>
       </c>
-      <c r="BD49" s="3">
+      <c r="BD49">
         <f>(M49/SUM($C49:$N49)-AB49/SUM($R49:$AC49))*SUM('RICBP-it0_damagesbyregionoutput'!$A48:$L48)</f>
         <v>3.5712081515896199</v>
       </c>
-      <c r="BE49" s="3">
+      <c r="BE49">
         <f>(N49/SUM($C49:$N49)-AC49/SUM($R49:$AC49))*SUM('RICBP-it0_damagesbyregionoutput'!$A48:$L48)</f>
         <v>-13.150806690774349</v>
       </c>
@@ -23056,51 +23056,51 @@
         <f t="shared" si="5"/>
         <v>-217.80064030679887</v>
       </c>
-      <c r="AT50" s="3">
+      <c r="AT50">
         <f>(C50/SUM($C50:$N50)-R50/SUM($R50:$AC50))*SUM('RICBP-it0_damagesbyregionoutput'!$A49:$L49)</f>
         <v>57.670338107390258</v>
       </c>
-      <c r="AU50" s="3">
+      <c r="AU50">
         <f>(D50/SUM($C50:$N50)-S50/SUM($R50:$AC50))*SUM('RICBP-it0_damagesbyregionoutput'!$A49:$L49)</f>
         <v>41.685678268983303</v>
       </c>
-      <c r="AV50" s="3">
+      <c r="AV50">
         <f>(E50/SUM($C50:$N50)-T50/SUM($R50:$AC50))*SUM('RICBP-it0_damagesbyregionoutput'!$A49:$L49)</f>
         <v>8.490215646955674</v>
       </c>
-      <c r="AW50" s="3">
+      <c r="AW50">
         <f>(F50/SUM($C50:$N50)-U50/SUM($R50:$AC50))*SUM('RICBP-it0_damagesbyregionoutput'!$A49:$L49)</f>
         <v>9.126974112508595</v>
       </c>
-      <c r="AX50" s="3">
+      <c r="AX50">
         <f>(G50/SUM($C50:$N50)-V50/SUM($R50:$AC50))*SUM('RICBP-it0_damagesbyregionoutput'!$A49:$L49)</f>
         <v>15.122923924234744</v>
       </c>
-      <c r="AY50" s="3">
+      <c r="AY50">
         <f>(H50/SUM($C50:$N50)-W50/SUM($R50:$AC50))*SUM('RICBP-it0_damagesbyregionoutput'!$A49:$L49)</f>
         <v>-35.338493420221809</v>
       </c>
-      <c r="AZ50" s="3">
+      <c r="AZ50">
         <f>(I50/SUM($C50:$N50)-X50/SUM($R50:$AC50))*SUM('RICBP-it0_damagesbyregionoutput'!$A49:$L49)</f>
         <v>5.1533297249301464</v>
       </c>
-      <c r="BA50" s="3">
+      <c r="BA50">
         <f>(J50/SUM($C50:$N50)-Y50/SUM($R50:$AC50))*SUM('RICBP-it0_damagesbyregionoutput'!$A49:$L49)</f>
         <v>-2.4108120364367149</v>
       </c>
-      <c r="BB50" s="3">
+      <c r="BB50">
         <f>(K50/SUM($C50:$N50)-Z50/SUM($R50:$AC50))*SUM('RICBP-it0_damagesbyregionoutput'!$A49:$L49)</f>
         <v>-93.781742993489161</v>
       </c>
-      <c r="BC50" s="3">
+      <c r="BC50">
         <f>(L50/SUM($C50:$N50)-AA50/SUM($R50:$AC50))*SUM('RICBP-it0_damagesbyregionoutput'!$A49:$L49)</f>
         <v>4.4574760377626355</v>
       </c>
-      <c r="BD50" s="3">
+      <c r="BD50">
         <f>(M50/SUM($C50:$N50)-AB50/SUM($R50:$AC50))*SUM('RICBP-it0_damagesbyregionoutput'!$A49:$L49)</f>
         <v>3.7697434148771793</v>
       </c>
-      <c r="BE50" s="3">
+      <c r="BE50">
         <f>(N50/SUM($C50:$N50)-AC50/SUM($R50:$AC50))*SUM('RICBP-it0_damagesbyregionoutput'!$A49:$L49)</f>
         <v>-13.945630787494922</v>
       </c>
@@ -23316,51 +23316,51 @@
         <f t="shared" si="5"/>
         <v>-234.40605301806013</v>
       </c>
-      <c r="AT51" s="3">
+      <c r="AT51">
         <f>(C51/SUM($C51:$N51)-R51/SUM($R51:$AC51))*SUM('RICBP-it0_damagesbyregionoutput'!$A50:$L50)</f>
         <v>60.683554686791695</v>
       </c>
-      <c r="AU51" s="3">
+      <c r="AU51">
         <f>(D51/SUM($C51:$N51)-S51/SUM($R51:$AC51))*SUM('RICBP-it0_damagesbyregionoutput'!$A50:$L50)</f>
         <v>43.861813749936445</v>
       </c>
-      <c r="AV51" s="3">
+      <c r="AV51">
         <f>(E51/SUM($C51:$N51)-T51/SUM($R51:$AC51))*SUM('RICBP-it0_damagesbyregionoutput'!$A50:$L50)</f>
         <v>8.9385114618485186</v>
       </c>
-      <c r="AW51" s="3">
+      <c r="AW51">
         <f>(F51/SUM($C51:$N51)-U51/SUM($R51:$AC51))*SUM('RICBP-it0_damagesbyregionoutput'!$A50:$L50)</f>
         <v>9.6026790598674445</v>
       </c>
-      <c r="AX51" s="3">
+      <c r="AX51">
         <f>(G51/SUM($C51:$N51)-V51/SUM($R51:$AC51))*SUM('RICBP-it0_damagesbyregionoutput'!$A50:$L50)</f>
         <v>15.906678723962406</v>
       </c>
-      <c r="AY51" s="3">
+      <c r="AY51">
         <f>(H51/SUM($C51:$N51)-W51/SUM($R51:$AC51))*SUM('RICBP-it0_damagesbyregionoutput'!$A50:$L50)</f>
         <v>-37.338464857175389</v>
       </c>
-      <c r="AZ51" s="3">
+      <c r="AZ51">
         <f>(I51/SUM($C51:$N51)-X51/SUM($R51:$AC51))*SUM('RICBP-it0_damagesbyregionoutput'!$A50:$L50)</f>
         <v>5.5777935243207981</v>
       </c>
-      <c r="BA51" s="3">
+      <c r="BA51">
         <f>(J51/SUM($C51:$N51)-Y51/SUM($R51:$AC51))*SUM('RICBP-it0_damagesbyregionoutput'!$A50:$L50)</f>
         <v>-2.4199624952778724</v>
       </c>
-      <c r="BB51" s="3">
+      <c r="BB51">
         <f>(K51/SUM($C51:$N51)-Z51/SUM($R51:$AC51))*SUM('RICBP-it0_damagesbyregionoutput'!$A50:$L50)</f>
         <v>-98.769828479997955</v>
       </c>
-      <c r="BC51" s="3">
+      <c r="BC51">
         <f>(L51/SUM($C51:$N51)-AA51/SUM($R51:$AC51))*SUM('RICBP-it0_damagesbyregionoutput'!$A50:$L50)</f>
         <v>4.7611249532182924</v>
       </c>
-      <c r="BD51" s="3">
+      <c r="BD51">
         <f>(M51/SUM($C51:$N51)-AB51/SUM($R51:$AC51))*SUM('RICBP-it0_damagesbyregionoutput'!$A50:$L50)</f>
         <v>3.9761630781180175</v>
       </c>
-      <c r="BE51" s="3">
+      <c r="BE51">
         <f>(N51/SUM($C51:$N51)-AC51/SUM($R51:$AC51))*SUM('RICBP-it0_damagesbyregionoutput'!$A50:$L50)</f>
         <v>-14.780063405612447</v>
       </c>
@@ -23576,51 +23576,51 @@
         <f t="shared" si="5"/>
         <v>-252.00659394284298</v>
       </c>
-      <c r="AT52" s="3">
+      <c r="AT52">
         <f>(C52/SUM($C52:$N52)-R52/SUM($R52:$AC52))*SUM('RICBP-it0_damagesbyregionoutput'!$A51:$L51)</f>
         <v>63.821164271582688</v>
       </c>
-      <c r="AU52" s="3">
+      <c r="AU52">
         <f>(D52/SUM($C52:$N52)-S52/SUM($R52:$AC52))*SUM('RICBP-it0_damagesbyregionoutput'!$A51:$L51)</f>
         <v>46.127218645720127</v>
       </c>
-      <c r="AV52" s="3">
+      <c r="AV52">
         <f>(E52/SUM($C52:$N52)-T52/SUM($R52:$AC52))*SUM('RICBP-it0_damagesbyregionoutput'!$A51:$L51)</f>
         <v>9.4054110670932083</v>
       </c>
-      <c r="AW52" s="3">
+      <c r="AW52">
         <f>(F52/SUM($C52:$N52)-U52/SUM($R52:$AC52))*SUM('RICBP-it0_damagesbyregionoutput'!$A51:$L51)</f>
         <v>10.098119667247303</v>
       </c>
-      <c r="AX52" s="3">
+      <c r="AX52">
         <f>(G52/SUM($C52:$N52)-V52/SUM($R52:$AC52))*SUM('RICBP-it0_damagesbyregionoutput'!$A51:$L51)</f>
         <v>16.722987522867797</v>
       </c>
-      <c r="AY52" s="3">
+      <c r="AY52">
         <f>(H52/SUM($C52:$N52)-W52/SUM($R52:$AC52))*SUM('RICBP-it0_damagesbyregionoutput'!$A51:$L51)</f>
         <v>-39.424579848408619</v>
       </c>
-      <c r="AZ52" s="3">
+      <c r="AZ52">
         <f>(I52/SUM($C52:$N52)-X52/SUM($R52:$AC52))*SUM('RICBP-it0_damagesbyregionoutput'!$A51:$L51)</f>
         <v>6.0241762257724538</v>
       </c>
-      <c r="BA52" s="3">
+      <c r="BA52">
         <f>(J52/SUM($C52:$N52)-Y52/SUM($R52:$AC52))*SUM('RICBP-it0_damagesbyregionoutput'!$A51:$L51)</f>
         <v>-2.427408740676102</v>
       </c>
-      <c r="BB52" s="3">
+      <c r="BB52">
         <f>(K52/SUM($C52:$N52)-Z52/SUM($R52:$AC52))*SUM('RICBP-it0_damagesbyregionoutput'!$A51:$L51)</f>
         <v>-103.96067183823433</v>
       </c>
-      <c r="BC52" s="3">
+      <c r="BC52">
         <f>(L52/SUM($C52:$N52)-AA52/SUM($R52:$AC52))*SUM('RICBP-it0_damagesbyregionoutput'!$A51:$L51)</f>
         <v>5.0787519514500366</v>
       </c>
-      <c r="BD52" s="3">
+      <c r="BD52">
         <f>(M52/SUM($C52:$N52)-AB52/SUM($R52:$AC52))*SUM('RICBP-it0_damagesbyregionoutput'!$A51:$L51)</f>
         <v>4.1907987550772807</v>
       </c>
-      <c r="BE52" s="3">
+      <c r="BE52">
         <f>(N52/SUM($C52:$N52)-AC52/SUM($R52:$AC52))*SUM('RICBP-it0_damagesbyregionoutput'!$A51:$L51)</f>
         <v>-15.655967679491887</v>
       </c>
@@ -23836,51 +23836,51 @@
         <f t="shared" si="5"/>
         <v>-270.65020265674747</v>
       </c>
-      <c r="AT53" s="3">
+      <c r="AT53">
         <f>(C53/SUM($C53:$N53)-R53/SUM($R53:$AC53))*SUM('RICBP-it0_damagesbyregionoutput'!$A52:$L52)</f>
         <v>67.088689984522432</v>
       </c>
-      <c r="AU53" s="3">
+      <c r="AU53">
         <f>(D53/SUM($C53:$N53)-S53/SUM($R53:$AC53))*SUM('RICBP-it0_damagesbyregionoutput'!$A52:$L52)</f>
         <v>48.485819805440798</v>
       </c>
-      <c r="AV53" s="3">
+      <c r="AV53">
         <f>(E53/SUM($C53:$N53)-T53/SUM($R53:$AC53))*SUM('RICBP-it0_damagesbyregionoutput'!$A52:$L52)</f>
         <v>9.8917433777100321</v>
       </c>
-      <c r="AW53" s="3">
+      <c r="AW53">
         <f>(F53/SUM($C53:$N53)-U53/SUM($R53:$AC53))*SUM('RICBP-it0_damagesbyregionoutput'!$A52:$L52)</f>
         <v>10.614173625387316</v>
       </c>
-      <c r="AX53" s="3">
+      <c r="AX53">
         <f>(G53/SUM($C53:$N53)-V53/SUM($R53:$AC53))*SUM('RICBP-it0_damagesbyregionoutput'!$A52:$L52)</f>
         <v>17.573297151179791</v>
       </c>
-      <c r="AY53" s="3">
+      <c r="AY53">
         <f>(H53/SUM($C53:$N53)-W53/SUM($R53:$AC53))*SUM('RICBP-it0_damagesbyregionoutput'!$A52:$L52)</f>
         <v>-41.60071842510078</v>
       </c>
-      <c r="AZ53" s="3">
+      <c r="AZ53">
         <f>(I53/SUM($C53:$N53)-X53/SUM($R53:$AC53))*SUM('RICBP-it0_damagesbyregionoutput'!$A52:$L52)</f>
         <v>6.4934869466763425</v>
       </c>
-      <c r="BA53" s="3">
+      <c r="BA53">
         <f>(J53/SUM($C53:$N53)-Y53/SUM($R53:$AC53))*SUM('RICBP-it0_damagesbyregionoutput'!$A52:$L52)</f>
         <v>-2.4330579941536343</v>
       </c>
-      <c r="BB53" s="3">
+      <c r="BB53">
         <f>(K53/SUM($C53:$N53)-Z53/SUM($R53:$AC53))*SUM('RICBP-it0_damagesbyregionoutput'!$A52:$L52)</f>
         <v>-109.36313621188417</v>
       </c>
-      <c r="BC53" s="3">
+      <c r="BC53">
         <f>(L53/SUM($C53:$N53)-AA53/SUM($R53:$AC53))*SUM('RICBP-it0_damagesbyregionoutput'!$A52:$L52)</f>
         <v>5.4109991381781279</v>
       </c>
-      <c r="BD53" s="3">
+      <c r="BD53">
         <f>(M53/SUM($C53:$N53)-AB53/SUM($R53:$AC53))*SUM('RICBP-it0_damagesbyregionoutput'!$A52:$L52)</f>
         <v>4.4139979197537702</v>
       </c>
-      <c r="BE53" s="3">
+      <c r="BE53">
         <f>(N53/SUM($C53:$N53)-AC53/SUM($R53:$AC53))*SUM('RICBP-it0_damagesbyregionoutput'!$A52:$L52)</f>
         <v>-16.575295317710026</v>
       </c>
@@ -24096,51 +24096,51 @@
         <f t="shared" si="5"/>
         <v>-290.38699228551553</v>
       </c>
-      <c r="AT54" s="3">
+      <c r="AT54">
         <f>(C54/SUM($C54:$N54)-R54/SUM($R54:$AC54))*SUM('RICBP-it0_damagesbyregionoutput'!$A53:$L53)</f>
         <v>70.491893736429802</v>
       </c>
-      <c r="AU54" s="3">
+      <c r="AU54">
         <f>(D54/SUM($C54:$N54)-S54/SUM($R54:$AC54))*SUM('RICBP-it0_damagesbyregionoutput'!$A53:$L53)</f>
         <v>50.941715144398728</v>
       </c>
-      <c r="AV54" s="3">
+      <c r="AV54">
         <f>(E54/SUM($C54:$N54)-T54/SUM($R54:$AC54))*SUM('RICBP-it0_damagesbyregionoutput'!$A53:$L53)</f>
         <v>10.398373298928046</v>
       </c>
-      <c r="AW54" s="3">
+      <c r="AW54">
         <f>(F54/SUM($C54:$N54)-U54/SUM($R54:$AC54))*SUM('RICBP-it0_damagesbyregionoutput'!$A53:$L53)</f>
         <v>11.151756574081825</v>
       </c>
-      <c r="AX54" s="3">
+      <c r="AX54">
         <f>(G54/SUM($C54:$N54)-V54/SUM($R54:$AC54))*SUM('RICBP-it0_damagesbyregionoutput'!$A53:$L53)</f>
         <v>18.459116882172395</v>
       </c>
-      <c r="AY54" s="3">
+      <c r="AY54">
         <f>(H54/SUM($C54:$N54)-W54/SUM($R54:$AC54))*SUM('RICBP-it0_damagesbyregionoutput'!$A53:$L53)</f>
         <v>-43.870932254521712</v>
       </c>
-      <c r="AZ54" s="3">
+      <c r="AZ54">
         <f>(I54/SUM($C54:$N54)-X54/SUM($R54:$AC54))*SUM('RICBP-it0_damagesbyregionoutput'!$A53:$L53)</f>
         <v>6.9867868337614238</v>
       </c>
-      <c r="BA54" s="3">
+      <c r="BA54">
         <f>(J54/SUM($C54:$N54)-Y54/SUM($R54:$AC54))*SUM('RICBP-it0_damagesbyregionoutput'!$A53:$L53)</f>
         <v>-2.4368072917337846</v>
       </c>
-      <c r="BB54" s="3">
+      <c r="BB54">
         <f>(K54/SUM($C54:$N54)-Z54/SUM($R54:$AC54))*SUM('RICBP-it0_damagesbyregionoutput'!$A53:$L53)</f>
         <v>-114.9864772740772</v>
       </c>
-      <c r="BC54" s="3">
+      <c r="BC54">
         <f>(L54/SUM($C54:$N54)-AA54/SUM($R54:$AC54))*SUM('RICBP-it0_damagesbyregionoutput'!$A53:$L53)</f>
         <v>5.7585398149740294</v>
       </c>
-      <c r="BD54" s="3">
+      <c r="BD54">
         <f>(M54/SUM($C54:$N54)-AB54/SUM($R54:$AC54))*SUM('RICBP-it0_damagesbyregionoutput'!$A53:$L53)</f>
         <v>4.6461241469811014</v>
       </c>
-      <c r="BE54" s="3">
+      <c r="BE54">
         <f>(N54/SUM($C54:$N54)-AC54/SUM($R54:$AC54))*SUM('RICBP-it0_damagesbyregionoutput'!$A53:$L53)</f>
         <v>-17.540089611394709</v>
       </c>
@@ -24356,51 +24356,51 @@
         <f t="shared" si="5"/>
         <v>-311.26934837743261</v>
       </c>
-      <c r="AT55" s="3">
+      <c r="AT55">
         <f>(C55/SUM($C55:$N55)-R55/SUM($R55:$AC55))*SUM('RICBP-it0_damagesbyregionoutput'!$A54:$L54)</f>
         <v>74.036782605489819</v>
       </c>
-      <c r="AU55" s="3">
+      <c r="AU55">
         <f>(D55/SUM($C55:$N55)-S55/SUM($R55:$AC55))*SUM('RICBP-it0_damagesbyregionoutput'!$A54:$L54)</f>
         <v>53.499178027795345</v>
       </c>
-      <c r="AV55" s="3">
+      <c r="AV55">
         <f>(E55/SUM($C55:$N55)-T55/SUM($R55:$AC55))*SUM('RICBP-it0_damagesbyregionoutput'!$A54:$L54)</f>
         <v>10.926202689953204</v>
       </c>
-      <c r="AW55" s="3">
+      <c r="AW55">
         <f>(F55/SUM($C55:$N55)-U55/SUM($R55:$AC55))*SUM('RICBP-it0_damagesbyregionoutput'!$A54:$L54)</f>
         <v>11.71182313464182</v>
       </c>
-      <c r="AX55" s="3">
+      <c r="AX55">
         <f>(G55/SUM($C55:$N55)-V55/SUM($R55:$AC55))*SUM('RICBP-it0_damagesbyregionoutput'!$A54:$L54)</f>
         <v>19.382020150183184</v>
       </c>
-      <c r="AY55" s="3">
+      <c r="AY55">
         <f>(H55/SUM($C55:$N55)-W55/SUM($R55:$AC55))*SUM('RICBP-it0_damagesbyregionoutput'!$A54:$L54)</f>
         <v>-46.239448982413428</v>
       </c>
-      <c r="AZ55" s="3">
+      <c r="AZ55">
         <f>(I55/SUM($C55:$N55)-X55/SUM($R55:$AC55))*SUM('RICBP-it0_damagesbyregionoutput'!$A54:$L54)</f>
         <v>7.5051903203002892</v>
       </c>
-      <c r="BA55" s="3">
+      <c r="BA55">
         <f>(J55/SUM($C55:$N55)-Y55/SUM($R55:$AC55))*SUM('RICBP-it0_damagesbyregionoutput'!$A54:$L54)</f>
         <v>-2.4385434889347066</v>
       </c>
-      <c r="BB55" s="3">
+      <c r="BB55">
         <f>(K55/SUM($C55:$N55)-Z55/SUM($R55:$AC55))*SUM('RICBP-it0_damagesbyregionoutput'!$A54:$L54)</f>
         <v>-120.84035244666786</v>
       </c>
-      <c r="BC55" s="3">
+      <c r="BC55">
         <f>(L55/SUM($C55:$N55)-AA55/SUM($R55:$AC55))*SUM('RICBP-it0_damagesbyregionoutput'!$A54:$L54)</f>
         <v>6.1220791932664422</v>
       </c>
-      <c r="BD55" s="3">
+      <c r="BD55">
         <f>(M55/SUM($C55:$N55)-AB55/SUM($R55:$AC55))*SUM('RICBP-it0_damagesbyregionoutput'!$A54:$L54)</f>
         <v>4.8875574053420108</v>
       </c>
-      <c r="BE55" s="3">
+      <c r="BE55">
         <f>(N55/SUM($C55:$N55)-AC55/SUM($R55:$AC55))*SUM('RICBP-it0_damagesbyregionoutput'!$A54:$L54)</f>
         <v>-18.552488608956203</v>
       </c>
@@ -24616,51 +24616,51 @@
         <f t="shared" si="5"/>
         <v>-333.35203075860755</v>
       </c>
-      <c r="AT56" s="3">
+      <c r="AT56">
         <f>(C56/SUM($C56:$N56)-R56/SUM($R56:$AC56))*SUM('RICBP-it0_damagesbyregionoutput'!$A55:$L55)</f>
         <v>77.729615954514628</v>
       </c>
-      <c r="AU56" s="3">
+      <c r="AU56">
         <f>(D56/SUM($C56:$N56)-S56/SUM($R56:$AC56))*SUM('RICBP-it0_damagesbyregionoutput'!$A55:$L55)</f>
         <v>56.162662178460167</v>
       </c>
-      <c r="AV56" s="3">
+      <c r="AV56">
         <f>(E56/SUM($C56:$N56)-T56/SUM($R56:$AC56))*SUM('RICBP-it0_damagesbyregionoutput'!$A55:$L55)</f>
         <v>11.476171438255585</v>
       </c>
-      <c r="AW56" s="3">
+      <c r="AW56">
         <f>(F56/SUM($C56:$N56)-U56/SUM($R56:$AC56))*SUM('RICBP-it0_damagesbyregionoutput'!$A55:$L55)</f>
         <v>12.295368058029288</v>
       </c>
-      <c r="AX56" s="3">
+      <c r="AX56">
         <f>(G56/SUM($C56:$N56)-V56/SUM($R56:$AC56))*SUM('RICBP-it0_damagesbyregionoutput'!$A55:$L55)</f>
         <v>20.343646457295481</v>
       </c>
-      <c r="AY56" s="3">
+      <c r="AY56">
         <f>(H56/SUM($C56:$N56)-W56/SUM($R56:$AC56))*SUM('RICBP-it0_damagesbyregionoutput'!$A55:$L55)</f>
         <v>-48.710677130161564</v>
       </c>
-      <c r="AZ56" s="3">
+      <c r="AZ56">
         <f>(I56/SUM($C56:$N56)-X56/SUM($R56:$AC56))*SUM('RICBP-it0_damagesbyregionoutput'!$A55:$L55)</f>
         <v>8.0498665318818237</v>
       </c>
-      <c r="BA56" s="3">
+      <c r="BA56">
         <f>(J56/SUM($C56:$N56)-Y56/SUM($R56:$AC56))*SUM('RICBP-it0_damagesbyregionoutput'!$A55:$L55)</f>
         <v>-2.4381432340097007</v>
       </c>
-      <c r="BB56" s="3">
+      <c r="BB56">
         <f>(K56/SUM($C56:$N56)-Z56/SUM($R56:$AC56))*SUM('RICBP-it0_damagesbyregionoutput'!$A55:$L55)</f>
         <v>-126.93483139820903</v>
       </c>
-      <c r="BC56" s="3">
+      <c r="BC56">
         <f>(L56/SUM($C56:$N56)-AA56/SUM($R56:$AC56))*SUM('RICBP-it0_damagesbyregionoutput'!$A55:$L55)</f>
         <v>6.5023552080411768</v>
       </c>
-      <c r="BD56" s="3">
+      <c r="BD56">
         <f>(M56/SUM($C56:$N56)-AB56/SUM($R56:$AC56))*SUM('RICBP-it0_damagesbyregionoutput'!$A55:$L55)</f>
         <v>5.1386944015512084</v>
       </c>
-      <c r="BE56" s="3">
+      <c r="BE56">
         <f>(N56/SUM($C56:$N56)-AC56/SUM($R56:$AC56))*SUM('RICBP-it0_damagesbyregionoutput'!$A55:$L55)</f>
         <v>-19.614728465649161</v>
       </c>
@@ -24876,51 +24876,51 @@
         <f t="shared" si="5"/>
         <v>-356.69227860866869</v>
       </c>
-      <c r="AT57" s="3">
+      <c r="AT57">
         <f>(C57/SUM($C57:$N57)-R57/SUM($R57:$AC57))*SUM('RICBP-it0_damagesbyregionoutput'!$A56:$L56)</f>
         <v>81.576913262748135</v>
       </c>
-      <c r="AU57" s="3">
+      <c r="AU57">
         <f>(D57/SUM($C57:$N57)-S57/SUM($R57:$AC57))*SUM('RICBP-it0_damagesbyregionoutput'!$A56:$L56)</f>
         <v>58.93680709358884</v>
       </c>
-      <c r="AV57" s="3">
+      <c r="AV57">
         <f>(E57/SUM($C57:$N57)-T57/SUM($R57:$AC57))*SUM('RICBP-it0_damagesbyregionoutput'!$A56:$L56)</f>
         <v>12.049258641004576</v>
       </c>
-      <c r="AW57" s="3">
+      <c r="AW57">
         <f>(F57/SUM($C57:$N57)-U57/SUM($R57:$AC57))*SUM('RICBP-it0_damagesbyregionoutput'!$A56:$L56)</f>
         <v>12.903427485135591</v>
       </c>
-      <c r="AX57" s="3">
+      <c r="AX57">
         <f>(G57/SUM($C57:$N57)-V57/SUM($R57:$AC57))*SUM('RICBP-it0_damagesbyregionoutput'!$A56:$L56)</f>
         <v>21.345703463039193</v>
       </c>
-      <c r="AY57" s="3">
+      <c r="AY57">
         <f>(H57/SUM($C57:$N57)-W57/SUM($R57:$AC57))*SUM('RICBP-it0_damagesbyregionoutput'!$A56:$L56)</f>
         <v>-51.289211524621365</v>
       </c>
-      <c r="AZ57" s="3">
+      <c r="AZ57">
         <f>(I57/SUM($C57:$N57)-X57/SUM($R57:$AC57))*SUM('RICBP-it0_damagesbyregionoutput'!$A56:$L56)</f>
         <v>8.6220408392309213</v>
       </c>
-      <c r="BA57" s="3">
+      <c r="BA57">
         <f>(J57/SUM($C57:$N57)-Y57/SUM($R57:$AC57))*SUM('RICBP-it0_damagesbyregionoutput'!$A56:$L56)</f>
         <v>-2.4354729086025633</v>
       </c>
-      <c r="BB57" s="3">
+      <c r="BB57">
         <f>(K57/SUM($C57:$N57)-Z57/SUM($R57:$AC57))*SUM('RICBP-it0_damagesbyregionoutput'!$A56:$L56)</f>
         <v>-133.28040777991606</v>
       </c>
-      <c r="BC57" s="3">
+      <c r="BC57">
         <f>(L57/SUM($C57:$N57)-AA57/SUM($R57:$AC57))*SUM('RICBP-it0_damagesbyregionoutput'!$A56:$L56)</f>
         <v>6.9001394284695694</v>
       </c>
-      <c r="BD57" s="3">
+      <c r="BD57">
         <f>(M57/SUM($C57:$N57)-AB57/SUM($R57:$AC57))*SUM('RICBP-it0_damagesbyregionoutput'!$A56:$L56)</f>
         <v>5.399948975244242</v>
       </c>
-      <c r="BE57" s="3">
+      <c r="BE57">
         <f>(N57/SUM($C57:$N57)-AC57/SUM($R57:$AC57))*SUM('RICBP-it0_damagesbyregionoutput'!$A56:$L56)</f>
         <v>-20.729146975321111</v>
       </c>
@@ -25136,51 +25136,51 @@
         <f t="shared" si="5"/>
         <v>-381.34991899426205</v>
       </c>
-      <c r="AT58" s="3">
+      <c r="AT58">
         <f>(C58/SUM($C58:$N58)-R58/SUM($R58:$AC58))*SUM('RICBP-it0_damagesbyregionoutput'!$A57:$L57)</f>
         <v>85.585462651698037</v>
       </c>
-      <c r="AU58" s="3">
+      <c r="AU58">
         <f>(D58/SUM($C58:$N58)-S58/SUM($R58:$AC58))*SUM('RICBP-it0_damagesbyregionoutput'!$A57:$L57)</f>
         <v>61.826443956954975</v>
       </c>
-      <c r="AV58" s="3">
+      <c r="AV58">
         <f>(E58/SUM($C58:$N58)-T58/SUM($R58:$AC58))*SUM('RICBP-it0_damagesbyregionoutput'!$A57:$L57)</f>
         <v>12.646483890688396</v>
       </c>
-      <c r="AW58" s="3">
+      <c r="AW58">
         <f>(F58/SUM($C58:$N58)-U58/SUM($R58:$AC58))*SUM('RICBP-it0_damagesbyregionoutput'!$A57:$L57)</f>
         <v>13.53708031612671</v>
       </c>
-      <c r="AX58" s="3">
+      <c r="AX58">
         <f>(G58/SUM($C58:$N58)-V58/SUM($R58:$AC58))*SUM('RICBP-it0_damagesbyregionoutput'!$A57:$L57)</f>
         <v>22.38996925220664</v>
       </c>
-      <c r="AY58" s="3">
+      <c r="AY58">
         <f>(H58/SUM($C58:$N58)-W58/SUM($R58:$AC58))*SUM('RICBP-it0_damagesbyregionoutput'!$A57:$L57)</f>
         <v>-53.979839241447841</v>
       </c>
-      <c r="AZ58" s="3">
+      <c r="AZ58">
         <f>(I58/SUM($C58:$N58)-X58/SUM($R58:$AC58))*SUM('RICBP-it0_damagesbyregionoutput'!$A57:$L57)</f>
         <v>9.2229965565797674</v>
       </c>
-      <c r="BA58" s="3">
+      <c r="BA58">
         <f>(J58/SUM($C58:$N58)-Y58/SUM($R58:$AC58))*SUM('RICBP-it0_damagesbyregionoutput'!$A57:$L57)</f>
         <v>-2.4303885354651045</v>
       </c>
-      <c r="BB58" s="3">
+      <c r="BB58">
         <f>(K58/SUM($C58:$N58)-Z58/SUM($R58:$AC58))*SUM('RICBP-it0_damagesbyregionoutput'!$A57:$L57)</f>
         <v>-139.88801216235299</v>
       </c>
-      <c r="BC58" s="3">
+      <c r="BC58">
         <f>(L58/SUM($C58:$N58)-AA58/SUM($R58:$AC58))*SUM('RICBP-it0_damagesbyregionoutput'!$A57:$L57)</f>
         <v>7.3162380629410739</v>
       </c>
-      <c r="BD58" s="3">
+      <c r="BD58">
         <f>(M58/SUM($C58:$N58)-AB58/SUM($R58:$AC58))*SUM('RICBP-it0_damagesbyregionoutput'!$A57:$L57)</f>
         <v>5.6717525430167868</v>
       </c>
-      <c r="BE58" s="3">
+      <c r="BE58">
         <f>(N58/SUM($C58:$N58)-AC58/SUM($R58:$AC58))*SUM('RICBP-it0_damagesbyregionoutput'!$A57:$L57)</f>
         <v>-21.898187290946591</v>
       </c>
@@ -25396,51 +25396,51 @@
         <f t="shared" si="5"/>
         <v>-407.38747909771917</v>
       </c>
-      <c r="AT59" s="3">
+      <c r="AT59">
         <f>(C59/SUM($C59:$N59)-R59/SUM($R59:$AC59))*SUM('RICBP-it0_damagesbyregionoutput'!$A58:$L58)</f>
         <v>89.762330087701315</v>
       </c>
-      <c r="AU59" s="3">
+      <c r="AU59">
         <f>(D59/SUM($C59:$N59)-S59/SUM($R59:$AC59))*SUM('RICBP-it0_damagesbyregionoutput'!$A58:$L58)</f>
         <v>64.836602034887946</v>
       </c>
-      <c r="AV59" s="3">
+      <c r="AV59">
         <f>(E59/SUM($C59:$N59)-T59/SUM($R59:$AC59))*SUM('RICBP-it0_damagesbyregionoutput'!$A58:$L58)</f>
         <v>13.268908662416621</v>
       </c>
-      <c r="AW59" s="3">
+      <c r="AW59">
         <f>(F59/SUM($C59:$N59)-U59/SUM($R59:$AC59))*SUM('RICBP-it0_damagesbyregionoutput'!$A58:$L58)</f>
         <v>14.197449686280057</v>
       </c>
-      <c r="AX59" s="3">
+      <c r="AX59">
         <f>(G59/SUM($C59:$N59)-V59/SUM($R59:$AC59))*SUM('RICBP-it0_damagesbyregionoutput'!$A58:$L58)</f>
         <v>23.478294776699798</v>
       </c>
-      <c r="AY59" s="3">
+      <c r="AY59">
         <f>(H59/SUM($C59:$N59)-W59/SUM($R59:$AC59))*SUM('RICBP-it0_damagesbyregionoutput'!$A58:$L58)</f>
         <v>-56.787546045862399</v>
       </c>
-      <c r="AZ59" s="3">
+      <c r="AZ59">
         <f>(I59/SUM($C59:$N59)-X59/SUM($R59:$AC59))*SUM('RICBP-it0_damagesbyregionoutput'!$A58:$L58)</f>
         <v>9.8540767842860006</v>
       </c>
-      <c r="BA59" s="3">
+      <c r="BA59">
         <f>(J59/SUM($C59:$N59)-Y59/SUM($R59:$AC59))*SUM('RICBP-it0_damagesbyregionoutput'!$A58:$L58)</f>
         <v>-2.422735653219807</v>
       </c>
-      <c r="BB59" s="3">
+      <c r="BB59">
         <f>(K59/SUM($C59:$N59)-Z59/SUM($R59:$AC59))*SUM('RICBP-it0_damagesbyregionoutput'!$A58:$L58)</f>
         <v>-146.76902613999215</v>
       </c>
-      <c r="BC59" s="3">
+      <c r="BC59">
         <f>(L59/SUM($C59:$N59)-AA59/SUM($R59:$AC59))*SUM('RICBP-it0_damagesbyregionoutput'!$A58:$L58)</f>
         <v>7.7514930562945814</v>
       </c>
-      <c r="BD59" s="3">
+      <c r="BD59">
         <f>(M59/SUM($C59:$N59)-AB59/SUM($R59:$AC59))*SUM('RICBP-it0_damagesbyregionoutput'!$A58:$L58)</f>
         <v>5.9545545905561426</v>
       </c>
-      <c r="BE59" s="3">
+      <c r="BE59">
         <f>(N59/SUM($C59:$N59)-AC59/SUM($R59:$AC59))*SUM('RICBP-it0_damagesbyregionoutput'!$A58:$L58)</f>
         <v>-23.124401840048129</v>
       </c>
@@ -25656,51 +25656,51 @@
         <f t="shared" si="7"/>
         <v>-434.87030237859312</v>
       </c>
-      <c r="AT60" s="3">
+      <c r="AT60">
         <f>(C60/SUM($C60:$N60)-R60/SUM($R60:$AC60))*SUM('RICBP-it0_damagesbyregionoutput'!$A59:$L59)</f>
         <v>94.114869247337637</v>
       </c>
-      <c r="AU60" s="3">
+      <c r="AU60">
         <f>(D60/SUM($C60:$N60)-S60/SUM($R60:$AC60))*SUM('RICBP-it0_damagesbyregionoutput'!$A59:$L59)</f>
         <v>67.972515546374439</v>
       </c>
-      <c r="AV60" s="3">
+      <c r="AV60">
         <f>(E60/SUM($C60:$N60)-T60/SUM($R60:$AC60))*SUM('RICBP-it0_damagesbyregionoutput'!$A59:$L59)</f>
         <v>13.917637800898751</v>
       </c>
-      <c r="AW60" s="3">
+      <c r="AW60">
         <f>(F60/SUM($C60:$N60)-U60/SUM($R60:$AC60))*SUM('RICBP-it0_damagesbyregionoutput'!$A59:$L59)</f>
         <v>14.885704546267464</v>
       </c>
-      <c r="AX60" s="3">
+      <c r="AX60">
         <f>(G60/SUM($C60:$N60)-V60/SUM($R60:$AC60))*SUM('RICBP-it0_damagesbyregionoutput'!$A59:$L59)</f>
         <v>24.61260646818954</v>
       </c>
-      <c r="AY60" s="3">
+      <c r="AY60">
         <f>(H60/SUM($C60:$N60)-W60/SUM($R60:$AC60))*SUM('RICBP-it0_damagesbyregionoutput'!$A59:$L59)</f>
         <v>-59.717523317880328</v>
       </c>
-      <c r="AZ60" s="3">
+      <c r="AZ60">
         <f>(I60/SUM($C60:$N60)-X60/SUM($R60:$AC60))*SUM('RICBP-it0_damagesbyregionoutput'!$A59:$L59)</f>
         <v>10.516686394702603</v>
       </c>
-      <c r="BA60" s="3">
+      <c r="BA60">
         <f>(J60/SUM($C60:$N60)-Y60/SUM($R60:$AC60))*SUM('RICBP-it0_damagesbyregionoutput'!$A59:$L59)</f>
         <v>-2.4123491583764873</v>
       </c>
-      <c r="BB60" s="3">
+      <c r="BB60">
         <f>(K60/SUM($C60:$N60)-Z60/SUM($R60:$AC60))*SUM('RICBP-it0_damagesbyregionoutput'!$A59:$L59)</f>
         <v>-153.93529757587288</v>
       </c>
-      <c r="BC60" s="3">
+      <c r="BC60">
         <f>(L60/SUM($C60:$N60)-AA60/SUM($R60:$AC60))*SUM('RICBP-it0_damagesbyregionoutput'!$A59:$L59)</f>
         <v>8.2067832774124572</v>
       </c>
-      <c r="BD60" s="3">
+      <c r="BD60">
         <f>(M60/SUM($C60:$N60)-AB60/SUM($R60:$AC60))*SUM('RICBP-it0_damagesbyregionoutput'!$A59:$L59)</f>
         <v>6.2488232117716525</v>
       </c>
-      <c r="BE60" s="3">
+      <c r="BE60">
         <f>(N60/SUM($C60:$N60)-AC60/SUM($R60:$AC60))*SUM('RICBP-it0_damagesbyregionoutput'!$A59:$L59)</f>
         <v>-24.410456440824934</v>
       </c>
@@ -25916,51 +25916,51 @@
         <f t="shared" si="7"/>
         <v>-463.86666890657818</v>
       </c>
-      <c r="AT61" s="3">
+      <c r="AT61">
         <f>(C61/SUM($C61:$N61)-R61/SUM($R61:$AC61))*SUM('RICBP-it0_damagesbyregionoutput'!$A60:$L60)</f>
         <v>98.650732035239415</v>
       </c>
-      <c r="AU61" s="3">
+      <c r="AU61">
         <f>(D61/SUM($C61:$N61)-S61/SUM($R61:$AC61))*SUM('RICBP-it0_damagesbyregionoutput'!$A60:$L60)</f>
         <v>71.239630999810288</v>
       </c>
-      <c r="AV61" s="3">
+      <c r="AV61">
         <f>(E61/SUM($C61:$N61)-T61/SUM($R61:$AC61))*SUM('RICBP-it0_damagesbyregionoutput'!$A60:$L60)</f>
         <v>14.593821105593975</v>
       </c>
-      <c r="AW61" s="3">
+      <c r="AW61">
         <f>(F61/SUM($C61:$N61)-U61/SUM($R61:$AC61))*SUM('RICBP-it0_damagesbyregionoutput'!$A60:$L60)</f>
         <v>15.603061345372877</v>
       </c>
-      <c r="AX61" s="3">
+      <c r="AX61">
         <f>(G61/SUM($C61:$N61)-V61/SUM($R61:$AC61))*SUM('RICBP-it0_damagesbyregionoutput'!$A60:$L60)</f>
         <v>25.79490901923646</v>
       </c>
-      <c r="AY61" s="3">
+      <c r="AY61">
         <f>(H61/SUM($C61:$N61)-W61/SUM($R61:$AC61))*SUM('RICBP-it0_damagesbyregionoutput'!$A60:$L60)</f>
         <v>-62.77517545202133</v>
       </c>
-      <c r="AZ61" s="3">
+      <c r="AZ61">
         <f>(I61/SUM($C61:$N61)-X61/SUM($R61:$AC61))*SUM('RICBP-it0_damagesbyregionoutput'!$A60:$L60)</f>
         <v>11.212294160691492</v>
       </c>
-      <c r="BA61" s="3">
+      <c r="BA61">
         <f>(J61/SUM($C61:$N61)-Y61/SUM($R61:$AC61))*SUM('RICBP-it0_damagesbyregionoutput'!$A60:$L60)</f>
         <v>-2.3990531149500356</v>
       </c>
-      <c r="BB61" s="3">
+      <c r="BB61">
         <f>(K61/SUM($C61:$N61)-Z61/SUM($R61:$AC61))*SUM('RICBP-it0_damagesbyregionoutput'!$A60:$L60)</f>
         <v>-161.39915696395474</v>
       </c>
-      <c r="BC61" s="3">
+      <c r="BC61">
         <f>(L61/SUM($C61:$N61)-AA61/SUM($R61:$AC61))*SUM('RICBP-it0_damagesbyregionoutput'!$A60:$L60)</f>
         <v>8.6830257957361976</v>
       </c>
-      <c r="BD61" s="3">
+      <c r="BD61">
         <f>(M61/SUM($C61:$N61)-AB61/SUM($R61:$AC61))*SUM('RICBP-it0_damagesbyregionoutput'!$A60:$L60)</f>
         <v>6.555045693941417</v>
       </c>
-      <c r="BE61" s="3">
+      <c r="BE61">
         <f>(N61/SUM($C61:$N61)-AC61/SUM($R61:$AC61))*SUM('RICBP-it0_damagesbyregionoutput'!$A60:$L60)</f>
         <v>-25.759134624696156</v>
       </c>
@@ -26176,51 +26176,51 @@
         <f t="shared" si="7"/>
         <v>-494.4479201057348</v>
       </c>
-      <c r="AT62" s="3">
+      <c r="AT62">
         <f>(C62/SUM($C62:$N62)-R62/SUM($R62:$AC62))*SUM('RICBP-it0_damagesbyregionoutput'!$A61:$L61)</f>
         <v>103.37787974724468</v>
       </c>
-      <c r="AU62" s="3">
+      <c r="AU62">
         <f>(D62/SUM($C62:$N62)-S62/SUM($R62:$AC62))*SUM('RICBP-it0_damagesbyregionoutput'!$A61:$L61)</f>
         <v>74.643614991136786</v>
       </c>
-      <c r="AV62" s="3">
+      <c r="AV62">
         <f>(E62/SUM($C62:$N62)-T62/SUM($R62:$AC62))*SUM('RICBP-it0_damagesbyregionoutput'!$A61:$L61)</f>
         <v>15.298655013026533</v>
       </c>
-      <c r="AW62" s="3">
+      <c r="AW62">
         <f>(F62/SUM($C62:$N62)-U62/SUM($R62:$AC62))*SUM('RICBP-it0_damagesbyregionoutput'!$A61:$L61)</f>
         <v>16.35078581666118</v>
       </c>
-      <c r="AX62" s="3">
+      <c r="AX62">
         <f>(G62/SUM($C62:$N62)-V62/SUM($R62:$AC62))*SUM('RICBP-it0_damagesbyregionoutput'!$A61:$L61)</f>
         <v>27.027288331381104</v>
       </c>
-      <c r="AY62" s="3">
+      <c r="AY62">
         <f>(H62/SUM($C62:$N62)-W62/SUM($R62:$AC62))*SUM('RICBP-it0_damagesbyregionoutput'!$A61:$L61)</f>
         <v>-65.966127724405396</v>
       </c>
-      <c r="AZ62" s="3">
+      <c r="AZ62">
         <f>(I62/SUM($C62:$N62)-X62/SUM($R62:$AC62))*SUM('RICBP-it0_damagesbyregionoutput'!$A61:$L61)</f>
         <v>11.942435026609157</v>
       </c>
-      <c r="BA62" s="3">
+      <c r="BA62">
         <f>(J62/SUM($C62:$N62)-Y62/SUM($R62:$AC62))*SUM('RICBP-it0_damagesbyregionoutput'!$A61:$L61)</f>
         <v>-2.3826605321002083</v>
       </c>
-      <c r="BB62" s="3">
+      <c r="BB62">
         <f>(K62/SUM($C62:$N62)-Z62/SUM($R62:$AC62))*SUM('RICBP-it0_damagesbyregionoutput'!$A61:$L61)</f>
         <v>-169.17343489226641</v>
       </c>
-      <c r="BC62" s="3">
+      <c r="BC62">
         <f>(L62/SUM($C62:$N62)-AA62/SUM($R62:$AC62))*SUM('RICBP-it0_damagesbyregionoutput'!$A61:$L61)</f>
         <v>9.1811772456685077</v>
       </c>
-      <c r="BD62" s="3">
+      <c r="BD62">
         <f>(M62/SUM($C62:$N62)-AB62/SUM($R62:$AC62))*SUM('RICBP-it0_damagesbyregionoutput'!$A61:$L61)</f>
         <v>6.8737291480348892</v>
       </c>
-      <c r="BE62" s="3">
+      <c r="BE62">
         <f>(N62/SUM($C62:$N62)-AC62/SUM($R62:$AC62))*SUM('RICBP-it0_damagesbyregionoutput'!$A61:$L61)</f>
         <v>-27.173342170990924</v>
       </c>
@@ -28940,12 +28940,24 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A394C3DE-E302-6E41-92AA-7D0129EED7DD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D45004-EEFC-8F42-98FB-57E2E780FE96}">
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:N64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -39765,8 +39777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34409AE1-4CF1-EC4D-AAA0-E4DDDD54BA87}">
   <dimension ref="A1:BR62"/>
   <sheetViews>
-    <sheetView topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AT3" sqref="AT3:BE3"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AT13" sqref="AT13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>